<commit_message>
Full mapping of ObjectUse function by class
Plus loads of other things now figured out in the disassembly
</commit_message>
<xml_diff>
--- a/File Research/Game Object Research File.xlsx
+++ b/File Research/Game Object Research File.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F01444D-66C0-4B1B-B82F-E28973A44531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DC9BF2-1939-4623-933E-3DB03D98C529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="14985" windowHeight="10980" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="191">
   <si>
     <t>Static Object</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>For NPCs does this mean they are in combat?</t>
+  </si>
+  <si>
+    <t>Does npc_hunger mean the npc is aware of the player</t>
   </si>
 </sst>
 </file>
@@ -1694,10 +1697,10 @@
   <dimension ref="A1:HI48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="BZ23" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="AH10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="CD34" sqref="CD34"/>
+      <selection pane="bottomRight" activeCell="BC25" sqref="BC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6242,7 +6245,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>41</v>
       </c>
@@ -6286,8 +6289,11 @@
       <c r="FS17" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="18" spans="1:175" x14ac:dyDescent="0.45">
+      <c r="GV17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -6329,7 +6335,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>71</v>
       </c>
@@ -6368,7 +6374,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A20" s="7"/>
       <c r="N20" s="34" t="s">
         <v>161</v>
@@ -6399,7 +6405,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A21" s="7"/>
       <c r="E21" t="s">
         <v>120</v>
@@ -6451,7 +6457,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A22" s="7"/>
       <c r="E22">
         <v>5972</v>
@@ -6506,7 +6512,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="23" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A23" s="7"/>
       <c r="G23">
         <v>1</v>
@@ -6548,7 +6554,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A24" s="7"/>
       <c r="G24">
         <v>2</v>
@@ -6573,7 +6579,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A25" s="7"/>
       <c r="G25">
         <v>3</v>
@@ -6598,7 +6604,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A26" s="7"/>
       <c r="G26">
         <v>4</v>
@@ -6620,7 +6626,7 @@
       <c r="CJ26" s="105"/>
       <c r="CK26" s="105"/>
     </row>
-    <row r="27" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A27" s="7"/>
       <c r="G27">
         <v>5</v>
@@ -6642,7 +6648,7 @@
       <c r="CJ27" s="105"/>
       <c r="CK27" s="105"/>
     </row>
-    <row r="28" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A28" s="7"/>
       <c r="G28">
         <v>6</v>
@@ -6664,7 +6670,7 @@
       <c r="CJ28" s="105"/>
       <c r="CK28" s="105"/>
     </row>
-    <row r="29" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A29" s="7"/>
       <c r="G29">
         <v>7</v>
@@ -6686,7 +6692,7 @@
       <c r="CJ29" s="105"/>
       <c r="CK29" s="105"/>
     </row>
-    <row r="30" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A30" s="7"/>
       <c r="G30">
         <v>8</v>
@@ -6703,7 +6709,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A31" s="7"/>
       <c r="G31">
         <v>9</v>
@@ -6717,7 +6723,7 @@
         <v>597B</v>
       </c>
     </row>
-    <row r="32" spans="1:175" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A32" s="7"/>
       <c r="G32">
         <v>10</v>

</xml_diff>

<commit_message>
Object research midway into position, terrain, some dat files exported to xls
</commit_message>
<xml_diff>
--- a/File Research/Game Object Research File.xlsx
+++ b/File Research/Game Object Research File.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF20524-FD2D-47E0-B31E-AC339AB37337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EFD6F6-F900-4FD8-91FB-D820CA2CCA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8325" yWindow="563" windowWidth="12195" windowHeight="12667" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Object" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="263">
   <si>
     <t>Static Object</t>
   </si>
@@ -552,14 +552,6 @@
   </si>
   <si>
     <t>Does npc_hunger mean the npc is aware of the player and wants to eat them (ie become hostile)</t>
-  </si>
-  <si>
-    <t>Race number of the owner of the object or a general parameter of the object
-For Npcs tileY</t>
-  </si>
-  <si>
-    <t>Generally the health of an object or a general use parameter for a trap
-For NPCS tileX</t>
   </si>
   <si>
     <t>Bits 4 to 7 are probably a single value</t>
@@ -876,6 +868,25 @@
   </si>
   <si>
     <t>Looked at when object hits the ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gtarg is the npc being targeted by this npc. Usually it is one for the avatar
+When petrified the value is the timer for how long petrification lasts
+</t>
+  </si>
+  <si>
+    <t>Generally the health of an object or a general use parameter for a trap
+For NPCS tileX  (or xhome)</t>
+  </si>
+  <si>
+    <t>Race number of the owner of the object or a general parameter of the object
+For Npcs tileY (or yhome)</t>
+  </si>
+  <si>
+    <t>Value affects Hp returned by study monster</t>
+  </si>
+  <si>
+    <t>Bit relevant to magic effects</t>
   </si>
 </sst>
 </file>
@@ -1575,6 +1586,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1597,9 +1611,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2222,10 +2233,10 @@
   <dimension ref="A1:HI48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9:H11"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2262,1075 +2273,1075 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="60"/>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="60"/>
-      <c r="AF1" s="60"/>
-      <c r="AG1" s="60"/>
-      <c r="AH1" s="60"/>
-      <c r="AI1" s="60"/>
-      <c r="AJ1" s="60"/>
-      <c r="AK1" s="60"/>
-      <c r="AL1" s="60"/>
-      <c r="AM1" s="60"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="60"/>
-      <c r="AP1" s="60"/>
-      <c r="AQ1" s="60"/>
-      <c r="AR1" s="60"/>
-      <c r="AS1" s="60"/>
-      <c r="AT1" s="60"/>
-      <c r="AU1" s="60"/>
-      <c r="AV1" s="60"/>
-      <c r="AW1" s="60"/>
-      <c r="AX1" s="60"/>
-      <c r="AY1" s="60"/>
-      <c r="AZ1" s="60"/>
-      <c r="BA1" s="60"/>
-      <c r="BB1" s="60"/>
-      <c r="BC1" s="60"/>
-      <c r="BD1" s="60"/>
-      <c r="BE1" s="60"/>
-      <c r="BF1" s="60"/>
-      <c r="BG1" s="60"/>
-      <c r="BH1" s="60"/>
-      <c r="BI1" s="60"/>
-      <c r="BJ1" s="60"/>
-      <c r="BK1" s="60"/>
-      <c r="BL1" s="60"/>
-      <c r="BM1" s="61"/>
-      <c r="BN1" s="59" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="61"/>
+      <c r="AF1" s="61"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="61"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="61"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="61"/>
+      <c r="AN1" s="61"/>
+      <c r="AO1" s="61"/>
+      <c r="AP1" s="61"/>
+      <c r="AQ1" s="61"/>
+      <c r="AR1" s="61"/>
+      <c r="AS1" s="61"/>
+      <c r="AT1" s="61"/>
+      <c r="AU1" s="61"/>
+      <c r="AV1" s="61"/>
+      <c r="AW1" s="61"/>
+      <c r="AX1" s="61"/>
+      <c r="AY1" s="61"/>
+      <c r="AZ1" s="61"/>
+      <c r="BA1" s="61"/>
+      <c r="BB1" s="61"/>
+      <c r="BC1" s="61"/>
+      <c r="BD1" s="61"/>
+      <c r="BE1" s="61"/>
+      <c r="BF1" s="61"/>
+      <c r="BG1" s="61"/>
+      <c r="BH1" s="61"/>
+      <c r="BI1" s="61"/>
+      <c r="BJ1" s="61"/>
+      <c r="BK1" s="61"/>
+      <c r="BL1" s="61"/>
+      <c r="BM1" s="62"/>
+      <c r="BN1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="BO1" s="60"/>
-      <c r="BP1" s="60"/>
-      <c r="BQ1" s="60"/>
-      <c r="BR1" s="60"/>
-      <c r="BS1" s="60"/>
-      <c r="BT1" s="60"/>
-      <c r="BU1" s="60"/>
-      <c r="BV1" s="60"/>
-      <c r="BW1" s="60"/>
-      <c r="BX1" s="60"/>
-      <c r="BY1" s="60"/>
-      <c r="BZ1" s="60"/>
-      <c r="CA1" s="60"/>
-      <c r="CB1" s="60"/>
-      <c r="CC1" s="60"/>
-      <c r="CD1" s="60"/>
-      <c r="CE1" s="60"/>
-      <c r="CF1" s="60"/>
-      <c r="CG1" s="60"/>
-      <c r="CH1" s="60"/>
-      <c r="CI1" s="60"/>
-      <c r="CJ1" s="60"/>
-      <c r="CK1" s="60"/>
-      <c r="CL1" s="60"/>
-      <c r="CM1" s="60"/>
-      <c r="CN1" s="60"/>
-      <c r="CO1" s="60"/>
-      <c r="CP1" s="60"/>
-      <c r="CQ1" s="60"/>
-      <c r="CR1" s="60"/>
-      <c r="CS1" s="60"/>
-      <c r="CT1" s="60"/>
-      <c r="CU1" s="60"/>
-      <c r="CV1" s="60"/>
-      <c r="CW1" s="60"/>
-      <c r="CX1" s="60"/>
-      <c r="CY1" s="60"/>
-      <c r="CZ1" s="60"/>
-      <c r="DA1" s="60"/>
-      <c r="DB1" s="60"/>
-      <c r="DC1" s="60"/>
-      <c r="DD1" s="60"/>
-      <c r="DE1" s="60"/>
-      <c r="DF1" s="60"/>
-      <c r="DG1" s="60"/>
-      <c r="DH1" s="60"/>
-      <c r="DI1" s="60"/>
-      <c r="DJ1" s="60"/>
-      <c r="DK1" s="60"/>
-      <c r="DL1" s="60"/>
-      <c r="DM1" s="60"/>
-      <c r="DN1" s="60"/>
-      <c r="DO1" s="60"/>
-      <c r="DP1" s="60"/>
-      <c r="DQ1" s="60"/>
-      <c r="DR1" s="60"/>
-      <c r="DS1" s="60"/>
-      <c r="DT1" s="60"/>
-      <c r="DU1" s="60"/>
-      <c r="DV1" s="60"/>
-      <c r="DW1" s="60"/>
-      <c r="DX1" s="60"/>
-      <c r="DY1" s="60"/>
-      <c r="DZ1" s="60"/>
-      <c r="EA1" s="60"/>
-      <c r="EB1" s="60"/>
-      <c r="EC1" s="60"/>
-      <c r="ED1" s="60"/>
-      <c r="EE1" s="60"/>
-      <c r="EF1" s="60"/>
-      <c r="EG1" s="60"/>
-      <c r="EH1" s="60"/>
-      <c r="EI1" s="60"/>
-      <c r="EJ1" s="60"/>
-      <c r="EK1" s="60"/>
-      <c r="EL1" s="60"/>
-      <c r="EM1" s="60"/>
-      <c r="EN1" s="60"/>
-      <c r="EO1" s="60"/>
-      <c r="EP1" s="60"/>
-      <c r="EQ1" s="60"/>
-      <c r="ER1" s="60"/>
-      <c r="ES1" s="60"/>
-      <c r="ET1" s="60"/>
-      <c r="EU1" s="60"/>
-      <c r="EV1" s="60"/>
-      <c r="EW1" s="60"/>
-      <c r="EX1" s="60"/>
-      <c r="EY1" s="60"/>
-      <c r="EZ1" s="60"/>
-      <c r="FA1" s="60"/>
-      <c r="FB1" s="60"/>
-      <c r="FC1" s="60"/>
-      <c r="FD1" s="60"/>
-      <c r="FE1" s="60"/>
-      <c r="FF1" s="60"/>
-      <c r="FG1" s="60"/>
-      <c r="FH1" s="60"/>
-      <c r="FI1" s="60"/>
-      <c r="FJ1" s="60"/>
-      <c r="FK1" s="60"/>
-      <c r="FL1" s="60"/>
-      <c r="FM1" s="60"/>
-      <c r="FN1" s="60"/>
-      <c r="FO1" s="60"/>
-      <c r="FP1" s="60"/>
-      <c r="FQ1" s="60"/>
-      <c r="FR1" s="60"/>
-      <c r="FS1" s="60"/>
-      <c r="FT1" s="60"/>
-      <c r="FU1" s="60"/>
-      <c r="FV1" s="60"/>
-      <c r="FW1" s="60"/>
-      <c r="FX1" s="60"/>
-      <c r="FY1" s="60"/>
-      <c r="FZ1" s="60"/>
-      <c r="GA1" s="60"/>
-      <c r="GB1" s="60"/>
-      <c r="GC1" s="60"/>
-      <c r="GD1" s="60"/>
-      <c r="GE1" s="60"/>
-      <c r="GF1" s="60"/>
-      <c r="GG1" s="60"/>
-      <c r="GH1" s="60"/>
-      <c r="GI1" s="60"/>
-      <c r="GJ1" s="60"/>
-      <c r="GK1" s="60"/>
-      <c r="GL1" s="60"/>
-      <c r="GM1" s="60"/>
-      <c r="GN1" s="60"/>
-      <c r="GO1" s="60"/>
-      <c r="GP1" s="60"/>
-      <c r="GQ1" s="60"/>
-      <c r="GR1" s="60"/>
-      <c r="GS1" s="60"/>
-      <c r="GT1" s="60"/>
-      <c r="GU1" s="60"/>
-      <c r="GV1" s="60"/>
-      <c r="GW1" s="60"/>
-      <c r="GX1" s="60"/>
-      <c r="GY1" s="60"/>
-      <c r="GZ1" s="60"/>
-      <c r="HA1" s="60"/>
-      <c r="HB1" s="60"/>
-      <c r="HC1" s="60"/>
-      <c r="HD1" s="60"/>
-      <c r="HE1" s="60"/>
-      <c r="HF1" s="60"/>
-      <c r="HG1" s="60"/>
-      <c r="HH1" s="60"/>
-      <c r="HI1" s="60"/>
+      <c r="BO1" s="61"/>
+      <c r="BP1" s="61"/>
+      <c r="BQ1" s="61"/>
+      <c r="BR1" s="61"/>
+      <c r="BS1" s="61"/>
+      <c r="BT1" s="61"/>
+      <c r="BU1" s="61"/>
+      <c r="BV1" s="61"/>
+      <c r="BW1" s="61"/>
+      <c r="BX1" s="61"/>
+      <c r="BY1" s="61"/>
+      <c r="BZ1" s="61"/>
+      <c r="CA1" s="61"/>
+      <c r="CB1" s="61"/>
+      <c r="CC1" s="61"/>
+      <c r="CD1" s="61"/>
+      <c r="CE1" s="61"/>
+      <c r="CF1" s="61"/>
+      <c r="CG1" s="61"/>
+      <c r="CH1" s="61"/>
+      <c r="CI1" s="61"/>
+      <c r="CJ1" s="61"/>
+      <c r="CK1" s="61"/>
+      <c r="CL1" s="61"/>
+      <c r="CM1" s="61"/>
+      <c r="CN1" s="61"/>
+      <c r="CO1" s="61"/>
+      <c r="CP1" s="61"/>
+      <c r="CQ1" s="61"/>
+      <c r="CR1" s="61"/>
+      <c r="CS1" s="61"/>
+      <c r="CT1" s="61"/>
+      <c r="CU1" s="61"/>
+      <c r="CV1" s="61"/>
+      <c r="CW1" s="61"/>
+      <c r="CX1" s="61"/>
+      <c r="CY1" s="61"/>
+      <c r="CZ1" s="61"/>
+      <c r="DA1" s="61"/>
+      <c r="DB1" s="61"/>
+      <c r="DC1" s="61"/>
+      <c r="DD1" s="61"/>
+      <c r="DE1" s="61"/>
+      <c r="DF1" s="61"/>
+      <c r="DG1" s="61"/>
+      <c r="DH1" s="61"/>
+      <c r="DI1" s="61"/>
+      <c r="DJ1" s="61"/>
+      <c r="DK1" s="61"/>
+      <c r="DL1" s="61"/>
+      <c r="DM1" s="61"/>
+      <c r="DN1" s="61"/>
+      <c r="DO1" s="61"/>
+      <c r="DP1" s="61"/>
+      <c r="DQ1" s="61"/>
+      <c r="DR1" s="61"/>
+      <c r="DS1" s="61"/>
+      <c r="DT1" s="61"/>
+      <c r="DU1" s="61"/>
+      <c r="DV1" s="61"/>
+      <c r="DW1" s="61"/>
+      <c r="DX1" s="61"/>
+      <c r="DY1" s="61"/>
+      <c r="DZ1" s="61"/>
+      <c r="EA1" s="61"/>
+      <c r="EB1" s="61"/>
+      <c r="EC1" s="61"/>
+      <c r="ED1" s="61"/>
+      <c r="EE1" s="61"/>
+      <c r="EF1" s="61"/>
+      <c r="EG1" s="61"/>
+      <c r="EH1" s="61"/>
+      <c r="EI1" s="61"/>
+      <c r="EJ1" s="61"/>
+      <c r="EK1" s="61"/>
+      <c r="EL1" s="61"/>
+      <c r="EM1" s="61"/>
+      <c r="EN1" s="61"/>
+      <c r="EO1" s="61"/>
+      <c r="EP1" s="61"/>
+      <c r="EQ1" s="61"/>
+      <c r="ER1" s="61"/>
+      <c r="ES1" s="61"/>
+      <c r="ET1" s="61"/>
+      <c r="EU1" s="61"/>
+      <c r="EV1" s="61"/>
+      <c r="EW1" s="61"/>
+      <c r="EX1" s="61"/>
+      <c r="EY1" s="61"/>
+      <c r="EZ1" s="61"/>
+      <c r="FA1" s="61"/>
+      <c r="FB1" s="61"/>
+      <c r="FC1" s="61"/>
+      <c r="FD1" s="61"/>
+      <c r="FE1" s="61"/>
+      <c r="FF1" s="61"/>
+      <c r="FG1" s="61"/>
+      <c r="FH1" s="61"/>
+      <c r="FI1" s="61"/>
+      <c r="FJ1" s="61"/>
+      <c r="FK1" s="61"/>
+      <c r="FL1" s="61"/>
+      <c r="FM1" s="61"/>
+      <c r="FN1" s="61"/>
+      <c r="FO1" s="61"/>
+      <c r="FP1" s="61"/>
+      <c r="FQ1" s="61"/>
+      <c r="FR1" s="61"/>
+      <c r="FS1" s="61"/>
+      <c r="FT1" s="61"/>
+      <c r="FU1" s="61"/>
+      <c r="FV1" s="61"/>
+      <c r="FW1" s="61"/>
+      <c r="FX1" s="61"/>
+      <c r="FY1" s="61"/>
+      <c r="FZ1" s="61"/>
+      <c r="GA1" s="61"/>
+      <c r="GB1" s="61"/>
+      <c r="GC1" s="61"/>
+      <c r="GD1" s="61"/>
+      <c r="GE1" s="61"/>
+      <c r="GF1" s="61"/>
+      <c r="GG1" s="61"/>
+      <c r="GH1" s="61"/>
+      <c r="GI1" s="61"/>
+      <c r="GJ1" s="61"/>
+      <c r="GK1" s="61"/>
+      <c r="GL1" s="61"/>
+      <c r="GM1" s="61"/>
+      <c r="GN1" s="61"/>
+      <c r="GO1" s="61"/>
+      <c r="GP1" s="61"/>
+      <c r="GQ1" s="61"/>
+      <c r="GR1" s="61"/>
+      <c r="GS1" s="61"/>
+      <c r="GT1" s="61"/>
+      <c r="GU1" s="61"/>
+      <c r="GV1" s="61"/>
+      <c r="GW1" s="61"/>
+      <c r="GX1" s="61"/>
+      <c r="GY1" s="61"/>
+      <c r="GZ1" s="61"/>
+      <c r="HA1" s="61"/>
+      <c r="HB1" s="61"/>
+      <c r="HC1" s="61"/>
+      <c r="HD1" s="61"/>
+      <c r="HE1" s="61"/>
+      <c r="HF1" s="61"/>
+      <c r="HG1" s="61"/>
+      <c r="HH1" s="61"/>
+      <c r="HI1" s="61"/>
     </row>
     <row r="2" spans="1:217" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="60">
         <v>0</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="59">
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="60">
         <v>1</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="59">
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="60">
         <v>2</v>
       </c>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="59">
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="60">
         <v>3</v>
       </c>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="61"/>
-      <c r="AH2" s="59">
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
+      <c r="AF2" s="61"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="60">
         <v>4</v>
       </c>
-      <c r="AI2" s="60"/>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="61"/>
-      <c r="AP2" s="59">
+      <c r="AI2" s="61"/>
+      <c r="AJ2" s="61"/>
+      <c r="AK2" s="61"/>
+      <c r="AL2" s="61"/>
+      <c r="AM2" s="61"/>
+      <c r="AN2" s="61"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="60">
         <v>5</v>
       </c>
-      <c r="AQ2" s="60"/>
-      <c r="AR2" s="60"/>
-      <c r="AS2" s="60"/>
-      <c r="AT2" s="60"/>
-      <c r="AU2" s="60"/>
-      <c r="AV2" s="60"/>
-      <c r="AW2" s="61"/>
-      <c r="AX2" s="59">
+      <c r="AQ2" s="61"/>
+      <c r="AR2" s="61"/>
+      <c r="AS2" s="61"/>
+      <c r="AT2" s="61"/>
+      <c r="AU2" s="61"/>
+      <c r="AV2" s="61"/>
+      <c r="AW2" s="62"/>
+      <c r="AX2" s="60">
         <v>6</v>
       </c>
-      <c r="AY2" s="60"/>
-      <c r="AZ2" s="60"/>
-      <c r="BA2" s="60"/>
-      <c r="BB2" s="60"/>
-      <c r="BC2" s="60"/>
-      <c r="BD2" s="60"/>
-      <c r="BE2" s="61"/>
-      <c r="BF2" s="59">
+      <c r="AY2" s="61"/>
+      <c r="AZ2" s="61"/>
+      <c r="BA2" s="61"/>
+      <c r="BB2" s="61"/>
+      <c r="BC2" s="61"/>
+      <c r="BD2" s="61"/>
+      <c r="BE2" s="62"/>
+      <c r="BF2" s="60">
         <v>7</v>
       </c>
-      <c r="BG2" s="60"/>
-      <c r="BH2" s="60"/>
-      <c r="BI2" s="60"/>
-      <c r="BJ2" s="60"/>
-      <c r="BK2" s="60"/>
-      <c r="BL2" s="60"/>
-      <c r="BM2" s="61"/>
-      <c r="BN2" s="59">
+      <c r="BG2" s="61"/>
+      <c r="BH2" s="61"/>
+      <c r="BI2" s="61"/>
+      <c r="BJ2" s="61"/>
+      <c r="BK2" s="61"/>
+      <c r="BL2" s="61"/>
+      <c r="BM2" s="62"/>
+      <c r="BN2" s="60">
         <v>8</v>
       </c>
-      <c r="BO2" s="60"/>
-      <c r="BP2" s="60"/>
-      <c r="BQ2" s="60"/>
-      <c r="BR2" s="60"/>
-      <c r="BS2" s="60"/>
-      <c r="BT2" s="60"/>
-      <c r="BU2" s="61"/>
-      <c r="BV2" s="59">
+      <c r="BO2" s="61"/>
+      <c r="BP2" s="61"/>
+      <c r="BQ2" s="61"/>
+      <c r="BR2" s="61"/>
+      <c r="BS2" s="61"/>
+      <c r="BT2" s="61"/>
+      <c r="BU2" s="62"/>
+      <c r="BV2" s="60">
         <v>9</v>
       </c>
-      <c r="BW2" s="60"/>
-      <c r="BX2" s="60"/>
-      <c r="BY2" s="60"/>
-      <c r="BZ2" s="60"/>
-      <c r="CA2" s="60"/>
-      <c r="CB2" s="60"/>
-      <c r="CC2" s="61"/>
-      <c r="CD2" s="59">
+      <c r="BW2" s="61"/>
+      <c r="BX2" s="61"/>
+      <c r="BY2" s="61"/>
+      <c r="BZ2" s="61"/>
+      <c r="CA2" s="61"/>
+      <c r="CB2" s="61"/>
+      <c r="CC2" s="62"/>
+      <c r="CD2" s="60">
         <v>10</v>
       </c>
-      <c r="CE2" s="60"/>
-      <c r="CF2" s="60"/>
-      <c r="CG2" s="60"/>
-      <c r="CH2" s="60"/>
-      <c r="CI2" s="60"/>
-      <c r="CJ2" s="60"/>
-      <c r="CK2" s="61"/>
-      <c r="CL2" s="59">
+      <c r="CE2" s="61"/>
+      <c r="CF2" s="61"/>
+      <c r="CG2" s="61"/>
+      <c r="CH2" s="61"/>
+      <c r="CI2" s="61"/>
+      <c r="CJ2" s="61"/>
+      <c r="CK2" s="62"/>
+      <c r="CL2" s="60">
         <v>11</v>
       </c>
-      <c r="CM2" s="60"/>
-      <c r="CN2" s="60"/>
-      <c r="CO2" s="60"/>
-      <c r="CP2" s="60"/>
-      <c r="CQ2" s="60"/>
-      <c r="CR2" s="60"/>
-      <c r="CS2" s="61"/>
-      <c r="CT2" s="59">
+      <c r="CM2" s="61"/>
+      <c r="CN2" s="61"/>
+      <c r="CO2" s="61"/>
+      <c r="CP2" s="61"/>
+      <c r="CQ2" s="61"/>
+      <c r="CR2" s="61"/>
+      <c r="CS2" s="62"/>
+      <c r="CT2" s="60">
         <v>12</v>
       </c>
-      <c r="CU2" s="60"/>
-      <c r="CV2" s="60"/>
-      <c r="CW2" s="60"/>
-      <c r="CX2" s="60"/>
-      <c r="CY2" s="60"/>
-      <c r="CZ2" s="60"/>
-      <c r="DA2" s="61"/>
-      <c r="DB2" s="59">
+      <c r="CU2" s="61"/>
+      <c r="CV2" s="61"/>
+      <c r="CW2" s="61"/>
+      <c r="CX2" s="61"/>
+      <c r="CY2" s="61"/>
+      <c r="CZ2" s="61"/>
+      <c r="DA2" s="62"/>
+      <c r="DB2" s="60">
         <v>13</v>
       </c>
-      <c r="DC2" s="60"/>
-      <c r="DD2" s="60"/>
-      <c r="DE2" s="60"/>
-      <c r="DF2" s="60"/>
-      <c r="DG2" s="60"/>
-      <c r="DH2" s="60"/>
-      <c r="DI2" s="61"/>
-      <c r="DJ2" s="59">
+      <c r="DC2" s="61"/>
+      <c r="DD2" s="61"/>
+      <c r="DE2" s="61"/>
+      <c r="DF2" s="61"/>
+      <c r="DG2" s="61"/>
+      <c r="DH2" s="61"/>
+      <c r="DI2" s="62"/>
+      <c r="DJ2" s="60">
         <v>14</v>
       </c>
-      <c r="DK2" s="60"/>
-      <c r="DL2" s="60"/>
-      <c r="DM2" s="60"/>
-      <c r="DN2" s="60"/>
-      <c r="DO2" s="60"/>
-      <c r="DP2" s="60"/>
-      <c r="DQ2" s="61"/>
-      <c r="DR2" s="59">
+      <c r="DK2" s="61"/>
+      <c r="DL2" s="61"/>
+      <c r="DM2" s="61"/>
+      <c r="DN2" s="61"/>
+      <c r="DO2" s="61"/>
+      <c r="DP2" s="61"/>
+      <c r="DQ2" s="62"/>
+      <c r="DR2" s="60">
         <v>15</v>
       </c>
-      <c r="DS2" s="60"/>
-      <c r="DT2" s="60"/>
-      <c r="DU2" s="60"/>
-      <c r="DV2" s="60"/>
-      <c r="DW2" s="60"/>
-      <c r="DX2" s="60"/>
-      <c r="DY2" s="61"/>
-      <c r="DZ2" s="59">
+      <c r="DS2" s="61"/>
+      <c r="DT2" s="61"/>
+      <c r="DU2" s="61"/>
+      <c r="DV2" s="61"/>
+      <c r="DW2" s="61"/>
+      <c r="DX2" s="61"/>
+      <c r="DY2" s="62"/>
+      <c r="DZ2" s="60">
         <v>16</v>
       </c>
-      <c r="EA2" s="60"/>
-      <c r="EB2" s="60"/>
-      <c r="EC2" s="60"/>
-      <c r="ED2" s="60"/>
-      <c r="EE2" s="60"/>
-      <c r="EF2" s="60"/>
-      <c r="EG2" s="61"/>
-      <c r="EH2" s="59">
+      <c r="EA2" s="61"/>
+      <c r="EB2" s="61"/>
+      <c r="EC2" s="61"/>
+      <c r="ED2" s="61"/>
+      <c r="EE2" s="61"/>
+      <c r="EF2" s="61"/>
+      <c r="EG2" s="62"/>
+      <c r="EH2" s="60">
         <v>17</v>
       </c>
-      <c r="EI2" s="60"/>
-      <c r="EJ2" s="60"/>
-      <c r="EK2" s="60"/>
-      <c r="EL2" s="60"/>
-      <c r="EM2" s="60"/>
-      <c r="EN2" s="60"/>
-      <c r="EO2" s="61"/>
-      <c r="EP2" s="59">
+      <c r="EI2" s="61"/>
+      <c r="EJ2" s="61"/>
+      <c r="EK2" s="61"/>
+      <c r="EL2" s="61"/>
+      <c r="EM2" s="61"/>
+      <c r="EN2" s="61"/>
+      <c r="EO2" s="62"/>
+      <c r="EP2" s="60">
         <v>18</v>
       </c>
-      <c r="EQ2" s="60"/>
-      <c r="ER2" s="60"/>
-      <c r="ES2" s="60"/>
-      <c r="ET2" s="60"/>
-      <c r="EU2" s="60"/>
-      <c r="EV2" s="60"/>
-      <c r="EW2" s="61"/>
-      <c r="EX2" s="59">
+      <c r="EQ2" s="61"/>
+      <c r="ER2" s="61"/>
+      <c r="ES2" s="61"/>
+      <c r="ET2" s="61"/>
+      <c r="EU2" s="61"/>
+      <c r="EV2" s="61"/>
+      <c r="EW2" s="62"/>
+      <c r="EX2" s="60">
         <v>19</v>
       </c>
-      <c r="EY2" s="60"/>
-      <c r="EZ2" s="60"/>
-      <c r="FA2" s="60"/>
-      <c r="FB2" s="60"/>
-      <c r="FC2" s="60"/>
-      <c r="FD2" s="60"/>
-      <c r="FE2" s="61"/>
-      <c r="FF2" s="59">
+      <c r="EY2" s="61"/>
+      <c r="EZ2" s="61"/>
+      <c r="FA2" s="61"/>
+      <c r="FB2" s="61"/>
+      <c r="FC2" s="61"/>
+      <c r="FD2" s="61"/>
+      <c r="FE2" s="62"/>
+      <c r="FF2" s="60">
         <v>20</v>
       </c>
-      <c r="FG2" s="60"/>
-      <c r="FH2" s="60"/>
-      <c r="FI2" s="60"/>
-      <c r="FJ2" s="60"/>
-      <c r="FK2" s="60"/>
-      <c r="FL2" s="60"/>
-      <c r="FM2" s="61"/>
-      <c r="FN2" s="59">
+      <c r="FG2" s="61"/>
+      <c r="FH2" s="61"/>
+      <c r="FI2" s="61"/>
+      <c r="FJ2" s="61"/>
+      <c r="FK2" s="61"/>
+      <c r="FL2" s="61"/>
+      <c r="FM2" s="62"/>
+      <c r="FN2" s="60">
         <v>21</v>
       </c>
-      <c r="FO2" s="60"/>
-      <c r="FP2" s="60"/>
-      <c r="FQ2" s="60"/>
-      <c r="FR2" s="60"/>
-      <c r="FS2" s="60"/>
-      <c r="FT2" s="60"/>
-      <c r="FU2" s="61"/>
-      <c r="FV2" s="59">
+      <c r="FO2" s="61"/>
+      <c r="FP2" s="61"/>
+      <c r="FQ2" s="61"/>
+      <c r="FR2" s="61"/>
+      <c r="FS2" s="61"/>
+      <c r="FT2" s="61"/>
+      <c r="FU2" s="62"/>
+      <c r="FV2" s="60">
         <v>22</v>
       </c>
-      <c r="FW2" s="60"/>
-      <c r="FX2" s="60"/>
-      <c r="FY2" s="60"/>
-      <c r="FZ2" s="60"/>
-      <c r="GA2" s="60"/>
-      <c r="GB2" s="60"/>
-      <c r="GC2" s="61"/>
-      <c r="GD2" s="59">
+      <c r="FW2" s="61"/>
+      <c r="FX2" s="61"/>
+      <c r="FY2" s="61"/>
+      <c r="FZ2" s="61"/>
+      <c r="GA2" s="61"/>
+      <c r="GB2" s="61"/>
+      <c r="GC2" s="62"/>
+      <c r="GD2" s="60">
         <v>23</v>
       </c>
-      <c r="GE2" s="60"/>
-      <c r="GF2" s="60"/>
-      <c r="GG2" s="60"/>
-      <c r="GH2" s="60"/>
-      <c r="GI2" s="60"/>
-      <c r="GJ2" s="60"/>
-      <c r="GK2" s="61"/>
-      <c r="GL2" s="59">
+      <c r="GE2" s="61"/>
+      <c r="GF2" s="61"/>
+      <c r="GG2" s="61"/>
+      <c r="GH2" s="61"/>
+      <c r="GI2" s="61"/>
+      <c r="GJ2" s="61"/>
+      <c r="GK2" s="62"/>
+      <c r="GL2" s="60">
         <v>24</v>
       </c>
-      <c r="GM2" s="60"/>
-      <c r="GN2" s="60"/>
-      <c r="GO2" s="60"/>
-      <c r="GP2" s="60"/>
-      <c r="GQ2" s="60"/>
-      <c r="GR2" s="60"/>
-      <c r="GS2" s="61"/>
-      <c r="GT2" s="59">
+      <c r="GM2" s="61"/>
+      <c r="GN2" s="61"/>
+      <c r="GO2" s="61"/>
+      <c r="GP2" s="61"/>
+      <c r="GQ2" s="61"/>
+      <c r="GR2" s="61"/>
+      <c r="GS2" s="62"/>
+      <c r="GT2" s="60">
         <v>25</v>
       </c>
-      <c r="GU2" s="60"/>
-      <c r="GV2" s="60"/>
-      <c r="GW2" s="60"/>
-      <c r="GX2" s="60"/>
-      <c r="GY2" s="60"/>
-      <c r="GZ2" s="60"/>
-      <c r="HA2" s="61"/>
-      <c r="HB2" s="59">
+      <c r="GU2" s="61"/>
+      <c r="GV2" s="61"/>
+      <c r="GW2" s="61"/>
+      <c r="GX2" s="61"/>
+      <c r="GY2" s="61"/>
+      <c r="GZ2" s="61"/>
+      <c r="HA2" s="62"/>
+      <c r="HB2" s="60">
         <v>26</v>
       </c>
-      <c r="HC2" s="60"/>
-      <c r="HD2" s="60"/>
-      <c r="HE2" s="60"/>
-      <c r="HF2" s="60"/>
-      <c r="HG2" s="60"/>
-      <c r="HH2" s="60"/>
-      <c r="HI2" s="61"/>
+      <c r="HC2" s="61"/>
+      <c r="HD2" s="61"/>
+      <c r="HE2" s="61"/>
+      <c r="HF2" s="61"/>
+      <c r="HG2" s="61"/>
+      <c r="HH2" s="61"/>
+      <c r="HI2" s="62"/>
     </row>
     <row r="3" spans="1:217" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="59" t="str">
+      <c r="B3" s="60" t="str">
         <f>DEC2HEX(B2)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="59" t="str">
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="60" t="str">
         <f t="shared" ref="J3" si="0">DEC2HEX(J2)</f>
         <v>1</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="59" t="str">
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="60" t="str">
         <f t="shared" ref="R3" si="1">DEC2HEX(R2)</f>
         <v>2</v>
       </c>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="59" t="str">
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="60" t="str">
         <f t="shared" ref="Z3" si="2">DEC2HEX(Z2)</f>
         <v>3</v>
       </c>
-      <c r="AA3" s="60"/>
-      <c r="AB3" s="60"/>
-      <c r="AC3" s="60"/>
-      <c r="AD3" s="60"/>
-      <c r="AE3" s="60"/>
-      <c r="AF3" s="60"/>
-      <c r="AG3" s="61"/>
-      <c r="AH3" s="59" t="str">
+      <c r="AA3" s="61"/>
+      <c r="AB3" s="61"/>
+      <c r="AC3" s="61"/>
+      <c r="AD3" s="61"/>
+      <c r="AE3" s="61"/>
+      <c r="AF3" s="61"/>
+      <c r="AG3" s="62"/>
+      <c r="AH3" s="60" t="str">
         <f t="shared" ref="AH3" si="3">DEC2HEX(AH2)</f>
         <v>4</v>
       </c>
-      <c r="AI3" s="60"/>
-      <c r="AJ3" s="60"/>
-      <c r="AK3" s="60"/>
-      <c r="AL3" s="60"/>
-      <c r="AM3" s="60"/>
-      <c r="AN3" s="60"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="59" t="str">
+      <c r="AI3" s="61"/>
+      <c r="AJ3" s="61"/>
+      <c r="AK3" s="61"/>
+      <c r="AL3" s="61"/>
+      <c r="AM3" s="61"/>
+      <c r="AN3" s="61"/>
+      <c r="AO3" s="62"/>
+      <c r="AP3" s="60" t="str">
         <f t="shared" ref="AP3" si="4">DEC2HEX(AP2)</f>
         <v>5</v>
       </c>
-      <c r="AQ3" s="60"/>
-      <c r="AR3" s="60"/>
-      <c r="AS3" s="60"/>
-      <c r="AT3" s="60"/>
-      <c r="AU3" s="60"/>
-      <c r="AV3" s="60"/>
-      <c r="AW3" s="61"/>
-      <c r="AX3" s="59" t="str">
+      <c r="AQ3" s="61"/>
+      <c r="AR3" s="61"/>
+      <c r="AS3" s="61"/>
+      <c r="AT3" s="61"/>
+      <c r="AU3" s="61"/>
+      <c r="AV3" s="61"/>
+      <c r="AW3" s="62"/>
+      <c r="AX3" s="60" t="str">
         <f t="shared" ref="AX3" si="5">DEC2HEX(AX2)</f>
         <v>6</v>
       </c>
-      <c r="AY3" s="60"/>
-      <c r="AZ3" s="60"/>
-      <c r="BA3" s="60"/>
-      <c r="BB3" s="60"/>
-      <c r="BC3" s="60"/>
-      <c r="BD3" s="60"/>
-      <c r="BE3" s="61"/>
-      <c r="BF3" s="59" t="str">
+      <c r="AY3" s="61"/>
+      <c r="AZ3" s="61"/>
+      <c r="BA3" s="61"/>
+      <c r="BB3" s="61"/>
+      <c r="BC3" s="61"/>
+      <c r="BD3" s="61"/>
+      <c r="BE3" s="62"/>
+      <c r="BF3" s="60" t="str">
         <f t="shared" ref="BF3" si="6">DEC2HEX(BF2)</f>
         <v>7</v>
       </c>
-      <c r="BG3" s="60"/>
-      <c r="BH3" s="60"/>
-      <c r="BI3" s="60"/>
-      <c r="BJ3" s="60"/>
-      <c r="BK3" s="60"/>
-      <c r="BL3" s="60"/>
-      <c r="BM3" s="61"/>
-      <c r="BN3" s="59" t="str">
+      <c r="BG3" s="61"/>
+      <c r="BH3" s="61"/>
+      <c r="BI3" s="61"/>
+      <c r="BJ3" s="61"/>
+      <c r="BK3" s="61"/>
+      <c r="BL3" s="61"/>
+      <c r="BM3" s="62"/>
+      <c r="BN3" s="60" t="str">
         <f t="shared" ref="BN3" si="7">DEC2HEX(BN2)</f>
         <v>8</v>
       </c>
-      <c r="BO3" s="60"/>
-      <c r="BP3" s="60"/>
-      <c r="BQ3" s="60"/>
-      <c r="BR3" s="60"/>
-      <c r="BS3" s="60"/>
-      <c r="BT3" s="60"/>
-      <c r="BU3" s="61"/>
-      <c r="BV3" s="59" t="str">
+      <c r="BO3" s="61"/>
+      <c r="BP3" s="61"/>
+      <c r="BQ3" s="61"/>
+      <c r="BR3" s="61"/>
+      <c r="BS3" s="61"/>
+      <c r="BT3" s="61"/>
+      <c r="BU3" s="62"/>
+      <c r="BV3" s="60" t="str">
         <f t="shared" ref="BV3" si="8">DEC2HEX(BV2)</f>
         <v>9</v>
       </c>
-      <c r="BW3" s="60"/>
-      <c r="BX3" s="60"/>
-      <c r="BY3" s="60"/>
-      <c r="BZ3" s="60"/>
-      <c r="CA3" s="60"/>
-      <c r="CB3" s="60"/>
-      <c r="CC3" s="61"/>
-      <c r="CD3" s="59" t="str">
+      <c r="BW3" s="61"/>
+      <c r="BX3" s="61"/>
+      <c r="BY3" s="61"/>
+      <c r="BZ3" s="61"/>
+      <c r="CA3" s="61"/>
+      <c r="CB3" s="61"/>
+      <c r="CC3" s="62"/>
+      <c r="CD3" s="60" t="str">
         <f t="shared" ref="CD3" si="9">DEC2HEX(CD2)</f>
         <v>A</v>
       </c>
-      <c r="CE3" s="60"/>
-      <c r="CF3" s="60"/>
-      <c r="CG3" s="60"/>
-      <c r="CH3" s="60"/>
-      <c r="CI3" s="60"/>
-      <c r="CJ3" s="60"/>
-      <c r="CK3" s="61"/>
-      <c r="CL3" s="59" t="str">
+      <c r="CE3" s="61"/>
+      <c r="CF3" s="61"/>
+      <c r="CG3" s="61"/>
+      <c r="CH3" s="61"/>
+      <c r="CI3" s="61"/>
+      <c r="CJ3" s="61"/>
+      <c r="CK3" s="62"/>
+      <c r="CL3" s="60" t="str">
         <f t="shared" ref="CL3" si="10">DEC2HEX(CL2)</f>
         <v>B</v>
       </c>
-      <c r="CM3" s="60"/>
-      <c r="CN3" s="60"/>
-      <c r="CO3" s="60"/>
-      <c r="CP3" s="60"/>
-      <c r="CQ3" s="60"/>
-      <c r="CR3" s="60"/>
-      <c r="CS3" s="61"/>
-      <c r="CT3" s="59" t="str">
+      <c r="CM3" s="61"/>
+      <c r="CN3" s="61"/>
+      <c r="CO3" s="61"/>
+      <c r="CP3" s="61"/>
+      <c r="CQ3" s="61"/>
+      <c r="CR3" s="61"/>
+      <c r="CS3" s="62"/>
+      <c r="CT3" s="60" t="str">
         <f t="shared" ref="CT3" si="11">DEC2HEX(CT2)</f>
         <v>C</v>
       </c>
-      <c r="CU3" s="60"/>
-      <c r="CV3" s="60"/>
-      <c r="CW3" s="60"/>
-      <c r="CX3" s="60"/>
-      <c r="CY3" s="60"/>
-      <c r="CZ3" s="60"/>
-      <c r="DA3" s="61"/>
-      <c r="DB3" s="59" t="str">
+      <c r="CU3" s="61"/>
+      <c r="CV3" s="61"/>
+      <c r="CW3" s="61"/>
+      <c r="CX3" s="61"/>
+      <c r="CY3" s="61"/>
+      <c r="CZ3" s="61"/>
+      <c r="DA3" s="62"/>
+      <c r="DB3" s="60" t="str">
         <f t="shared" ref="DB3" si="12">DEC2HEX(DB2)</f>
         <v>D</v>
       </c>
-      <c r="DC3" s="60"/>
-      <c r="DD3" s="60"/>
-      <c r="DE3" s="60"/>
-      <c r="DF3" s="60"/>
-      <c r="DG3" s="60"/>
-      <c r="DH3" s="60"/>
-      <c r="DI3" s="61"/>
-      <c r="DJ3" s="59" t="str">
+      <c r="DC3" s="61"/>
+      <c r="DD3" s="61"/>
+      <c r="DE3" s="61"/>
+      <c r="DF3" s="61"/>
+      <c r="DG3" s="61"/>
+      <c r="DH3" s="61"/>
+      <c r="DI3" s="62"/>
+      <c r="DJ3" s="60" t="str">
         <f t="shared" ref="DJ3" si="13">DEC2HEX(DJ2)</f>
         <v>E</v>
       </c>
-      <c r="DK3" s="60"/>
-      <c r="DL3" s="60"/>
-      <c r="DM3" s="60"/>
-      <c r="DN3" s="60"/>
-      <c r="DO3" s="60"/>
-      <c r="DP3" s="60"/>
-      <c r="DQ3" s="61"/>
-      <c r="DR3" s="59" t="str">
+      <c r="DK3" s="61"/>
+      <c r="DL3" s="61"/>
+      <c r="DM3" s="61"/>
+      <c r="DN3" s="61"/>
+      <c r="DO3" s="61"/>
+      <c r="DP3" s="61"/>
+      <c r="DQ3" s="62"/>
+      <c r="DR3" s="60" t="str">
         <f t="shared" ref="DR3" si="14">DEC2HEX(DR2)</f>
         <v>F</v>
       </c>
-      <c r="DS3" s="60"/>
-      <c r="DT3" s="60"/>
-      <c r="DU3" s="60"/>
-      <c r="DV3" s="60"/>
-      <c r="DW3" s="60"/>
-      <c r="DX3" s="60"/>
-      <c r="DY3" s="61"/>
-      <c r="DZ3" s="59" t="str">
+      <c r="DS3" s="61"/>
+      <c r="DT3" s="61"/>
+      <c r="DU3" s="61"/>
+      <c r="DV3" s="61"/>
+      <c r="DW3" s="61"/>
+      <c r="DX3" s="61"/>
+      <c r="DY3" s="62"/>
+      <c r="DZ3" s="60" t="str">
         <f t="shared" ref="DZ3" si="15">DEC2HEX(DZ2)</f>
         <v>10</v>
       </c>
-      <c r="EA3" s="60"/>
-      <c r="EB3" s="60"/>
-      <c r="EC3" s="60"/>
-      <c r="ED3" s="60"/>
-      <c r="EE3" s="60"/>
-      <c r="EF3" s="60"/>
-      <c r="EG3" s="61"/>
-      <c r="EH3" s="59" t="str">
+      <c r="EA3" s="61"/>
+      <c r="EB3" s="61"/>
+      <c r="EC3" s="61"/>
+      <c r="ED3" s="61"/>
+      <c r="EE3" s="61"/>
+      <c r="EF3" s="61"/>
+      <c r="EG3" s="62"/>
+      <c r="EH3" s="60" t="str">
         <f t="shared" ref="EH3" si="16">DEC2HEX(EH2)</f>
         <v>11</v>
       </c>
-      <c r="EI3" s="60"/>
-      <c r="EJ3" s="60"/>
-      <c r="EK3" s="60"/>
-      <c r="EL3" s="60"/>
-      <c r="EM3" s="60"/>
-      <c r="EN3" s="60"/>
-      <c r="EO3" s="61"/>
-      <c r="EP3" s="59" t="str">
+      <c r="EI3" s="61"/>
+      <c r="EJ3" s="61"/>
+      <c r="EK3" s="61"/>
+      <c r="EL3" s="61"/>
+      <c r="EM3" s="61"/>
+      <c r="EN3" s="61"/>
+      <c r="EO3" s="62"/>
+      <c r="EP3" s="60" t="str">
         <f t="shared" ref="EP3" si="17">DEC2HEX(EP2)</f>
         <v>12</v>
       </c>
-      <c r="EQ3" s="60"/>
-      <c r="ER3" s="60"/>
-      <c r="ES3" s="60"/>
-      <c r="ET3" s="60"/>
-      <c r="EU3" s="60"/>
-      <c r="EV3" s="60"/>
-      <c r="EW3" s="61"/>
-      <c r="EX3" s="59" t="str">
+      <c r="EQ3" s="61"/>
+      <c r="ER3" s="61"/>
+      <c r="ES3" s="61"/>
+      <c r="ET3" s="61"/>
+      <c r="EU3" s="61"/>
+      <c r="EV3" s="61"/>
+      <c r="EW3" s="62"/>
+      <c r="EX3" s="60" t="str">
         <f t="shared" ref="EX3" si="18">DEC2HEX(EX2)</f>
         <v>13</v>
       </c>
-      <c r="EY3" s="60"/>
-      <c r="EZ3" s="60"/>
-      <c r="FA3" s="60"/>
-      <c r="FB3" s="60"/>
-      <c r="FC3" s="60"/>
-      <c r="FD3" s="60"/>
-      <c r="FE3" s="61"/>
-      <c r="FF3" s="59" t="str">
+      <c r="EY3" s="61"/>
+      <c r="EZ3" s="61"/>
+      <c r="FA3" s="61"/>
+      <c r="FB3" s="61"/>
+      <c r="FC3" s="61"/>
+      <c r="FD3" s="61"/>
+      <c r="FE3" s="62"/>
+      <c r="FF3" s="60" t="str">
         <f t="shared" ref="FF3" si="19">DEC2HEX(FF2)</f>
         <v>14</v>
       </c>
-      <c r="FG3" s="60"/>
-      <c r="FH3" s="60"/>
-      <c r="FI3" s="60"/>
-      <c r="FJ3" s="60"/>
-      <c r="FK3" s="60"/>
-      <c r="FL3" s="60"/>
-      <c r="FM3" s="61"/>
-      <c r="FN3" s="59" t="str">
+      <c r="FG3" s="61"/>
+      <c r="FH3" s="61"/>
+      <c r="FI3" s="61"/>
+      <c r="FJ3" s="61"/>
+      <c r="FK3" s="61"/>
+      <c r="FL3" s="61"/>
+      <c r="FM3" s="62"/>
+      <c r="FN3" s="60" t="str">
         <f t="shared" ref="FN3" si="20">DEC2HEX(FN2)</f>
         <v>15</v>
       </c>
-      <c r="FO3" s="60"/>
-      <c r="FP3" s="60"/>
-      <c r="FQ3" s="60"/>
-      <c r="FR3" s="60"/>
-      <c r="FS3" s="60"/>
-      <c r="FT3" s="60"/>
-      <c r="FU3" s="61"/>
-      <c r="FV3" s="59" t="str">
+      <c r="FO3" s="61"/>
+      <c r="FP3" s="61"/>
+      <c r="FQ3" s="61"/>
+      <c r="FR3" s="61"/>
+      <c r="FS3" s="61"/>
+      <c r="FT3" s="61"/>
+      <c r="FU3" s="62"/>
+      <c r="FV3" s="60" t="str">
         <f t="shared" ref="FV3" si="21">DEC2HEX(FV2)</f>
         <v>16</v>
       </c>
-      <c r="FW3" s="60"/>
-      <c r="FX3" s="60"/>
-      <c r="FY3" s="60"/>
-      <c r="FZ3" s="60"/>
-      <c r="GA3" s="60"/>
-      <c r="GB3" s="60"/>
-      <c r="GC3" s="61"/>
-      <c r="GD3" s="59" t="str">
+      <c r="FW3" s="61"/>
+      <c r="FX3" s="61"/>
+      <c r="FY3" s="61"/>
+      <c r="FZ3" s="61"/>
+      <c r="GA3" s="61"/>
+      <c r="GB3" s="61"/>
+      <c r="GC3" s="62"/>
+      <c r="GD3" s="60" t="str">
         <f t="shared" ref="GD3" si="22">DEC2HEX(GD2)</f>
         <v>17</v>
       </c>
-      <c r="GE3" s="60"/>
-      <c r="GF3" s="60"/>
-      <c r="GG3" s="60"/>
-      <c r="GH3" s="60"/>
-      <c r="GI3" s="60"/>
-      <c r="GJ3" s="60"/>
-      <c r="GK3" s="61"/>
-      <c r="GL3" s="59" t="str">
+      <c r="GE3" s="61"/>
+      <c r="GF3" s="61"/>
+      <c r="GG3" s="61"/>
+      <c r="GH3" s="61"/>
+      <c r="GI3" s="61"/>
+      <c r="GJ3" s="61"/>
+      <c r="GK3" s="62"/>
+      <c r="GL3" s="60" t="str">
         <f t="shared" ref="GL3" si="23">DEC2HEX(GL2)</f>
         <v>18</v>
       </c>
-      <c r="GM3" s="60"/>
-      <c r="GN3" s="60"/>
-      <c r="GO3" s="60"/>
-      <c r="GP3" s="60"/>
-      <c r="GQ3" s="60"/>
-      <c r="GR3" s="60"/>
-      <c r="GS3" s="61"/>
-      <c r="GT3" s="59" t="str">
+      <c r="GM3" s="61"/>
+      <c r="GN3" s="61"/>
+      <c r="GO3" s="61"/>
+      <c r="GP3" s="61"/>
+      <c r="GQ3" s="61"/>
+      <c r="GR3" s="61"/>
+      <c r="GS3" s="62"/>
+      <c r="GT3" s="60" t="str">
         <f t="shared" ref="GT3" si="24">DEC2HEX(GT2)</f>
         <v>19</v>
       </c>
-      <c r="GU3" s="60"/>
-      <c r="GV3" s="60"/>
-      <c r="GW3" s="60"/>
-      <c r="GX3" s="60"/>
-      <c r="GY3" s="60"/>
-      <c r="GZ3" s="60"/>
-      <c r="HA3" s="61"/>
-      <c r="HB3" s="59" t="str">
+      <c r="GU3" s="61"/>
+      <c r="GV3" s="61"/>
+      <c r="GW3" s="61"/>
+      <c r="GX3" s="61"/>
+      <c r="GY3" s="61"/>
+      <c r="GZ3" s="61"/>
+      <c r="HA3" s="62"/>
+      <c r="HB3" s="60" t="str">
         <f t="shared" ref="HB3" si="25">DEC2HEX(HB2)</f>
         <v>1A</v>
       </c>
-      <c r="HC3" s="60"/>
-      <c r="HD3" s="60"/>
-      <c r="HE3" s="60"/>
-      <c r="HF3" s="60"/>
-      <c r="HG3" s="60"/>
-      <c r="HH3" s="60"/>
-      <c r="HI3" s="61"/>
+      <c r="HC3" s="61"/>
+      <c r="HD3" s="61"/>
+      <c r="HE3" s="61"/>
+      <c r="HF3" s="61"/>
+      <c r="HG3" s="61"/>
+      <c r="HH3" s="61"/>
+      <c r="HI3" s="62"/>
     </row>
     <row r="4" spans="1:217" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="60">
         <v>0</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="59">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="60">
         <v>2</v>
       </c>
-      <c r="S4" s="60"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="60"/>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60"/>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="60"/>
-      <c r="Z4" s="60"/>
-      <c r="AA4" s="60"/>
-      <c r="AB4" s="60"/>
-      <c r="AC4" s="60"/>
-      <c r="AD4" s="60"/>
-      <c r="AE4" s="60"/>
-      <c r="AF4" s="60"/>
-      <c r="AG4" s="61"/>
-      <c r="AH4" s="59">
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="61"/>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="61"/>
+      <c r="AC4" s="61"/>
+      <c r="AD4" s="61"/>
+      <c r="AE4" s="61"/>
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="62"/>
+      <c r="AH4" s="60">
         <v>4</v>
       </c>
-      <c r="AI4" s="60"/>
-      <c r="AJ4" s="60"/>
-      <c r="AK4" s="60"/>
-      <c r="AL4" s="60"/>
-      <c r="AM4" s="60"/>
-      <c r="AN4" s="60"/>
-      <c r="AO4" s="60"/>
-      <c r="AP4" s="60"/>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="60"/>
-      <c r="AS4" s="60"/>
-      <c r="AT4" s="60"/>
-      <c r="AU4" s="60"/>
-      <c r="AV4" s="60"/>
-      <c r="AW4" s="61"/>
-      <c r="AX4" s="59">
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="61"/>
+      <c r="AM4" s="61"/>
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="61"/>
+      <c r="AP4" s="61"/>
+      <c r="AQ4" s="61"/>
+      <c r="AR4" s="61"/>
+      <c r="AS4" s="61"/>
+      <c r="AT4" s="61"/>
+      <c r="AU4" s="61"/>
+      <c r="AV4" s="61"/>
+      <c r="AW4" s="62"/>
+      <c r="AX4" s="60">
         <v>6</v>
       </c>
-      <c r="AY4" s="60"/>
-      <c r="AZ4" s="60"/>
-      <c r="BA4" s="60"/>
-      <c r="BB4" s="60"/>
-      <c r="BC4" s="60"/>
-      <c r="BD4" s="60"/>
-      <c r="BE4" s="60"/>
-      <c r="BF4" s="60"/>
-      <c r="BG4" s="60"/>
-      <c r="BH4" s="60"/>
-      <c r="BI4" s="60"/>
-      <c r="BJ4" s="60"/>
-      <c r="BK4" s="60"/>
-      <c r="BL4" s="60"/>
-      <c r="BM4" s="61"/>
-      <c r="BN4" s="59">
+      <c r="AY4" s="61"/>
+      <c r="AZ4" s="61"/>
+      <c r="BA4" s="61"/>
+      <c r="BB4" s="61"/>
+      <c r="BC4" s="61"/>
+      <c r="BD4" s="61"/>
+      <c r="BE4" s="61"/>
+      <c r="BF4" s="61"/>
+      <c r="BG4" s="61"/>
+      <c r="BH4" s="61"/>
+      <c r="BI4" s="61"/>
+      <c r="BJ4" s="61"/>
+      <c r="BK4" s="61"/>
+      <c r="BL4" s="61"/>
+      <c r="BM4" s="62"/>
+      <c r="BN4" s="60">
         <v>8</v>
       </c>
-      <c r="BO4" s="60"/>
-      <c r="BP4" s="60"/>
-      <c r="BQ4" s="60"/>
-      <c r="BR4" s="60"/>
-      <c r="BS4" s="60"/>
-      <c r="BT4" s="60"/>
-      <c r="BU4" s="61"/>
-      <c r="BV4" s="59">
+      <c r="BO4" s="61"/>
+      <c r="BP4" s="61"/>
+      <c r="BQ4" s="61"/>
+      <c r="BR4" s="61"/>
+      <c r="BS4" s="61"/>
+      <c r="BT4" s="61"/>
+      <c r="BU4" s="62"/>
+      <c r="BV4" s="60">
         <v>9</v>
       </c>
-      <c r="BW4" s="60"/>
-      <c r="BX4" s="60"/>
-      <c r="BY4" s="60"/>
-      <c r="BZ4" s="60"/>
-      <c r="CA4" s="60"/>
-      <c r="CB4" s="60"/>
-      <c r="CC4" s="61"/>
-      <c r="CD4" s="59" t="str">
+      <c r="BW4" s="61"/>
+      <c r="BX4" s="61"/>
+      <c r="BY4" s="61"/>
+      <c r="BZ4" s="61"/>
+      <c r="CA4" s="61"/>
+      <c r="CB4" s="61"/>
+      <c r="CC4" s="62"/>
+      <c r="CD4" s="60" t="str">
         <f>CD3</f>
         <v>A</v>
       </c>
-      <c r="CE4" s="60"/>
-      <c r="CF4" s="60"/>
-      <c r="CG4" s="60"/>
-      <c r="CH4" s="60"/>
-      <c r="CI4" s="60"/>
-      <c r="CJ4" s="60"/>
-      <c r="CK4" s="61"/>
-      <c r="CL4" s="59" t="str">
+      <c r="CE4" s="61"/>
+      <c r="CF4" s="61"/>
+      <c r="CG4" s="61"/>
+      <c r="CH4" s="61"/>
+      <c r="CI4" s="61"/>
+      <c r="CJ4" s="61"/>
+      <c r="CK4" s="62"/>
+      <c r="CL4" s="60" t="str">
         <f>CL3</f>
         <v>B</v>
       </c>
-      <c r="CM4" s="60"/>
-      <c r="CN4" s="60"/>
-      <c r="CO4" s="60"/>
-      <c r="CP4" s="60"/>
-      <c r="CQ4" s="60"/>
-      <c r="CR4" s="60"/>
-      <c r="CS4" s="60"/>
-      <c r="CT4" s="60"/>
-      <c r="CU4" s="60"/>
-      <c r="CV4" s="60"/>
-      <c r="CW4" s="60"/>
-      <c r="CX4" s="60"/>
-      <c r="CY4" s="60"/>
-      <c r="CZ4" s="60"/>
-      <c r="DA4" s="61"/>
-      <c r="DB4" s="59" t="str">
+      <c r="CM4" s="61"/>
+      <c r="CN4" s="61"/>
+      <c r="CO4" s="61"/>
+      <c r="CP4" s="61"/>
+      <c r="CQ4" s="61"/>
+      <c r="CR4" s="61"/>
+      <c r="CS4" s="61"/>
+      <c r="CT4" s="61"/>
+      <c r="CU4" s="61"/>
+      <c r="CV4" s="61"/>
+      <c r="CW4" s="61"/>
+      <c r="CX4" s="61"/>
+      <c r="CY4" s="61"/>
+      <c r="CZ4" s="61"/>
+      <c r="DA4" s="62"/>
+      <c r="DB4" s="60" t="str">
         <f>DB3</f>
         <v>D</v>
       </c>
-      <c r="DC4" s="60"/>
-      <c r="DD4" s="60"/>
-      <c r="DE4" s="60"/>
-      <c r="DF4" s="60"/>
-      <c r="DG4" s="60"/>
-      <c r="DH4" s="60"/>
-      <c r="DI4" s="60"/>
-      <c r="DJ4" s="60"/>
-      <c r="DK4" s="60"/>
-      <c r="DL4" s="60"/>
-      <c r="DM4" s="60"/>
-      <c r="DN4" s="60"/>
-      <c r="DO4" s="60"/>
-      <c r="DP4" s="60"/>
-      <c r="DQ4" s="61"/>
-      <c r="DR4" s="59" t="str">
+      <c r="DC4" s="61"/>
+      <c r="DD4" s="61"/>
+      <c r="DE4" s="61"/>
+      <c r="DF4" s="61"/>
+      <c r="DG4" s="61"/>
+      <c r="DH4" s="61"/>
+      <c r="DI4" s="61"/>
+      <c r="DJ4" s="61"/>
+      <c r="DK4" s="61"/>
+      <c r="DL4" s="61"/>
+      <c r="DM4" s="61"/>
+      <c r="DN4" s="61"/>
+      <c r="DO4" s="61"/>
+      <c r="DP4" s="61"/>
+      <c r="DQ4" s="62"/>
+      <c r="DR4" s="60" t="str">
         <f t="shared" ref="DR4" si="26">DR3</f>
         <v>F</v>
       </c>
-      <c r="DS4" s="60"/>
-      <c r="DT4" s="60"/>
-      <c r="DU4" s="60"/>
-      <c r="DV4" s="60"/>
-      <c r="DW4" s="60"/>
-      <c r="DX4" s="60"/>
-      <c r="DY4" s="60"/>
-      <c r="DZ4" s="60"/>
-      <c r="EA4" s="60"/>
-      <c r="EB4" s="60"/>
-      <c r="EC4" s="60"/>
-      <c r="ED4" s="60"/>
-      <c r="EE4" s="60"/>
-      <c r="EF4" s="60"/>
-      <c r="EG4" s="61"/>
-      <c r="EH4" s="59" t="str">
+      <c r="DS4" s="61"/>
+      <c r="DT4" s="61"/>
+      <c r="DU4" s="61"/>
+      <c r="DV4" s="61"/>
+      <c r="DW4" s="61"/>
+      <c r="DX4" s="61"/>
+      <c r="DY4" s="61"/>
+      <c r="DZ4" s="61"/>
+      <c r="EA4" s="61"/>
+      <c r="EB4" s="61"/>
+      <c r="EC4" s="61"/>
+      <c r="ED4" s="61"/>
+      <c r="EE4" s="61"/>
+      <c r="EF4" s="61"/>
+      <c r="EG4" s="62"/>
+      <c r="EH4" s="60" t="str">
         <f t="shared" ref="EH4" si="27">EH3</f>
         <v>11</v>
       </c>
-      <c r="EI4" s="60"/>
-      <c r="EJ4" s="60"/>
-      <c r="EK4" s="60"/>
-      <c r="EL4" s="60"/>
-      <c r="EM4" s="60"/>
-      <c r="EN4" s="60"/>
-      <c r="EO4" s="61"/>
-      <c r="EP4" s="59" t="str">
+      <c r="EI4" s="61"/>
+      <c r="EJ4" s="61"/>
+      <c r="EK4" s="61"/>
+      <c r="EL4" s="61"/>
+      <c r="EM4" s="61"/>
+      <c r="EN4" s="61"/>
+      <c r="EO4" s="62"/>
+      <c r="EP4" s="60" t="str">
         <f t="shared" ref="EP4" si="28">EP3</f>
         <v>12</v>
       </c>
-      <c r="EQ4" s="60"/>
-      <c r="ER4" s="60"/>
-      <c r="ES4" s="60"/>
-      <c r="ET4" s="60"/>
-      <c r="EU4" s="60"/>
-      <c r="EV4" s="60"/>
-      <c r="EW4" s="61"/>
-      <c r="EX4" s="59" t="str">
+      <c r="EQ4" s="61"/>
+      <c r="ER4" s="61"/>
+      <c r="ES4" s="61"/>
+      <c r="ET4" s="61"/>
+      <c r="EU4" s="61"/>
+      <c r="EV4" s="61"/>
+      <c r="EW4" s="62"/>
+      <c r="EX4" s="60" t="str">
         <f t="shared" ref="EX4" si="29">EX3</f>
         <v>13</v>
       </c>
-      <c r="EY4" s="60"/>
-      <c r="EZ4" s="60"/>
-      <c r="FA4" s="60"/>
-      <c r="FB4" s="60"/>
-      <c r="FC4" s="60"/>
-      <c r="FD4" s="60"/>
-      <c r="FE4" s="61"/>
-      <c r="FF4" s="59" t="str">
+      <c r="EY4" s="61"/>
+      <c r="EZ4" s="61"/>
+      <c r="FA4" s="61"/>
+      <c r="FB4" s="61"/>
+      <c r="FC4" s="61"/>
+      <c r="FD4" s="61"/>
+      <c r="FE4" s="62"/>
+      <c r="FF4" s="60" t="str">
         <f t="shared" ref="FF4" si="30">FF3</f>
         <v>14</v>
       </c>
-      <c r="FG4" s="60"/>
-      <c r="FH4" s="60"/>
-      <c r="FI4" s="60"/>
-      <c r="FJ4" s="60"/>
-      <c r="FK4" s="60"/>
-      <c r="FL4" s="60"/>
-      <c r="FM4" s="61"/>
-      <c r="FN4" s="59" t="str">
+      <c r="FG4" s="61"/>
+      <c r="FH4" s="61"/>
+      <c r="FI4" s="61"/>
+      <c r="FJ4" s="61"/>
+      <c r="FK4" s="61"/>
+      <c r="FL4" s="61"/>
+      <c r="FM4" s="62"/>
+      <c r="FN4" s="60" t="str">
         <f t="shared" ref="FN4" si="31">FN3</f>
         <v>15</v>
       </c>
-      <c r="FO4" s="60"/>
-      <c r="FP4" s="60"/>
-      <c r="FQ4" s="60"/>
-      <c r="FR4" s="60"/>
-      <c r="FS4" s="60"/>
-      <c r="FT4" s="60"/>
-      <c r="FU4" s="61"/>
-      <c r="FV4" s="59" t="str">
+      <c r="FO4" s="61"/>
+      <c r="FP4" s="61"/>
+      <c r="FQ4" s="61"/>
+      <c r="FR4" s="61"/>
+      <c r="FS4" s="61"/>
+      <c r="FT4" s="61"/>
+      <c r="FU4" s="62"/>
+      <c r="FV4" s="60" t="str">
         <f t="shared" ref="FV4" si="32">FV3</f>
         <v>16</v>
       </c>
-      <c r="FW4" s="60"/>
-      <c r="FX4" s="60"/>
-      <c r="FY4" s="60"/>
-      <c r="FZ4" s="60"/>
-      <c r="GA4" s="60"/>
-      <c r="GB4" s="60"/>
-      <c r="GC4" s="60"/>
-      <c r="GD4" s="60"/>
-      <c r="GE4" s="60"/>
-      <c r="GF4" s="60"/>
-      <c r="GG4" s="60"/>
-      <c r="GH4" s="60"/>
-      <c r="GI4" s="60"/>
-      <c r="GJ4" s="60"/>
-      <c r="GK4" s="61"/>
-      <c r="GL4" s="59" t="str">
+      <c r="FW4" s="61"/>
+      <c r="FX4" s="61"/>
+      <c r="FY4" s="61"/>
+      <c r="FZ4" s="61"/>
+      <c r="GA4" s="61"/>
+      <c r="GB4" s="61"/>
+      <c r="GC4" s="61"/>
+      <c r="GD4" s="61"/>
+      <c r="GE4" s="61"/>
+      <c r="GF4" s="61"/>
+      <c r="GG4" s="61"/>
+      <c r="GH4" s="61"/>
+      <c r="GI4" s="61"/>
+      <c r="GJ4" s="61"/>
+      <c r="GK4" s="62"/>
+      <c r="GL4" s="60" t="str">
         <f t="shared" ref="GL4" si="33">GL3</f>
         <v>18</v>
       </c>
-      <c r="GM4" s="60"/>
-      <c r="GN4" s="60"/>
-      <c r="GO4" s="60"/>
-      <c r="GP4" s="60"/>
-      <c r="GQ4" s="60"/>
-      <c r="GR4" s="60"/>
-      <c r="GS4" s="61"/>
-      <c r="GT4" s="59" t="str">
+      <c r="GM4" s="61"/>
+      <c r="GN4" s="61"/>
+      <c r="GO4" s="61"/>
+      <c r="GP4" s="61"/>
+      <c r="GQ4" s="61"/>
+      <c r="GR4" s="61"/>
+      <c r="GS4" s="62"/>
+      <c r="GT4" s="60" t="str">
         <f t="shared" ref="GT4" si="34">GT3</f>
         <v>19</v>
       </c>
-      <c r="GU4" s="60"/>
-      <c r="GV4" s="60"/>
-      <c r="GW4" s="60"/>
-      <c r="GX4" s="60"/>
-      <c r="GY4" s="60"/>
-      <c r="GZ4" s="60"/>
-      <c r="HA4" s="61"/>
-      <c r="HB4" s="59" t="str">
+      <c r="GU4" s="61"/>
+      <c r="GV4" s="61"/>
+      <c r="GW4" s="61"/>
+      <c r="GX4" s="61"/>
+      <c r="GY4" s="61"/>
+      <c r="GZ4" s="61"/>
+      <c r="HA4" s="62"/>
+      <c r="HB4" s="60" t="str">
         <f t="shared" ref="HB4" si="35">HB3</f>
         <v>1A</v>
       </c>
-      <c r="HC4" s="60"/>
-      <c r="HD4" s="60"/>
-      <c r="HE4" s="60"/>
-      <c r="HF4" s="60"/>
-      <c r="HG4" s="60"/>
-      <c r="HH4" s="60"/>
-      <c r="HI4" s="61"/>
+      <c r="HC4" s="61"/>
+      <c r="HD4" s="61"/>
+      <c r="HE4" s="61"/>
+      <c r="HF4" s="61"/>
+      <c r="HG4" s="61"/>
+      <c r="HH4" s="61"/>
+      <c r="HI4" s="62"/>
     </row>
     <row r="5" spans="1:217" ht="14.65" hidden="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
@@ -4981,7 +4992,7 @@
       <c r="CJ7" s="77"/>
       <c r="CK7" s="84"/>
       <c r="CL7" s="85" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="CM7" s="86"/>
       <c r="CN7" s="86"/>
@@ -5010,11 +5021,11 @@
         <v>29</v>
       </c>
       <c r="DE7" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="DF7" s="27"/>
       <c r="DG7" s="54" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="DH7" s="28"/>
       <c r="DI7" s="28"/>
@@ -5029,7 +5040,7 @@
       <c r="DP7" s="93"/>
       <c r="DQ7" s="94"/>
       <c r="DR7" s="72" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DS7" s="73"/>
       <c r="DT7" s="73"/>
@@ -5043,23 +5054,23 @@
       <c r="DZ7" s="104"/>
       <c r="EA7" s="105"/>
       <c r="EB7" s="106" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="EC7" s="104"/>
       <c r="ED7" s="104"/>
       <c r="EE7" s="104"/>
       <c r="EF7" s="104"/>
       <c r="EG7" s="105"/>
-      <c r="EH7" s="59" t="s">
+      <c r="EH7" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="EI7" s="60"/>
-      <c r="EJ7" s="60"/>
-      <c r="EK7" s="60"/>
-      <c r="EL7" s="60"/>
-      <c r="EM7" s="60"/>
-      <c r="EN7" s="60"/>
-      <c r="EO7" s="61"/>
+      <c r="EI7" s="61"/>
+      <c r="EJ7" s="61"/>
+      <c r="EK7" s="61"/>
+      <c r="EL7" s="61"/>
+      <c r="EM7" s="61"/>
+      <c r="EN7" s="61"/>
+      <c r="EO7" s="62"/>
       <c r="EP7" s="89" t="s">
         <v>48</v>
       </c>
@@ -5097,7 +5108,7 @@
       <c r="FN7" s="38"/>
       <c r="FO7" s="39"/>
       <c r="FP7" s="120" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="FQ7" s="121"/>
       <c r="FR7" s="121"/>
@@ -5120,17 +5131,17 @@
       <c r="GE7" s="73"/>
       <c r="GF7" s="73"/>
       <c r="GG7" s="74"/>
-      <c r="GH7" s="59" t="s">
+      <c r="GH7" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="GI7" s="60"/>
-      <c r="GJ7" s="60"/>
-      <c r="GK7" s="61"/>
-      <c r="GL7" s="59" t="s">
+      <c r="GI7" s="61"/>
+      <c r="GJ7" s="61"/>
+      <c r="GK7" s="62"/>
+      <c r="GL7" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="GM7" s="60"/>
-      <c r="GN7" s="61"/>
+      <c r="GM7" s="61"/>
+      <c r="GN7" s="62"/>
       <c r="GO7" s="72" t="s">
         <v>41</v>
       </c>
@@ -5142,14 +5153,14 @@
         <v>44</v>
       </c>
       <c r="GU7" s="2"/>
-      <c r="GV7" s="63" t="s">
+      <c r="GV7" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="GW7" s="64"/>
-      <c r="GX7" s="64"/>
-      <c r="GY7" s="64"/>
-      <c r="GZ7" s="64"/>
-      <c r="HA7" s="65"/>
+      <c r="GW7" s="65"/>
+      <c r="GX7" s="65"/>
+      <c r="GY7" s="65"/>
+      <c r="GZ7" s="65"/>
+      <c r="HA7" s="66"/>
       <c r="HB7" s="72" t="s">
         <v>45</v>
       </c>
@@ -5211,70 +5222,70 @@
       <c r="CI8" s="44"/>
       <c r="CJ8" s="44"/>
       <c r="CK8" s="45"/>
-      <c r="CL8" s="65" t="s">
+      <c r="CL8" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="CM8" s="62"/>
-      <c r="CN8" s="62"/>
-      <c r="CO8" s="62"/>
-      <c r="CP8" s="62"/>
-      <c r="CQ8" s="62"/>
-      <c r="CR8" s="62"/>
-      <c r="CS8" s="62"/>
-      <c r="CT8" s="62"/>
-      <c r="CU8" s="62"/>
-      <c r="CV8" s="62"/>
-      <c r="CW8" s="62"/>
-      <c r="CX8" s="62"/>
-      <c r="CY8" s="62"/>
-      <c r="CZ8" s="62"/>
-      <c r="DA8" s="62"/>
-      <c r="DB8" s="62" t="s">
+      <c r="CM8" s="63"/>
+      <c r="CN8" s="63"/>
+      <c r="CO8" s="63"/>
+      <c r="CP8" s="63"/>
+      <c r="CQ8" s="63"/>
+      <c r="CR8" s="63"/>
+      <c r="CS8" s="63"/>
+      <c r="CT8" s="63"/>
+      <c r="CU8" s="63"/>
+      <c r="CV8" s="63"/>
+      <c r="CW8" s="63"/>
+      <c r="CX8" s="63"/>
+      <c r="CY8" s="63"/>
+      <c r="CZ8" s="63"/>
+      <c r="DA8" s="63"/>
+      <c r="DB8" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="DC8" s="62"/>
-      <c r="DD8" s="62"/>
-      <c r="DE8" s="62"/>
-      <c r="DF8" s="62"/>
+      <c r="DC8" s="63"/>
+      <c r="DD8" s="63"/>
+      <c r="DE8" s="63"/>
+      <c r="DF8" s="63"/>
       <c r="DG8" s="102"/>
-      <c r="DH8" s="62"/>
-      <c r="DI8" s="62"/>
-      <c r="DJ8" s="62"/>
-      <c r="DK8" s="62"/>
-      <c r="DL8" s="62"/>
-      <c r="DM8" s="62"/>
-      <c r="DN8" s="62"/>
-      <c r="DO8" s="62"/>
-      <c r="DP8" s="62"/>
-      <c r="DQ8" s="62"/>
-      <c r="DR8" s="62" t="s">
-        <v>237</v>
-      </c>
-      <c r="DS8" s="62"/>
-      <c r="DT8" s="62"/>
-      <c r="DU8" s="62"/>
-      <c r="DV8" s="62"/>
-      <c r="DW8" s="62"/>
-      <c r="DX8" s="62"/>
-      <c r="DY8" s="62"/>
-      <c r="DZ8" s="62"/>
-      <c r="EA8" s="62"/>
-      <c r="EB8" s="62"/>
-      <c r="EC8" s="62"/>
-      <c r="ED8" s="62"/>
-      <c r="EE8" s="62"/>
-      <c r="EF8" s="62"/>
-      <c r="EG8" s="62"/>
-      <c r="EH8" s="63" t="s">
-        <v>227</v>
-      </c>
-      <c r="EI8" s="64"/>
-      <c r="EJ8" s="64"/>
-      <c r="EK8" s="64"/>
-      <c r="EL8" s="64"/>
-      <c r="EM8" s="64"/>
-      <c r="EN8" s="64"/>
-      <c r="EO8" s="64"/>
+      <c r="DH8" s="63"/>
+      <c r="DI8" s="63"/>
+      <c r="DJ8" s="63"/>
+      <c r="DK8" s="63"/>
+      <c r="DL8" s="63"/>
+      <c r="DM8" s="63"/>
+      <c r="DN8" s="63"/>
+      <c r="DO8" s="63"/>
+      <c r="DP8" s="63"/>
+      <c r="DQ8" s="63"/>
+      <c r="DR8" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="DS8" s="63"/>
+      <c r="DT8" s="63"/>
+      <c r="DU8" s="63"/>
+      <c r="DV8" s="63"/>
+      <c r="DW8" s="63"/>
+      <c r="DX8" s="63"/>
+      <c r="DY8" s="63"/>
+      <c r="DZ8" s="63"/>
+      <c r="EA8" s="63"/>
+      <c r="EB8" s="63"/>
+      <c r="EC8" s="63"/>
+      <c r="ED8" s="63"/>
+      <c r="EE8" s="63"/>
+      <c r="EF8" s="63"/>
+      <c r="EG8" s="63"/>
+      <c r="EH8" s="64" t="s">
+        <v>225</v>
+      </c>
+      <c r="EI8" s="65"/>
+      <c r="EJ8" s="65"/>
+      <c r="EK8" s="65"/>
+      <c r="EL8" s="65"/>
+      <c r="EM8" s="65"/>
+      <c r="EN8" s="65"/>
+      <c r="EO8" s="65"/>
       <c r="FH8" t="s">
         <v>123</v>
       </c>
@@ -5337,7 +5348,7 @@
       <c r="V9" s="96"/>
       <c r="W9" s="97"/>
       <c r="X9" s="95" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Y9" s="96"/>
       <c r="Z9" s="97"/>
@@ -5363,7 +5374,7 @@
       <c r="AP9" s="96"/>
       <c r="AQ9" s="97"/>
       <c r="AR9" s="95" t="s">
-        <v>171</v>
+        <v>259</v>
       </c>
       <c r="AS9" s="96"/>
       <c r="AT9" s="96"/>
@@ -5383,7 +5394,7 @@
       <c r="BF9" s="96"/>
       <c r="BG9" s="97"/>
       <c r="BH9" s="95" t="s">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="BI9" s="96"/>
       <c r="BJ9" s="96"/>
@@ -5411,15 +5422,15 @@
       <c r="CB9" s="75"/>
       <c r="CC9" s="76"/>
       <c r="CD9" s="57" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="CE9" s="96" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="CF9" s="96"/>
       <c r="CG9" s="96"/>
       <c r="CH9" s="96" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="CI9" s="96"/>
       <c r="CJ9" s="96"/>
@@ -5427,59 +5438,59 @@
       <c r="CL9" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="CM9" s="75"/>
-      <c r="CN9" s="75"/>
-      <c r="CO9" s="75"/>
-      <c r="CP9" s="75"/>
-      <c r="CQ9" s="75"/>
-      <c r="CR9" s="75"/>
-      <c r="CS9" s="75"/>
-      <c r="CT9" s="75"/>
-      <c r="CU9" s="75"/>
-      <c r="CV9" s="75"/>
-      <c r="CW9" s="75"/>
-      <c r="CX9" s="75"/>
-      <c r="CY9" s="75"/>
-      <c r="CZ9" s="75"/>
-      <c r="DA9" s="75"/>
+      <c r="CM9" s="96"/>
+      <c r="CN9" s="96"/>
+      <c r="CO9" s="96"/>
+      <c r="CP9" s="96"/>
+      <c r="CQ9" s="96"/>
+      <c r="CR9" s="96"/>
+      <c r="CS9" s="96"/>
+      <c r="CT9" s="96"/>
+      <c r="CU9" s="96"/>
+      <c r="CV9" s="96"/>
+      <c r="CW9" s="96"/>
+      <c r="CX9" s="96"/>
+      <c r="CY9" s="96"/>
+      <c r="CZ9" s="96"/>
+      <c r="DA9" s="97"/>
       <c r="DB9" s="146" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="DC9" s="147"/>
       <c r="DD9" s="158" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="DE9" s="158" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="DF9" s="51"/>
       <c r="DG9" s="152" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="DH9" s="51"/>
       <c r="DI9" s="55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="DJ9" s="146" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="DK9" s="155"/>
       <c r="DL9" s="155"/>
       <c r="DM9" s="147"/>
       <c r="DN9" s="146" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="DO9" s="155"/>
       <c r="DP9" s="155"/>
       <c r="DQ9" s="147"/>
       <c r="DR9" s="133" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DS9" s="133"/>
       <c r="DT9" s="133"/>
       <c r="DU9" s="133"/>
       <c r="DV9" s="95" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="DW9" s="96"/>
       <c r="DX9" s="96"/>
@@ -5487,7 +5498,7 @@
       <c r="DZ9" s="96"/>
       <c r="EA9" s="97"/>
       <c r="EB9" s="95" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="EC9" s="96"/>
       <c r="ED9" s="96"/>
@@ -5495,7 +5506,7 @@
       <c r="EF9" s="96"/>
       <c r="EG9" s="97"/>
       <c r="EP9" s="95" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="EQ9" s="96"/>
       <c r="ER9" s="96"/>
@@ -5505,7 +5516,7 @@
       <c r="EV9" s="96"/>
       <c r="EW9" s="97"/>
       <c r="EX9" s="95" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="EY9" s="96"/>
       <c r="EZ9" s="96"/>
@@ -5515,10 +5526,10 @@
       <c r="FD9" s="96"/>
       <c r="FE9" s="97"/>
       <c r="FG9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="FK9" s="109" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="FL9" s="109"/>
       <c r="FM9" s="140"/>
@@ -5531,7 +5542,7 @@
       <c r="FR9" s="46"/>
       <c r="FU9" s="30"/>
       <c r="FV9" s="96" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="FW9" s="75"/>
       <c r="FX9" s="75"/>
@@ -5539,33 +5550,33 @@
       <c r="FZ9" s="75"/>
       <c r="GA9" s="76"/>
       <c r="GB9" s="95" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="GC9" s="75"/>
       <c r="GD9" s="75"/>
       <c r="GE9" s="75"/>
       <c r="GF9" s="75"/>
       <c r="GG9" s="76"/>
-      <c r="GH9" s="66" t="s">
-        <v>257</v>
-      </c>
-      <c r="GI9" s="67"/>
-      <c r="GJ9" s="67"/>
-      <c r="GK9" s="67"/>
+      <c r="GH9" s="67" t="s">
+        <v>255</v>
+      </c>
+      <c r="GI9" s="59"/>
+      <c r="GJ9" s="59"/>
+      <c r="GK9" s="59"/>
       <c r="GL9" s="113"/>
       <c r="GM9" s="113"/>
       <c r="GN9" s="115" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="GO9" s="95" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="GP9" s="96"/>
       <c r="GQ9" s="96"/>
       <c r="GR9" s="96"/>
       <c r="GS9" s="97"/>
       <c r="GT9" s="95" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="GU9" s="96"/>
       <c r="GV9" s="96"/>
@@ -5575,7 +5586,7 @@
       <c r="GZ9" s="96"/>
       <c r="HA9" s="98"/>
       <c r="HB9" s="95" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="HC9" s="96"/>
       <c r="HD9" s="96"/>
@@ -5588,11 +5599,11 @@
     <row r="10" spans="1:217" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="7"/>
       <c r="B10" s="134"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
       <c r="H10" s="135"/>
       <c r="I10" s="77"/>
       <c r="J10" s="77"/>
@@ -5603,53 +5614,53 @@
       <c r="O10" s="77"/>
       <c r="P10" s="77"/>
       <c r="Q10" s="78"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="67"/>
+      <c r="R10" s="67"/>
+      <c r="S10" s="59"/>
       <c r="T10" s="98"/>
-      <c r="U10" s="66"/>
-      <c r="V10" s="67"/>
+      <c r="U10" s="67"/>
+      <c r="V10" s="59"/>
       <c r="W10" s="98"/>
-      <c r="X10" s="66"/>
-      <c r="Y10" s="67"/>
+      <c r="X10" s="67"/>
+      <c r="Y10" s="59"/>
       <c r="Z10" s="98"/>
-      <c r="AA10" s="66"/>
-      <c r="AB10" s="67"/>
-      <c r="AC10" s="67"/>
-      <c r="AD10" s="67"/>
-      <c r="AE10" s="67"/>
-      <c r="AF10" s="67"/>
+      <c r="AA10" s="67"/>
+      <c r="AB10" s="59"/>
+      <c r="AC10" s="59"/>
+      <c r="AD10" s="59"/>
+      <c r="AE10" s="59"/>
+      <c r="AF10" s="59"/>
       <c r="AG10" s="98"/>
-      <c r="AH10" s="66"/>
-      <c r="AI10" s="67"/>
-      <c r="AJ10" s="67"/>
-      <c r="AK10" s="67"/>
-      <c r="AL10" s="67"/>
-      <c r="AM10" s="67"/>
-      <c r="AN10" s="67"/>
-      <c r="AO10" s="67"/>
-      <c r="AP10" s="67"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="59"/>
+      <c r="AJ10" s="59"/>
+      <c r="AK10" s="59"/>
+      <c r="AL10" s="59"/>
+      <c r="AM10" s="59"/>
+      <c r="AN10" s="59"/>
+      <c r="AO10" s="59"/>
+      <c r="AP10" s="59"/>
       <c r="AQ10" s="98"/>
-      <c r="AR10" s="66"/>
-      <c r="AS10" s="67"/>
-      <c r="AT10" s="67"/>
-      <c r="AU10" s="67"/>
-      <c r="AV10" s="67"/>
+      <c r="AR10" s="67"/>
+      <c r="AS10" s="59"/>
+      <c r="AT10" s="59"/>
+      <c r="AU10" s="59"/>
+      <c r="AV10" s="59"/>
       <c r="AW10" s="98"/>
-      <c r="AX10" s="67"/>
-      <c r="AY10" s="67"/>
-      <c r="AZ10" s="67"/>
-      <c r="BA10" s="67"/>
-      <c r="BB10" s="67"/>
-      <c r="BC10" s="67"/>
-      <c r="BD10" s="67"/>
-      <c r="BE10" s="67"/>
-      <c r="BF10" s="67"/>
+      <c r="AX10" s="59"/>
+      <c r="AY10" s="59"/>
+      <c r="AZ10" s="59"/>
+      <c r="BA10" s="59"/>
+      <c r="BB10" s="59"/>
+      <c r="BC10" s="59"/>
+      <c r="BD10" s="59"/>
+      <c r="BE10" s="59"/>
+      <c r="BF10" s="59"/>
       <c r="BG10" s="98"/>
-      <c r="BH10" s="66"/>
-      <c r="BI10" s="67"/>
-      <c r="BJ10" s="67"/>
-      <c r="BK10" s="67"/>
-      <c r="BL10" s="67"/>
+      <c r="BH10" s="67"/>
+      <c r="BI10" s="59"/>
+      <c r="BJ10" s="59"/>
+      <c r="BK10" s="59"/>
+      <c r="BL10" s="59"/>
       <c r="BM10" s="98"/>
       <c r="BN10" s="79"/>
       <c r="BO10" s="77"/>
@@ -5668,33 +5679,33 @@
       <c r="CB10" s="77"/>
       <c r="CC10" s="78"/>
       <c r="CD10" s="47" t="s">
-        <v>251</v>
-      </c>
-      <c r="CE10" s="67" t="s">
-        <v>259</v>
-      </c>
-      <c r="CF10" s="67"/>
-      <c r="CG10" s="67"/>
+        <v>249</v>
+      </c>
+      <c r="CE10" s="59" t="s">
+        <v>257</v>
+      </c>
+      <c r="CF10" s="59"/>
+      <c r="CG10" s="59"/>
       <c r="CH10" s="16"/>
       <c r="CI10" s="16"/>
       <c r="CJ10" s="16"/>
       <c r="CK10" s="48"/>
-      <c r="CL10" s="79"/>
-      <c r="CM10" s="77"/>
-      <c r="CN10" s="77"/>
-      <c r="CO10" s="77"/>
-      <c r="CP10" s="77"/>
-      <c r="CQ10" s="77"/>
-      <c r="CR10" s="77"/>
-      <c r="CS10" s="77"/>
-      <c r="CT10" s="77"/>
-      <c r="CU10" s="77"/>
-      <c r="CV10" s="77"/>
-      <c r="CW10" s="77"/>
-      <c r="CX10" s="77"/>
-      <c r="CY10" s="77"/>
-      <c r="CZ10" s="77"/>
-      <c r="DA10" s="77"/>
+      <c r="CL10" s="67"/>
+      <c r="CM10" s="59"/>
+      <c r="CN10" s="59"/>
+      <c r="CO10" s="59"/>
+      <c r="CP10" s="59"/>
+      <c r="CQ10" s="59"/>
+      <c r="CR10" s="59"/>
+      <c r="CS10" s="59"/>
+      <c r="CT10" s="59"/>
+      <c r="CU10" s="59"/>
+      <c r="CV10" s="59"/>
+      <c r="CW10" s="59"/>
+      <c r="CX10" s="59"/>
+      <c r="CY10" s="59"/>
+      <c r="CZ10" s="59"/>
+      <c r="DA10" s="98"/>
       <c r="DB10" s="148"/>
       <c r="DC10" s="149"/>
       <c r="DD10" s="159"/>
@@ -5715,33 +5726,33 @@
       <c r="DS10" s="16"/>
       <c r="DT10" s="16"/>
       <c r="DU10" s="16"/>
-      <c r="DV10" s="66"/>
-      <c r="DW10" s="67"/>
-      <c r="DX10" s="67"/>
-      <c r="DY10" s="67"/>
-      <c r="DZ10" s="67"/>
+      <c r="DV10" s="67"/>
+      <c r="DW10" s="59"/>
+      <c r="DX10" s="59"/>
+      <c r="DY10" s="59"/>
+      <c r="DZ10" s="59"/>
       <c r="EA10" s="98"/>
-      <c r="EB10" s="66"/>
-      <c r="EC10" s="67"/>
-      <c r="ED10" s="67"/>
-      <c r="EE10" s="67"/>
-      <c r="EF10" s="67"/>
+      <c r="EB10" s="67"/>
+      <c r="EC10" s="59"/>
+      <c r="ED10" s="59"/>
+      <c r="EE10" s="59"/>
+      <c r="EF10" s="59"/>
       <c r="EG10" s="98"/>
-      <c r="EP10" s="66"/>
-      <c r="EQ10" s="67"/>
-      <c r="ER10" s="67"/>
-      <c r="ES10" s="67"/>
-      <c r="ET10" s="67"/>
-      <c r="EU10" s="67"/>
-      <c r="EV10" s="67"/>
+      <c r="EP10" s="67"/>
+      <c r="EQ10" s="59"/>
+      <c r="ER10" s="59"/>
+      <c r="ES10" s="59"/>
+      <c r="ET10" s="59"/>
+      <c r="EU10" s="59"/>
+      <c r="EV10" s="59"/>
       <c r="EW10" s="98"/>
       <c r="EX10" s="17"/>
       <c r="EY10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="FE10" s="18"/>
       <c r="FK10" s="109" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="FL10" s="109"/>
       <c r="FM10" s="140"/>
@@ -5763,10 +5774,10 @@
       <c r="GE10" s="77"/>
       <c r="GF10" s="77"/>
       <c r="GG10" s="78"/>
-      <c r="GH10" s="66"/>
-      <c r="GI10" s="67"/>
-      <c r="GJ10" s="67"/>
-      <c r="GK10" s="67"/>
+      <c r="GH10" s="67"/>
+      <c r="GI10" s="59"/>
+      <c r="GJ10" s="59"/>
+      <c r="GK10" s="59"/>
       <c r="GL10" s="114"/>
       <c r="GM10" s="114"/>
       <c r="GN10" s="112"/>
@@ -5775,21 +5786,21 @@
       <c r="GQ10" s="100"/>
       <c r="GR10" s="100"/>
       <c r="GS10" s="101"/>
-      <c r="GT10" s="66"/>
-      <c r="GU10" s="67"/>
-      <c r="GV10" s="67"/>
-      <c r="GW10" s="67"/>
-      <c r="GX10" s="67"/>
-      <c r="GY10" s="67"/>
-      <c r="GZ10" s="67"/>
+      <c r="GT10" s="67"/>
+      <c r="GU10" s="59"/>
+      <c r="GV10" s="59"/>
+      <c r="GW10" s="59"/>
+      <c r="GX10" s="59"/>
+      <c r="GY10" s="59"/>
+      <c r="GZ10" s="59"/>
       <c r="HA10" s="98"/>
-      <c r="HB10" s="66"/>
-      <c r="HC10" s="67"/>
-      <c r="HD10" s="67"/>
-      <c r="HE10" s="67"/>
-      <c r="HF10" s="67"/>
-      <c r="HG10" s="67"/>
-      <c r="HH10" s="67"/>
+      <c r="HB10" s="67"/>
+      <c r="HC10" s="59"/>
+      <c r="HD10" s="59"/>
+      <c r="HE10" s="59"/>
+      <c r="HF10" s="59"/>
+      <c r="HG10" s="59"/>
+      <c r="HH10" s="59"/>
       <c r="HI10" s="98"/>
     </row>
     <row r="11" spans="1:217" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -5810,53 +5821,53 @@
       <c r="O11" s="77"/>
       <c r="P11" s="77"/>
       <c r="Q11" s="78"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="59"/>
       <c r="T11" s="98"/>
-      <c r="U11" s="66"/>
-      <c r="V11" s="67"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="59"/>
       <c r="W11" s="98"/>
-      <c r="X11" s="66"/>
-      <c r="Y11" s="67"/>
+      <c r="X11" s="67"/>
+      <c r="Y11" s="59"/>
       <c r="Z11" s="98"/>
-      <c r="AA11" s="66"/>
-      <c r="AB11" s="67"/>
-      <c r="AC11" s="67"/>
-      <c r="AD11" s="67"/>
-      <c r="AE11" s="67"/>
-      <c r="AF11" s="67"/>
+      <c r="AA11" s="67"/>
+      <c r="AB11" s="59"/>
+      <c r="AC11" s="59"/>
+      <c r="AD11" s="59"/>
+      <c r="AE11" s="59"/>
+      <c r="AF11" s="59"/>
       <c r="AG11" s="98"/>
-      <c r="AH11" s="66"/>
-      <c r="AI11" s="67"/>
-      <c r="AJ11" s="67"/>
-      <c r="AK11" s="67"/>
-      <c r="AL11" s="67"/>
-      <c r="AM11" s="67"/>
-      <c r="AN11" s="67"/>
-      <c r="AO11" s="67"/>
-      <c r="AP11" s="67"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="59"/>
+      <c r="AJ11" s="59"/>
+      <c r="AK11" s="59"/>
+      <c r="AL11" s="59"/>
+      <c r="AM11" s="59"/>
+      <c r="AN11" s="59"/>
+      <c r="AO11" s="59"/>
+      <c r="AP11" s="59"/>
       <c r="AQ11" s="98"/>
-      <c r="AR11" s="66"/>
-      <c r="AS11" s="67"/>
-      <c r="AT11" s="67"/>
-      <c r="AU11" s="67"/>
-      <c r="AV11" s="67"/>
+      <c r="AR11" s="67"/>
+      <c r="AS11" s="59"/>
+      <c r="AT11" s="59"/>
+      <c r="AU11" s="59"/>
+      <c r="AV11" s="59"/>
       <c r="AW11" s="98"/>
-      <c r="AX11" s="67"/>
-      <c r="AY11" s="67"/>
-      <c r="AZ11" s="67"/>
-      <c r="BA11" s="67"/>
-      <c r="BB11" s="67"/>
-      <c r="BC11" s="67"/>
-      <c r="BD11" s="67"/>
-      <c r="BE11" s="67"/>
-      <c r="BF11" s="67"/>
+      <c r="AX11" s="59"/>
+      <c r="AY11" s="59"/>
+      <c r="AZ11" s="59"/>
+      <c r="BA11" s="59"/>
+      <c r="BB11" s="59"/>
+      <c r="BC11" s="59"/>
+      <c r="BD11" s="59"/>
+      <c r="BE11" s="59"/>
+      <c r="BF11" s="59"/>
       <c r="BG11" s="98"/>
-      <c r="BH11" s="66"/>
-      <c r="BI11" s="67"/>
-      <c r="BJ11" s="67"/>
-      <c r="BK11" s="67"/>
-      <c r="BL11" s="67"/>
+      <c r="BH11" s="67"/>
+      <c r="BI11" s="59"/>
+      <c r="BJ11" s="59"/>
+      <c r="BK11" s="59"/>
+      <c r="BL11" s="59"/>
       <c r="BM11" s="98"/>
       <c r="BN11" s="79"/>
       <c r="BO11" s="77"/>
@@ -5875,7 +5886,7 @@
       <c r="CB11" s="77"/>
       <c r="CC11" s="78"/>
       <c r="CD11" s="56" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CE11" s="16"/>
       <c r="CF11" s="16"/>
@@ -5884,22 +5895,22 @@
       <c r="CI11" s="16"/>
       <c r="CJ11" s="16"/>
       <c r="CK11" s="48"/>
-      <c r="CL11" s="79"/>
-      <c r="CM11" s="77"/>
-      <c r="CN11" s="77"/>
-      <c r="CO11" s="77"/>
-      <c r="CP11" s="77"/>
-      <c r="CQ11" s="77"/>
-      <c r="CR11" s="77"/>
-      <c r="CS11" s="77"/>
-      <c r="CT11" s="77"/>
-      <c r="CU11" s="77"/>
-      <c r="CV11" s="77"/>
-      <c r="CW11" s="77"/>
-      <c r="CX11" s="77"/>
-      <c r="CY11" s="77"/>
-      <c r="CZ11" s="77"/>
-      <c r="DA11" s="77"/>
+      <c r="CL11" s="67"/>
+      <c r="CM11" s="59"/>
+      <c r="CN11" s="59"/>
+      <c r="CO11" s="59"/>
+      <c r="CP11" s="59"/>
+      <c r="CQ11" s="59"/>
+      <c r="CR11" s="59"/>
+      <c r="CS11" s="59"/>
+      <c r="CT11" s="59"/>
+      <c r="CU11" s="59"/>
+      <c r="CV11" s="59"/>
+      <c r="CW11" s="59"/>
+      <c r="CX11" s="59"/>
+      <c r="CY11" s="59"/>
+      <c r="CZ11" s="59"/>
+      <c r="DA11" s="98"/>
       <c r="DB11" s="148"/>
       <c r="DC11" s="149"/>
       <c r="DD11" s="159"/>
@@ -5917,7 +5928,7 @@
       <c r="DP11" s="156"/>
       <c r="DQ11" s="149"/>
       <c r="DR11" s="107" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="DS11" s="107"/>
       <c r="DT11" s="107"/>
@@ -5934,58 +5945,58 @@
       <c r="EE11" s="107"/>
       <c r="EF11" s="107"/>
       <c r="EG11" s="108"/>
-      <c r="EH11" s="67" t="s">
-        <v>226</v>
-      </c>
-      <c r="EI11" s="67"/>
-      <c r="EJ11" s="67"/>
-      <c r="EK11" s="67"/>
-      <c r="EL11" s="67"/>
-      <c r="EM11" s="67"/>
-      <c r="EN11" s="67"/>
+      <c r="EH11" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="EI11" s="59"/>
+      <c r="EJ11" s="59"/>
+      <c r="EK11" s="59"/>
+      <c r="EL11" s="59"/>
+      <c r="EM11" s="59"/>
+      <c r="EN11" s="59"/>
       <c r="EO11" s="98"/>
-      <c r="EP11" s="66"/>
-      <c r="EQ11" s="67"/>
-      <c r="ER11" s="67"/>
-      <c r="ES11" s="67"/>
-      <c r="ET11" s="67"/>
-      <c r="EU11" s="67"/>
-      <c r="EV11" s="67"/>
+      <c r="EP11" s="67"/>
+      <c r="EQ11" s="59"/>
+      <c r="ER11" s="59"/>
+      <c r="ES11" s="59"/>
+      <c r="ET11" s="59"/>
+      <c r="EU11" s="59"/>
+      <c r="EV11" s="59"/>
       <c r="EW11" s="98"/>
       <c r="EX11" s="47" t="s">
-        <v>218</v>
-      </c>
-      <c r="EY11" s="66" t="s">
         <v>216</v>
       </c>
-      <c r="EZ11" s="67"/>
-      <c r="FA11" s="67"/>
-      <c r="FB11" s="67"/>
-      <c r="FC11" s="67"/>
-      <c r="FD11" s="67"/>
+      <c r="EY11" s="67" t="s">
+        <v>214</v>
+      </c>
+      <c r="EZ11" s="59"/>
+      <c r="FA11" s="59"/>
+      <c r="FB11" s="59"/>
+      <c r="FC11" s="59"/>
+      <c r="FD11" s="59"/>
       <c r="FE11" s="98"/>
       <c r="FF11" s="138" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="FG11" s="133"/>
       <c r="FH11" s="133"/>
       <c r="FI11" s="139"/>
       <c r="FK11" s="109" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="FL11" s="109"/>
       <c r="FM11" s="110"/>
       <c r="FN11" s="134" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="FO11" s="135"/>
       <c r="FP11" s="134" t="s">
-        <v>213</v>
-      </c>
-      <c r="FQ11" s="67"/>
-      <c r="FR11" s="67"/>
-      <c r="FS11" s="67"/>
-      <c r="FT11" s="67"/>
+        <v>211</v>
+      </c>
+      <c r="FQ11" s="59"/>
+      <c r="FR11" s="59"/>
+      <c r="FS11" s="59"/>
+      <c r="FT11" s="59"/>
       <c r="FU11" s="135"/>
       <c r="FV11" s="77"/>
       <c r="FW11" s="77"/>
@@ -5999,30 +6010,30 @@
       <c r="GE11" s="77"/>
       <c r="GF11" s="77"/>
       <c r="GG11" s="78"/>
-      <c r="GH11" s="66"/>
-      <c r="GI11" s="67"/>
-      <c r="GJ11" s="67"/>
-      <c r="GK11" s="67"/>
+      <c r="GH11" s="67"/>
+      <c r="GI11" s="59"/>
+      <c r="GJ11" s="59"/>
+      <c r="GK11" s="59"/>
       <c r="GL11" s="96" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="GM11" s="96"/>
       <c r="GN11" s="96"/>
-      <c r="GT11" s="66"/>
-      <c r="GU11" s="67"/>
-      <c r="GV11" s="67"/>
-      <c r="GW11" s="67"/>
-      <c r="GX11" s="67"/>
-      <c r="GY11" s="67"/>
-      <c r="GZ11" s="67"/>
+      <c r="GT11" s="67"/>
+      <c r="GU11" s="59"/>
+      <c r="GV11" s="59"/>
+      <c r="GW11" s="59"/>
+      <c r="GX11" s="59"/>
+      <c r="GY11" s="59"/>
+      <c r="GZ11" s="59"/>
       <c r="HA11" s="98"/>
-      <c r="HB11" s="66"/>
-      <c r="HC11" s="67"/>
-      <c r="HD11" s="67"/>
-      <c r="HE11" s="67"/>
-      <c r="HF11" s="67"/>
-      <c r="HG11" s="67"/>
-      <c r="HH11" s="67"/>
+      <c r="HB11" s="67"/>
+      <c r="HC11" s="59"/>
+      <c r="HD11" s="59"/>
+      <c r="HE11" s="59"/>
+      <c r="HF11" s="59"/>
+      <c r="HG11" s="59"/>
+      <c r="HH11" s="59"/>
       <c r="HI11" s="98"/>
     </row>
     <row r="12" spans="1:217" ht="88.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6031,7 +6042,9 @@
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="F12" s="16" t="s">
+        <v>262</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="H12" s="48"/>
       <c r="I12" s="79"/>
@@ -6043,53 +6056,53 @@
       <c r="O12" s="77"/>
       <c r="P12" s="77"/>
       <c r="Q12" s="78"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="59"/>
       <c r="T12" s="98"/>
-      <c r="U12" s="66"/>
-      <c r="V12" s="67"/>
+      <c r="U12" s="67"/>
+      <c r="V12" s="59"/>
       <c r="W12" s="98"/>
-      <c r="X12" s="66"/>
-      <c r="Y12" s="67"/>
+      <c r="X12" s="67"/>
+      <c r="Y12" s="59"/>
       <c r="Z12" s="98"/>
-      <c r="AA12" s="66"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="67"/>
-      <c r="AD12" s="67"/>
-      <c r="AE12" s="67"/>
-      <c r="AF12" s="67"/>
+      <c r="AA12" s="67"/>
+      <c r="AB12" s="59"/>
+      <c r="AC12" s="59"/>
+      <c r="AD12" s="59"/>
+      <c r="AE12" s="59"/>
+      <c r="AF12" s="59"/>
       <c r="AG12" s="98"/>
-      <c r="AH12" s="66"/>
-      <c r="AI12" s="67"/>
-      <c r="AJ12" s="67"/>
-      <c r="AK12" s="67"/>
-      <c r="AL12" s="67"/>
-      <c r="AM12" s="67"/>
-      <c r="AN12" s="67"/>
-      <c r="AO12" s="67"/>
-      <c r="AP12" s="67"/>
+      <c r="AH12" s="67"/>
+      <c r="AI12" s="59"/>
+      <c r="AJ12" s="59"/>
+      <c r="AK12" s="59"/>
+      <c r="AL12" s="59"/>
+      <c r="AM12" s="59"/>
+      <c r="AN12" s="59"/>
+      <c r="AO12" s="59"/>
+      <c r="AP12" s="59"/>
       <c r="AQ12" s="98"/>
-      <c r="AR12" s="66"/>
-      <c r="AS12" s="67"/>
-      <c r="AT12" s="67"/>
-      <c r="AU12" s="67"/>
-      <c r="AV12" s="67"/>
+      <c r="AR12" s="67"/>
+      <c r="AS12" s="59"/>
+      <c r="AT12" s="59"/>
+      <c r="AU12" s="59"/>
+      <c r="AV12" s="59"/>
       <c r="AW12" s="98"/>
-      <c r="AX12" s="67"/>
-      <c r="AY12" s="67"/>
-      <c r="AZ12" s="67"/>
-      <c r="BA12" s="67"/>
-      <c r="BB12" s="67"/>
-      <c r="BC12" s="67"/>
-      <c r="BD12" s="67"/>
-      <c r="BE12" s="67"/>
-      <c r="BF12" s="67"/>
+      <c r="AX12" s="59"/>
+      <c r="AY12" s="59"/>
+      <c r="AZ12" s="59"/>
+      <c r="BA12" s="59"/>
+      <c r="BB12" s="59"/>
+      <c r="BC12" s="59"/>
+      <c r="BD12" s="59"/>
+      <c r="BE12" s="59"/>
+      <c r="BF12" s="59"/>
       <c r="BG12" s="98"/>
-      <c r="BH12" s="66"/>
-      <c r="BI12" s="67"/>
-      <c r="BJ12" s="67"/>
-      <c r="BK12" s="67"/>
-      <c r="BL12" s="67"/>
+      <c r="BH12" s="67"/>
+      <c r="BI12" s="59"/>
+      <c r="BJ12" s="59"/>
+      <c r="BK12" s="59"/>
+      <c r="BL12" s="59"/>
       <c r="BM12" s="98"/>
       <c r="BN12" s="79"/>
       <c r="BO12" s="77"/>
@@ -6108,19 +6121,20 @@
       <c r="CB12" s="77"/>
       <c r="CC12" s="78"/>
       <c r="CD12" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="CE12" s="16"/>
-      <c r="CF12" s="16"/>
-      <c r="CG12" s="16"/>
+        <v>253</v>
+      </c>
+      <c r="CE12" s="59" t="s">
+        <v>261</v>
+      </c>
+      <c r="CF12" s="59"/>
+      <c r="CG12" s="59"/>
       <c r="CI12" s="16"/>
       <c r="CJ12" s="16"/>
       <c r="CK12" s="48"/>
-      <c r="CL12" s="79"/>
-      <c r="CM12" s="77"/>
-      <c r="CN12" s="77"/>
-      <c r="CO12" s="77"/>
-      <c r="CP12" s="77"/>
+      <c r="CL12" s="17"/>
+      <c r="CP12" s="59" t="s">
+        <v>258</v>
+      </c>
       <c r="CQ12" s="77"/>
       <c r="CR12" s="77"/>
       <c r="CS12" s="77"/>
@@ -6128,10 +6142,6 @@
       <c r="CU12" s="77"/>
       <c r="CV12" s="77"/>
       <c r="CW12" s="77"/>
-      <c r="CX12" s="77"/>
-      <c r="CY12" s="77"/>
-      <c r="CZ12" s="77"/>
-      <c r="DA12" s="77"/>
       <c r="DB12" s="150"/>
       <c r="DC12" s="151"/>
       <c r="DD12" s="159"/>
@@ -6164,39 +6174,39 @@
       <c r="EE12" s="16"/>
       <c r="EF12" s="16"/>
       <c r="EG12" s="48"/>
-      <c r="EH12" s="67"/>
-      <c r="EI12" s="67"/>
-      <c r="EJ12" s="67"/>
-      <c r="EK12" s="67"/>
-      <c r="EL12" s="67"/>
-      <c r="EM12" s="67"/>
-      <c r="EN12" s="67"/>
+      <c r="EH12" s="59"/>
+      <c r="EI12" s="59"/>
+      <c r="EJ12" s="59"/>
+      <c r="EK12" s="59"/>
+      <c r="EL12" s="59"/>
+      <c r="EM12" s="59"/>
+      <c r="EN12" s="59"/>
       <c r="EO12" s="98"/>
-      <c r="EP12" s="66"/>
-      <c r="EQ12" s="67"/>
-      <c r="ER12" s="67"/>
-      <c r="ES12" s="67"/>
-      <c r="ET12" s="67"/>
-      <c r="EU12" s="67"/>
-      <c r="EV12" s="67"/>
+      <c r="EP12" s="67"/>
+      <c r="EQ12" s="59"/>
+      <c r="ER12" s="59"/>
+      <c r="ES12" s="59"/>
+      <c r="ET12" s="59"/>
+      <c r="EU12" s="59"/>
+      <c r="EV12" s="59"/>
       <c r="EW12" s="98"/>
       <c r="EX12" s="111" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="EY12" s="17"/>
       <c r="FE12" s="18"/>
       <c r="FK12" s="132" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="FL12" s="132"/>
       <c r="FM12" s="132"/>
       <c r="FN12" s="134"/>
       <c r="FO12" s="135"/>
       <c r="FP12" s="134"/>
-      <c r="FQ12" s="67"/>
-      <c r="FR12" s="67"/>
-      <c r="FS12" s="67"/>
-      <c r="FT12" s="67"/>
+      <c r="FQ12" s="59"/>
+      <c r="FR12" s="59"/>
+      <c r="FS12" s="59"/>
+      <c r="FT12" s="59"/>
       <c r="FU12" s="135"/>
       <c r="FV12" s="77"/>
       <c r="FW12" s="77"/>
@@ -6210,40 +6220,40 @@
       <c r="GE12" s="77"/>
       <c r="GF12" s="77"/>
       <c r="GG12" s="78"/>
-      <c r="GH12" s="66"/>
-      <c r="GI12" s="67"/>
-      <c r="GJ12" s="67"/>
-      <c r="GK12" s="67"/>
+      <c r="GH12" s="67"/>
+      <c r="GI12" s="59"/>
+      <c r="GJ12" s="59"/>
+      <c r="GK12" s="59"/>
       <c r="GL12" t="s">
-        <v>202</v>
-      </c>
-      <c r="GT12" s="66"/>
-      <c r="GU12" s="67"/>
-      <c r="GV12" s="67"/>
-      <c r="GW12" s="67"/>
-      <c r="GX12" s="67"/>
-      <c r="GY12" s="67"/>
-      <c r="GZ12" s="67"/>
+        <v>200</v>
+      </c>
+      <c r="GT12" s="67"/>
+      <c r="GU12" s="59"/>
+      <c r="GV12" s="59"/>
+      <c r="GW12" s="59"/>
+      <c r="GX12" s="59"/>
+      <c r="GY12" s="59"/>
+      <c r="GZ12" s="59"/>
       <c r="HA12" s="98"/>
-      <c r="HB12" s="66"/>
-      <c r="HC12" s="67"/>
-      <c r="HD12" s="67"/>
-      <c r="HE12" s="67"/>
-      <c r="HF12" s="67"/>
-      <c r="HG12" s="67"/>
-      <c r="HH12" s="67"/>
+      <c r="HB12" s="67"/>
+      <c r="HC12" s="59"/>
+      <c r="HD12" s="59"/>
+      <c r="HE12" s="59"/>
+      <c r="HF12" s="59"/>
+      <c r="HG12" s="59"/>
+      <c r="HH12" s="59"/>
       <c r="HI12" s="98"/>
     </row>
     <row r="13" spans="1:217" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="131" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C13" s="131" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>239</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -6258,53 +6268,53 @@
       <c r="O13" s="77"/>
       <c r="P13" s="77"/>
       <c r="Q13" s="78"/>
-      <c r="R13" s="66"/>
-      <c r="S13" s="67"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="59"/>
       <c r="T13" s="98"/>
-      <c r="U13" s="66"/>
-      <c r="V13" s="67"/>
+      <c r="U13" s="67"/>
+      <c r="V13" s="59"/>
       <c r="W13" s="98"/>
-      <c r="X13" s="66"/>
-      <c r="Y13" s="67"/>
+      <c r="X13" s="67"/>
+      <c r="Y13" s="59"/>
       <c r="Z13" s="98"/>
-      <c r="AA13" s="66"/>
-      <c r="AB13" s="67"/>
-      <c r="AC13" s="67"/>
-      <c r="AD13" s="67"/>
-      <c r="AE13" s="67"/>
-      <c r="AF13" s="67"/>
+      <c r="AA13" s="67"/>
+      <c r="AB13" s="59"/>
+      <c r="AC13" s="59"/>
+      <c r="AD13" s="59"/>
+      <c r="AE13" s="59"/>
+      <c r="AF13" s="59"/>
       <c r="AG13" s="98"/>
-      <c r="AH13" s="66"/>
-      <c r="AI13" s="67"/>
-      <c r="AJ13" s="67"/>
-      <c r="AK13" s="67"/>
-      <c r="AL13" s="67"/>
-      <c r="AM13" s="67"/>
-      <c r="AN13" s="67"/>
-      <c r="AO13" s="67"/>
-      <c r="AP13" s="67"/>
+      <c r="AH13" s="67"/>
+      <c r="AI13" s="59"/>
+      <c r="AJ13" s="59"/>
+      <c r="AK13" s="59"/>
+      <c r="AL13" s="59"/>
+      <c r="AM13" s="59"/>
+      <c r="AN13" s="59"/>
+      <c r="AO13" s="59"/>
+      <c r="AP13" s="59"/>
       <c r="AQ13" s="98"/>
-      <c r="AR13" s="66"/>
-      <c r="AS13" s="67"/>
-      <c r="AT13" s="67"/>
-      <c r="AU13" s="67"/>
-      <c r="AV13" s="67"/>
+      <c r="AR13" s="67"/>
+      <c r="AS13" s="59"/>
+      <c r="AT13" s="59"/>
+      <c r="AU13" s="59"/>
+      <c r="AV13" s="59"/>
       <c r="AW13" s="98"/>
-      <c r="AX13" s="67"/>
-      <c r="AY13" s="67"/>
-      <c r="AZ13" s="67"/>
-      <c r="BA13" s="67"/>
-      <c r="BB13" s="67"/>
-      <c r="BC13" s="67"/>
-      <c r="BD13" s="67"/>
-      <c r="BE13" s="67"/>
-      <c r="BF13" s="67"/>
+      <c r="AX13" s="59"/>
+      <c r="AY13" s="59"/>
+      <c r="AZ13" s="59"/>
+      <c r="BA13" s="59"/>
+      <c r="BB13" s="59"/>
+      <c r="BC13" s="59"/>
+      <c r="BD13" s="59"/>
+      <c r="BE13" s="59"/>
+      <c r="BF13" s="59"/>
       <c r="BG13" s="98"/>
-      <c r="BH13" s="66"/>
-      <c r="BI13" s="67"/>
-      <c r="BJ13" s="67"/>
-      <c r="BK13" s="67"/>
-      <c r="BL13" s="67"/>
+      <c r="BH13" s="67"/>
+      <c r="BI13" s="59"/>
+      <c r="BJ13" s="59"/>
+      <c r="BK13" s="59"/>
+      <c r="BL13" s="59"/>
       <c r="BM13" s="98"/>
       <c r="BN13" s="79"/>
       <c r="BO13" s="77"/>
@@ -6323,7 +6333,7 @@
       <c r="CB13" s="77"/>
       <c r="CC13" s="78"/>
       <c r="CD13" s="47" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="CE13" s="16"/>
       <c r="CF13" s="16"/>
@@ -6332,10 +6342,7 @@
       <c r="CI13" s="16"/>
       <c r="CJ13" s="16"/>
       <c r="CK13" s="48"/>
-      <c r="CL13" s="79"/>
-      <c r="CM13" s="77"/>
-      <c r="CN13" s="77"/>
-      <c r="CO13" s="77"/>
+      <c r="CL13" s="17"/>
       <c r="CP13" s="77"/>
       <c r="CQ13" s="77"/>
       <c r="CR13" s="77"/>
@@ -6344,30 +6351,26 @@
       <c r="CU13" s="77"/>
       <c r="CV13" s="77"/>
       <c r="CW13" s="77"/>
-      <c r="CX13" s="77"/>
-      <c r="CY13" s="77"/>
-      <c r="CZ13" s="77"/>
-      <c r="DA13" s="77"/>
       <c r="DB13" s="134" t="s">
-        <v>200</v>
-      </c>
-      <c r="DC13" s="67"/>
-      <c r="DD13" s="67"/>
-      <c r="DE13" s="67"/>
-      <c r="DF13" s="67"/>
-      <c r="DG13" s="67"/>
-      <c r="DH13" s="67"/>
-      <c r="DI13" s="67"/>
-      <c r="DJ13" s="67"/>
-      <c r="DK13" s="67"/>
-      <c r="DL13" s="67"/>
-      <c r="DM13" s="67"/>
-      <c r="DN13" s="67"/>
-      <c r="DO13" s="67"/>
-      <c r="DP13" s="67"/>
+        <v>198</v>
+      </c>
+      <c r="DC13" s="59"/>
+      <c r="DD13" s="59"/>
+      <c r="DE13" s="59"/>
+      <c r="DF13" s="59"/>
+      <c r="DG13" s="59"/>
+      <c r="DH13" s="59"/>
+      <c r="DI13" s="59"/>
+      <c r="DJ13" s="59"/>
+      <c r="DK13" s="59"/>
+      <c r="DL13" s="59"/>
+      <c r="DM13" s="59"/>
+      <c r="DN13" s="59"/>
+      <c r="DO13" s="59"/>
+      <c r="DP13" s="59"/>
       <c r="DQ13" s="135"/>
       <c r="DR13" s="131" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="DS13" s="131"/>
       <c r="DT13" s="131"/>
@@ -6384,39 +6387,39 @@
       <c r="EE13" s="16"/>
       <c r="EF13" s="16"/>
       <c r="EG13" s="48"/>
-      <c r="EH13" s="67"/>
-      <c r="EI13" s="67"/>
-      <c r="EJ13" s="67"/>
-      <c r="EK13" s="67"/>
-      <c r="EL13" s="67"/>
-      <c r="EM13" s="67"/>
-      <c r="EN13" s="67"/>
+      <c r="EH13" s="59"/>
+      <c r="EI13" s="59"/>
+      <c r="EJ13" s="59"/>
+      <c r="EK13" s="59"/>
+      <c r="EL13" s="59"/>
+      <c r="EM13" s="59"/>
+      <c r="EN13" s="59"/>
       <c r="EO13" s="98"/>
-      <c r="EP13" s="66"/>
-      <c r="EQ13" s="67"/>
-      <c r="ER13" s="67"/>
-      <c r="ES13" s="67"/>
-      <c r="ET13" s="67"/>
-      <c r="EU13" s="67"/>
-      <c r="EV13" s="67"/>
+      <c r="EP13" s="67"/>
+      <c r="EQ13" s="59"/>
+      <c r="ER13" s="59"/>
+      <c r="ES13" s="59"/>
+      <c r="ET13" s="59"/>
+      <c r="EU13" s="59"/>
+      <c r="EV13" s="59"/>
       <c r="EW13" s="98"/>
       <c r="EX13" s="111"/>
       <c r="EY13" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="FE13" s="18"/>
       <c r="FK13" s="109" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="FL13" s="109"/>
       <c r="FM13" s="110"/>
       <c r="FN13" s="134"/>
       <c r="FO13" s="135"/>
       <c r="FP13" s="134"/>
-      <c r="FQ13" s="67"/>
-      <c r="FR13" s="67"/>
-      <c r="FS13" s="67"/>
-      <c r="FT13" s="67"/>
+      <c r="FQ13" s="59"/>
+      <c r="FR13" s="59"/>
+      <c r="FS13" s="59"/>
+      <c r="FT13" s="59"/>
       <c r="FU13" s="135"/>
       <c r="FV13" s="77"/>
       <c r="FW13" s="77"/>
@@ -6430,28 +6433,28 @@
       <c r="GE13" s="77"/>
       <c r="GF13" s="77"/>
       <c r="GG13" s="78"/>
-      <c r="GH13" s="66"/>
-      <c r="GI13" s="67"/>
-      <c r="GJ13" s="67"/>
-      <c r="GK13" s="67"/>
+      <c r="GH13" s="67"/>
+      <c r="GI13" s="59"/>
+      <c r="GJ13" s="59"/>
+      <c r="GK13" s="59"/>
       <c r="GN13" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="GT13" s="66"/>
-      <c r="GU13" s="67"/>
-      <c r="GV13" s="67"/>
-      <c r="GW13" s="67"/>
-      <c r="GX13" s="67"/>
-      <c r="GY13" s="67"/>
-      <c r="GZ13" s="67"/>
+        <v>228</v>
+      </c>
+      <c r="GT13" s="67"/>
+      <c r="GU13" s="59"/>
+      <c r="GV13" s="59"/>
+      <c r="GW13" s="59"/>
+      <c r="GX13" s="59"/>
+      <c r="GY13" s="59"/>
+      <c r="GZ13" s="59"/>
       <c r="HA13" s="98"/>
-      <c r="HB13" s="66"/>
-      <c r="HC13" s="67"/>
-      <c r="HD13" s="67"/>
-      <c r="HE13" s="67"/>
-      <c r="HF13" s="67"/>
-      <c r="HG13" s="67"/>
-      <c r="HH13" s="67"/>
+      <c r="HB13" s="67"/>
+      <c r="HC13" s="59"/>
+      <c r="HD13" s="59"/>
+      <c r="HE13" s="59"/>
+      <c r="HF13" s="59"/>
+      <c r="HG13" s="59"/>
+      <c r="HH13" s="59"/>
       <c r="HI13" s="98"/>
     </row>
     <row r="14" spans="1:217" ht="77.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6537,7 +6540,7 @@
       <c r="CB14" s="81"/>
       <c r="CC14" s="82"/>
       <c r="CD14" s="47" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="CE14" s="20"/>
       <c r="CF14" s="20"/>
@@ -6546,10 +6549,10 @@
       <c r="CI14" s="49"/>
       <c r="CJ14" s="49"/>
       <c r="CK14" s="50"/>
-      <c r="CL14" s="80"/>
-      <c r="CM14" s="81"/>
-      <c r="CN14" s="81"/>
-      <c r="CO14" s="81"/>
+      <c r="CL14" s="19"/>
+      <c r="CM14" s="20"/>
+      <c r="CN14" s="20"/>
+      <c r="CO14" s="20"/>
       <c r="CP14" s="81"/>
       <c r="CQ14" s="81"/>
       <c r="CR14" s="81"/>
@@ -6558,10 +6561,10 @@
       <c r="CU14" s="81"/>
       <c r="CV14" s="81"/>
       <c r="CW14" s="81"/>
-      <c r="CX14" s="81"/>
-      <c r="CY14" s="81"/>
-      <c r="CZ14" s="81"/>
-      <c r="DA14" s="81"/>
+      <c r="CX14" s="20"/>
+      <c r="CY14" s="20"/>
+      <c r="CZ14" s="20"/>
+      <c r="DA14" s="20"/>
       <c r="DB14" s="136"/>
       <c r="DC14" s="69"/>
       <c r="DD14" s="69"/>
@@ -6579,7 +6582,7 @@
       <c r="DP14" s="69"/>
       <c r="DQ14" s="137"/>
       <c r="DR14" s="131" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="DS14" s="131"/>
       <c r="DT14" s="131"/>
@@ -6615,7 +6618,7 @@
       <c r="FD14" s="20"/>
       <c r="FE14" s="21"/>
       <c r="FK14" s="141" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="FL14" s="141"/>
       <c r="FM14" s="142"/>
@@ -6644,7 +6647,7 @@
       <c r="GJ14" s="69"/>
       <c r="GK14" s="69"/>
       <c r="GM14" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="GT14" s="99"/>
       <c r="GU14" s="100"/>
@@ -6757,7 +6760,7 @@
       <c r="CJ16" s="130"/>
       <c r="CK16" s="130"/>
       <c r="DE16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="DS16" t="s">
         <v>120</v>
@@ -6850,7 +6853,7 @@
       <c r="CN18" s="28"/>
       <c r="CO18" s="29"/>
       <c r="DE18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="EC18" t="s">
         <v>126</v>
@@ -6892,7 +6895,7 @@
         <v>153</v>
       </c>
       <c r="DE19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="EC19" t="s">
         <v>127</v>
@@ -7589,7 +7592,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="172">
+  <mergeCells count="174">
     <mergeCell ref="B9:H11"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
@@ -7613,6 +7616,7 @@
     <mergeCell ref="CE9:CG9"/>
     <mergeCell ref="CH9:CK9"/>
     <mergeCell ref="CE10:CG10"/>
+    <mergeCell ref="CL9:DA11"/>
     <mergeCell ref="CD16:CK29"/>
     <mergeCell ref="GT9:HA14"/>
     <mergeCell ref="EH11:EO13"/>
@@ -7636,7 +7640,7 @@
     <mergeCell ref="FK11:FM11"/>
     <mergeCell ref="FK10:FM10"/>
     <mergeCell ref="FK14:FM14"/>
-    <mergeCell ref="CL9:DA14"/>
+    <mergeCell ref="CP12:CW14"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="R2:Y2"/>
@@ -7752,6 +7756,7 @@
     <mergeCell ref="EX12:EX14"/>
     <mergeCell ref="GM9:GM10"/>
     <mergeCell ref="GN9:GN10"/>
+    <mergeCell ref="CE12:CG12"/>
     <mergeCell ref="GL7:GN7"/>
     <mergeCell ref="DR8:EG8"/>
     <mergeCell ref="GL4:GS4"/>
@@ -7783,7 +7788,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="161">
         <v>0</v>
@@ -8101,7 +8106,7 @@
     </row>
     <row r="5" spans="1:33" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B5" s="34">
         <f t="shared" ref="B5:H5" si="1">B2-8</f>
@@ -8229,37 +8234,37 @@
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D6" s="70" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E6" s="116"/>
       <c r="F6" s="116"/>
       <c r="G6" s="71"/>
       <c r="H6" s="54" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I6" s="58" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J6" s="164" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K6" s="165"/>
       <c r="L6" s="165"/>
       <c r="M6" s="166"/>
       <c r="N6" s="164" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="O6" s="165"/>
       <c r="P6" s="165"/>
       <c r="Q6" s="166"/>
       <c r="R6" s="164" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="S6" s="165"/>
       <c r="T6" s="165"/>
@@ -8271,7 +8276,7 @@
       <c r="Z6" s="165"/>
       <c r="AA6" s="166"/>
       <c r="AB6" s="164" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AC6" s="165"/>
       <c r="AD6" s="165"/>
@@ -8281,40 +8286,40 @@
     </row>
     <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" s="167" t="s">
         <v>186</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" s="167" t="s">
-        <v>188</v>
       </c>
       <c r="E7" s="167"/>
       <c r="F7" s="167"/>
       <c r="G7" s="167"/>
       <c r="H7" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J7" s="167" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K7" s="167"/>
       <c r="L7" s="167"/>
       <c r="M7" s="167"/>
       <c r="N7" s="167" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="O7" s="167"/>
       <c r="P7" s="167"/>
       <c r="Q7" s="167"/>
       <c r="R7" s="167" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="S7" s="167"/>
       <c r="T7" s="167"/>
@@ -8326,7 +8331,7 @@
       <c r="Z7" s="167"/>
       <c r="AA7" s="167"/>
       <c r="AB7" s="167" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AC7" s="167"/>
       <c r="AD7" s="167"/>
@@ -8337,7 +8342,7 @@
     <row r="8" spans="1:33" ht="114" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="I8" s="16" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected details on loot, some other flags and playerdat details updated.
</commit_message>
<xml_diff>
--- a/File Research/Game Object Research File.xlsx
+++ b/File Research/Game Object Research File.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3C0E8B-BAED-4DBF-B015-DB8A8EA7864A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3CDBF4-5DD5-4AA1-A512-869E570645CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
   </bookViews>
@@ -790,7 +790,121 @@
     <t>set to 1 after conversation</t>
   </si>
   <si>
-    <t>When standing still with an attitude of 0 an attempt will be made to detect the player. If found set bit 0 and set attack goals
+    <t>TargetTileX</t>
+  </si>
+  <si>
+    <t>Bit 7 is set for lady tori, mors and some guards in the castle and is 
+checked when they die</t>
+  </si>
+  <si>
+    <t>Bit set when creating pit fighter
+Later checked for skipping when spawning npcs.
+References with createobject traps</t>
+  </si>
+  <si>
+    <t>Relevant to projectile motion</t>
+  </si>
+  <si>
+    <t>In a homing dart/satellite if bit 7 is set projectile hp is set to 0. (hp in this case is ticking down slowly)</t>
+  </si>
+  <si>
+    <t>Bit 7 gets set in a babl_hack</t>
+  </si>
+  <si>
+    <t>If unset set_race_attitude does not apply to the NPC
+In anger npc if owner is 32d then owner is only angered if bit 7 set</t>
+  </si>
+  <si>
+    <t>Referenced in npcgoto
+Value used as a lookup
+into a table in Seg57,
+Record size 0x1Ch (28d) Pathfinding Table???
+relationship to bit 7 in 0x15h</t>
+  </si>
+  <si>
+    <t>if set ignore code been ran on similar npcs. Probably an isSpecial Flag for NPCs?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gtarg is the npc being targeted by this npc. Usually it is one for the avatar
+When petrified the value is the timer for how long petrification lasts
+</t>
+  </si>
+  <si>
+    <t>Generally the health of an object or a general use parameter for a trap
+For NPCS tileX  (or xhome)</t>
+  </si>
+  <si>
+    <t>Race number of the owner of the object or a general parameter of the object
+For Npcs tileY (or yhome)</t>
+  </si>
+  <si>
+    <t>Value affects Hp returned by study monster</t>
+  </si>
+  <si>
+    <t>Bit relevant to magic effects</t>
+  </si>
+  <si>
+    <t>Facing direction of the object
+For magical objectsthe value(s) to show it has been identified (0=unidentified, 1=know it is magical, 2=fully identified)
+Bit 3 controls is an attempt has been made to identify the object (gets cleared when the lore skill is leveled up)</t>
+  </si>
+  <si>
+    <t>Changed in transform_talker</t>
+  </si>
+  <si>
+    <t>bit 7 is unset when a projectile is launched, it gets set to 1 when it hits an NPC
+bit 7 might mean the npc is in combat?
+For npcs this value is relevant in Study monstor. When whoamis is 64h(krillner?) this value is used
+When the avatar is killed the bit 7 is used to check if the avatar has to go to jail in the castle
+bit 7 checked in set_Race_attitude
+bit 7 is checked in special death cases relating to lady tory
+DOES IT MEAN OBJECT IS AN NPC???? not sure since bit 7 is unset after a missile hits it target
+possibly a tileY reference used closely with projectilesourceID value</t>
+  </si>
+  <si>
+    <t>Bit 7 is unset when projectile is launched
+Also unset when a satellite hits it source</t>
+  </si>
+  <si>
+    <t>Texture is used for signs, tmaps, bridges, where there is a variation in how it will be displayed.
+Eg values&gt;2 for bridges give a index into the texture map
+The flag controls the type of writing a wall plaque has</t>
+  </si>
+  <si>
+    <t>Tracks value of rotary switches</t>
+  </si>
+  <si>
+    <t>NPC Talked To Value</t>
+  </si>
+  <si>
+    <t>doordir/TalkedTo</t>
+  </si>
+  <si>
+    <t>Used for some special objects: Academy wand, Mors Spellbook, signet rings used to mark places of power that have yet to be cleansed</t>
+  </si>
+  <si>
+    <t>In damage objects this controls if a container is immune to damage to bash it open</t>
+  </si>
+  <si>
+    <t>Object is protected from culling. Cannot be destroyed when thrown into water.</t>
+  </si>
+  <si>
+    <t>Looked at when object hits the ground. When value is 1 the object is removed on impact and a splash occurs</t>
+  </si>
+  <si>
+    <t>Bits 6 &amp; 7 set when NPC based on npc active state
+Bit 6 might have something to do with the need to move to a location
+If Bit 7 is set then the unk value in 0x16 is used for an unknown reason
+Bit 7 is set when in a walking animation</t>
+  </si>
+  <si>
+    <t>Set to 1 for open doors (so animation for closing moves in correct direction)</t>
+  </si>
+  <si>
+    <t>Tracks motion of  the closing or opening door animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When standing still with an attitude of 0 an attempt will be made to detect the player. If found set bit 0 and set attack goals
 Bit 0 indicates that the npc is aware of the avatar's position, use in combat to chase the avatar
 Bit 1 is somehow connect to bit 0 behaviours, maybe used to indicate npc should turn towards target
 Bits 2 &amp; 3 when &lt;&gt; 0 the npc will execute a magic attack when it's animation is a ranged attack, value is alookup into critter data at 0x2Ah (bytes 2Ah to 2Ch) to get spell effect id to use. Value of lookup is based on RNG call in NpcStartMagicAttack()
@@ -801,121 +915,9 @@
 Bits 6 and 7 randomly set in a subfunction of player updates()!!!
 Bit 6 and 7 stop npcs from hurting each other in combat when they are the same? 
 Bit 6 checked after the avatar hits an npc
-Possibly a series of bit fields representing combat and AI decisions</t>
-  </si>
-  <si>
-    <t>TargetTileX</t>
-  </si>
-  <si>
-    <t>Bit 7 is set for lady tori, mors and some guards in the castle and is 
-checked when they die</t>
-  </si>
-  <si>
-    <t>Bit set when creating pit fighter
-Later checked for skipping when spawning npcs.
-References with createobject traps</t>
-  </si>
-  <si>
-    <t>Relevant to projectile motion</t>
-  </si>
-  <si>
-    <t>In a homing dart/satellite if bit 7 is set projectile hp is set to 0. (hp in this case is ticking down slowly)</t>
-  </si>
-  <si>
-    <t>Bit 7 gets set in a babl_hack</t>
-  </si>
-  <si>
-    <t>If unset set_race_attitude does not apply to the NPC
-In anger npc if owner is 32d then owner is only angered if bit 7 set</t>
-  </si>
-  <si>
-    <t>Referenced in npcgoto
-Value used as a lookup
-into a table in Seg57,
-Record size 0x1Ch (28d) Pathfinding Table???
-relationship to bit 7 in 0x15h</t>
-  </si>
-  <si>
-    <t>if set ignore code been ran on similar npcs. Probably an isSpecial Flag for NPCs?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gtarg is the npc being targeted by this npc. Usually it is one for the avatar
-When petrified the value is the timer for how long petrification lasts
-</t>
-  </si>
-  <si>
-    <t>Generally the health of an object or a general use parameter for a trap
-For NPCS tileX  (or xhome)</t>
-  </si>
-  <si>
-    <t>Race number of the owner of the object or a general parameter of the object
-For Npcs tileY (or yhome)</t>
-  </si>
-  <si>
-    <t>Value affects Hp returned by study monster</t>
-  </si>
-  <si>
-    <t>Bit relevant to magic effects</t>
-  </si>
-  <si>
-    <t>Facing direction of the object
-For magical objectsthe value(s) to show it has been identified (0=unidentified, 1=know it is magical, 2=fully identified)
-Bit 3 controls is an attempt has been made to identify the object (gets cleared when the lore skill is leveled up)</t>
-  </si>
-  <si>
-    <t>Changed in transform_talker</t>
-  </si>
-  <si>
-    <t>bit 7 is unset when a projectile is launched, it gets set to 1 when it hits an NPC
-bit 7 might mean the npc is in combat?
-For npcs this value is relevant in Study monstor. When whoamis is 64h(krillner?) this value is used
-When the avatar is killed the bit 7 is used to check if the avatar has to go to jail in the castle
-bit 7 checked in set_Race_attitude
-bit 7 is checked in special death cases relating to lady tory
-DOES IT MEAN OBJECT IS AN NPC???? not sure since bit 7 is unset after a missile hits it target
-possibly a tileY reference used closely with projectilesourceID value</t>
-  </si>
-  <si>
-    <t>Bit 7 is unset when projectile is launched
-Also unset when a satellite hits it source</t>
-  </si>
-  <si>
-    <t>Texture is used for signs, tmaps, bridges, where there is a variation in how it will be displayed.
-Eg values&gt;2 for bridges give a index into the texture map
-The flag controls the type of writing a wall plaque has</t>
-  </si>
-  <si>
-    <t>Tracks value of rotary switches</t>
-  </si>
-  <si>
-    <t>NPC Talked To Value</t>
-  </si>
-  <si>
-    <t>doordir/TalkedTo</t>
-  </si>
-  <si>
-    <t>Used for some special objects: Academy wand, Mors Spellbook, signet rings used to mark places of power that have yet to be cleansed</t>
-  </si>
-  <si>
-    <t>In damage objects this controls if a container is immune to damage to bash it open</t>
-  </si>
-  <si>
-    <t>Object is protected from culling. Cannot be destroyed when thrown into water.</t>
-  </si>
-  <si>
-    <t>Looked at when object hits the ground. When value is 1 the object is removed on impact and a splash occurs</t>
-  </si>
-  <si>
-    <t>Bits 6 &amp; 7 set when NPC based on npc active state
-Bit 6 might have something to do with the need to move to a location
-If Bit 7 is set then the unk value in 0x16 is used for an unknown reason
-Bit 7 is set when in a walking animation</t>
-  </si>
-  <si>
-    <t>Set to 1 for open doors (so animation for closing moves in correct direction)</t>
-  </si>
-  <si>
-    <t>Tracks motion of  the closing or opening door animation</t>
+Possibly a series of bit fields representing combat and AI decisions
+Bit 6 used in conversations. when set  it will import 6 as the value of npc_attitude (when goal&lt;&gt;5 and gtart&lt;&gt;1)
+Bit 7 is used in conversations. when used as a imported it will either import 16 (when bit is set) or 192(when bit is 0) into the conversation </t>
   </si>
 </sst>
 </file>
@@ -1731,6 +1733,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1795,9 +1800,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2279,10 +2281,10 @@
   <dimension ref="A1:HI48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B12" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="GN13" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="GV17" sqref="GV17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4983,147 +4985,147 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="115"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="110" t="s">
+      <c r="G7" s="116"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="110"/>
-      <c r="R7" s="107" t="s">
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="111"/>
+      <c r="N7" s="111"/>
+      <c r="O7" s="111"/>
+      <c r="P7" s="111"/>
+      <c r="Q7" s="111"/>
+      <c r="R7" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="108"/>
-      <c r="T7" s="109"/>
-      <c r="U7" s="107" t="s">
+      <c r="S7" s="109"/>
+      <c r="T7" s="110"/>
+      <c r="U7" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="V7" s="108"/>
-      <c r="W7" s="109"/>
+      <c r="V7" s="109"/>
+      <c r="W7" s="110"/>
       <c r="X7" s="136" t="s">
         <v>14</v>
       </c>
       <c r="Y7" s="137"/>
       <c r="Z7" s="138"/>
-      <c r="AA7" s="107" t="s">
+      <c r="AA7" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="AB7" s="108"/>
-      <c r="AC7" s="108"/>
-      <c r="AD7" s="108"/>
-      <c r="AE7" s="108"/>
-      <c r="AF7" s="108"/>
-      <c r="AG7" s="109"/>
-      <c r="AH7" s="107" t="s">
+      <c r="AB7" s="109"/>
+      <c r="AC7" s="109"/>
+      <c r="AD7" s="109"/>
+      <c r="AE7" s="109"/>
+      <c r="AF7" s="109"/>
+      <c r="AG7" s="110"/>
+      <c r="AH7" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="AI7" s="108"/>
-      <c r="AJ7" s="108"/>
-      <c r="AK7" s="108"/>
-      <c r="AL7" s="108"/>
-      <c r="AM7" s="108"/>
-      <c r="AN7" s="108"/>
-      <c r="AO7" s="108"/>
-      <c r="AP7" s="108"/>
-      <c r="AQ7" s="109"/>
-      <c r="AR7" s="107" t="s">
+      <c r="AI7" s="109"/>
+      <c r="AJ7" s="109"/>
+      <c r="AK7" s="109"/>
+      <c r="AL7" s="109"/>
+      <c r="AM7" s="109"/>
+      <c r="AN7" s="109"/>
+      <c r="AO7" s="109"/>
+      <c r="AP7" s="109"/>
+      <c r="AQ7" s="110"/>
+      <c r="AR7" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="AS7" s="108"/>
-      <c r="AT7" s="108"/>
-      <c r="AU7" s="108"/>
-      <c r="AV7" s="108"/>
-      <c r="AW7" s="109"/>
-      <c r="AX7" s="107" t="s">
+      <c r="AS7" s="109"/>
+      <c r="AT7" s="109"/>
+      <c r="AU7" s="109"/>
+      <c r="AV7" s="109"/>
+      <c r="AW7" s="110"/>
+      <c r="AX7" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="AY7" s="108"/>
-      <c r="AZ7" s="108"/>
-      <c r="BA7" s="108"/>
-      <c r="BB7" s="108"/>
-      <c r="BC7" s="108"/>
-      <c r="BD7" s="108"/>
-      <c r="BE7" s="108"/>
-      <c r="BF7" s="108"/>
-      <c r="BG7" s="109"/>
-      <c r="BH7" s="107" t="s">
+      <c r="AY7" s="109"/>
+      <c r="AZ7" s="109"/>
+      <c r="BA7" s="109"/>
+      <c r="BB7" s="109"/>
+      <c r="BC7" s="109"/>
+      <c r="BD7" s="109"/>
+      <c r="BE7" s="109"/>
+      <c r="BF7" s="109"/>
+      <c r="BG7" s="110"/>
+      <c r="BH7" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="BI7" s="108"/>
-      <c r="BJ7" s="108"/>
-      <c r="BK7" s="108"/>
-      <c r="BL7" s="108"/>
-      <c r="BM7" s="109"/>
-      <c r="BN7" s="107" t="s">
+      <c r="BI7" s="109"/>
+      <c r="BJ7" s="109"/>
+      <c r="BK7" s="109"/>
+      <c r="BL7" s="109"/>
+      <c r="BM7" s="110"/>
+      <c r="BN7" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="BO7" s="108"/>
-      <c r="BP7" s="108"/>
-      <c r="BQ7" s="108"/>
-      <c r="BR7" s="108"/>
-      <c r="BS7" s="108"/>
-      <c r="BT7" s="108"/>
-      <c r="BU7" s="109"/>
-      <c r="BV7" s="107" t="s">
+      <c r="BO7" s="109"/>
+      <c r="BP7" s="109"/>
+      <c r="BQ7" s="109"/>
+      <c r="BR7" s="109"/>
+      <c r="BS7" s="109"/>
+      <c r="BT7" s="109"/>
+      <c r="BU7" s="110"/>
+      <c r="BV7" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="BW7" s="108"/>
-      <c r="BX7" s="108"/>
-      <c r="BY7" s="108"/>
-      <c r="BZ7" s="108"/>
-      <c r="CA7" s="108"/>
-      <c r="CB7" s="108"/>
-      <c r="CC7" s="109"/>
-      <c r="CD7" s="105" t="s">
+      <c r="BW7" s="109"/>
+      <c r="BX7" s="109"/>
+      <c r="BY7" s="109"/>
+      <c r="BZ7" s="109"/>
+      <c r="CA7" s="109"/>
+      <c r="CB7" s="109"/>
+      <c r="CC7" s="110"/>
+      <c r="CD7" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="CE7" s="99"/>
-      <c r="CF7" s="99"/>
-      <c r="CG7" s="99"/>
-      <c r="CH7" s="99"/>
-      <c r="CI7" s="99"/>
-      <c r="CJ7" s="99"/>
-      <c r="CK7" s="106"/>
-      <c r="CL7" s="107" t="s">
+      <c r="CE7" s="100"/>
+      <c r="CF7" s="100"/>
+      <c r="CG7" s="100"/>
+      <c r="CH7" s="100"/>
+      <c r="CI7" s="100"/>
+      <c r="CJ7" s="100"/>
+      <c r="CK7" s="107"/>
+      <c r="CL7" s="108" t="s">
         <v>193</v>
       </c>
-      <c r="CM7" s="108"/>
-      <c r="CN7" s="108"/>
-      <c r="CO7" s="109"/>
-      <c r="CP7" s="111" t="s">
+      <c r="CM7" s="109"/>
+      <c r="CN7" s="109"/>
+      <c r="CO7" s="110"/>
+      <c r="CP7" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="CQ7" s="112"/>
-      <c r="CR7" s="112"/>
-      <c r="CS7" s="112"/>
-      <c r="CT7" s="112"/>
-      <c r="CU7" s="112"/>
-      <c r="CV7" s="112"/>
-      <c r="CW7" s="113"/>
-      <c r="CX7" s="107" t="s">
+      <c r="CQ7" s="113"/>
+      <c r="CR7" s="113"/>
+      <c r="CS7" s="113"/>
+      <c r="CT7" s="113"/>
+      <c r="CU7" s="113"/>
+      <c r="CV7" s="113"/>
+      <c r="CW7" s="114"/>
+      <c r="CX7" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="CY7" s="108"/>
-      <c r="CZ7" s="108"/>
-      <c r="DA7" s="109"/>
-      <c r="DB7" s="107" t="s">
+      <c r="CY7" s="109"/>
+      <c r="CZ7" s="109"/>
+      <c r="DA7" s="110"/>
+      <c r="DB7" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="DC7" s="109"/>
+      <c r="DC7" s="110"/>
       <c r="DD7" s="6" t="s">
         <v>28</v>
       </c>
@@ -5140,12 +5142,12 @@
       <c r="DK7" s="28"/>
       <c r="DL7" s="28"/>
       <c r="DM7" s="29"/>
-      <c r="DN7" s="114" t="s">
+      <c r="DN7" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="DO7" s="115"/>
-      <c r="DP7" s="115"/>
-      <c r="DQ7" s="116"/>
+      <c r="DO7" s="116"/>
+      <c r="DP7" s="116"/>
+      <c r="DQ7" s="117"/>
       <c r="DR7" s="83" t="s">
         <v>229</v>
       </c>
@@ -5161,7 +5163,7 @@
       <c r="DZ7" s="125"/>
       <c r="EA7" s="126"/>
       <c r="EB7" s="127" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="EC7" s="125"/>
       <c r="ED7" s="125"/>
@@ -5178,16 +5180,16 @@
       <c r="EM7" s="81"/>
       <c r="EN7" s="81"/>
       <c r="EO7" s="82"/>
-      <c r="EP7" s="111" t="s">
+      <c r="EP7" s="112" t="s">
         <v>47</v>
       </c>
-      <c r="EQ7" s="112"/>
-      <c r="ER7" s="112"/>
-      <c r="ES7" s="112"/>
-      <c r="ET7" s="112"/>
-      <c r="EU7" s="112"/>
-      <c r="EV7" s="112"/>
-      <c r="EW7" s="113"/>
+      <c r="EQ7" s="113"/>
+      <c r="ER7" s="113"/>
+      <c r="ES7" s="113"/>
+      <c r="ET7" s="113"/>
+      <c r="EU7" s="113"/>
+      <c r="EV7" s="113"/>
+      <c r="EW7" s="114"/>
       <c r="EX7" s="22"/>
       <c r="EY7" s="87" t="s">
         <v>33</v>
@@ -5427,141 +5429,141 @@
       <c r="B9" s="62"/>
       <c r="C9" s="63"/>
       <c r="D9" s="63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E9" s="71" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
       <c r="H9" s="73"/>
-      <c r="I9" s="97" t="s">
+      <c r="I9" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="97"/>
-      <c r="K9" s="97"/>
-      <c r="L9" s="97"/>
-      <c r="M9" s="97"/>
-      <c r="N9" s="97"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="98"/>
+      <c r="P9" s="98"/>
+      <c r="Q9" s="99"/>
       <c r="R9" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="S9" s="117"/>
-      <c r="T9" s="118"/>
+      <c r="S9" s="118"/>
+      <c r="T9" s="119"/>
       <c r="U9" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="V9" s="117"/>
-      <c r="W9" s="118"/>
+      <c r="V9" s="118"/>
+      <c r="W9" s="119"/>
       <c r="X9" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="Y9" s="117"/>
-      <c r="Z9" s="118"/>
+        <v>255</v>
+      </c>
+      <c r="Y9" s="118"/>
+      <c r="Z9" s="119"/>
       <c r="AA9" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="AB9" s="117"/>
-      <c r="AC9" s="117"/>
-      <c r="AD9" s="117"/>
-      <c r="AE9" s="117"/>
-      <c r="AF9" s="117"/>
-      <c r="AG9" s="118"/>
+      <c r="AB9" s="118"/>
+      <c r="AC9" s="118"/>
+      <c r="AD9" s="118"/>
+      <c r="AE9" s="118"/>
+      <c r="AF9" s="118"/>
+      <c r="AG9" s="119"/>
       <c r="AH9" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="AI9" s="117"/>
-      <c r="AJ9" s="117"/>
-      <c r="AK9" s="117"/>
-      <c r="AL9" s="117"/>
-      <c r="AM9" s="117"/>
-      <c r="AN9" s="117"/>
-      <c r="AO9" s="117"/>
-      <c r="AP9" s="117"/>
-      <c r="AQ9" s="118"/>
+      <c r="AI9" s="118"/>
+      <c r="AJ9" s="118"/>
+      <c r="AK9" s="118"/>
+      <c r="AL9" s="118"/>
+      <c r="AM9" s="118"/>
+      <c r="AN9" s="118"/>
+      <c r="AO9" s="118"/>
+      <c r="AP9" s="118"/>
+      <c r="AQ9" s="119"/>
       <c r="AR9" s="95" t="s">
+        <v>251</v>
+      </c>
+      <c r="AS9" s="118"/>
+      <c r="AT9" s="118"/>
+      <c r="AU9" s="118"/>
+      <c r="AV9" s="118"/>
+      <c r="AW9" s="119"/>
+      <c r="AX9" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY9" s="118"/>
+      <c r="AZ9" s="118"/>
+      <c r="BA9" s="118"/>
+      <c r="BB9" s="118"/>
+      <c r="BC9" s="118"/>
+      <c r="BD9" s="118"/>
+      <c r="BE9" s="118"/>
+      <c r="BF9" s="118"/>
+      <c r="BG9" s="119"/>
+      <c r="BH9" s="95" t="s">
         <v>252</v>
       </c>
-      <c r="AS9" s="117"/>
-      <c r="AT9" s="117"/>
-      <c r="AU9" s="117"/>
-      <c r="AV9" s="117"/>
-      <c r="AW9" s="118"/>
-      <c r="AX9" s="117" t="s">
-        <v>54</v>
-      </c>
-      <c r="AY9" s="117"/>
-      <c r="AZ9" s="117"/>
-      <c r="BA9" s="117"/>
-      <c r="BB9" s="117"/>
-      <c r="BC9" s="117"/>
-      <c r="BD9" s="117"/>
-      <c r="BE9" s="117"/>
-      <c r="BF9" s="117"/>
-      <c r="BG9" s="118"/>
-      <c r="BH9" s="95" t="s">
-        <v>253</v>
-      </c>
-      <c r="BI9" s="117"/>
-      <c r="BJ9" s="117"/>
-      <c r="BK9" s="117"/>
-      <c r="BL9" s="117"/>
-      <c r="BM9" s="118"/>
+      <c r="BI9" s="118"/>
+      <c r="BJ9" s="118"/>
+      <c r="BK9" s="118"/>
+      <c r="BL9" s="118"/>
+      <c r="BM9" s="119"/>
       <c r="BN9" s="165" t="s">
         <v>49</v>
       </c>
-      <c r="BO9" s="97"/>
-      <c r="BP9" s="97"/>
-      <c r="BQ9" s="97"/>
-      <c r="BR9" s="97"/>
-      <c r="BS9" s="97"/>
-      <c r="BT9" s="97"/>
-      <c r="BU9" s="98"/>
+      <c r="BO9" s="98"/>
+      <c r="BP9" s="98"/>
+      <c r="BQ9" s="98"/>
+      <c r="BR9" s="98"/>
+      <c r="BS9" s="98"/>
+      <c r="BT9" s="98"/>
+      <c r="BU9" s="99"/>
       <c r="BV9" s="95" t="s">
         <v>141</v>
       </c>
-      <c r="BW9" s="97"/>
-      <c r="BX9" s="97"/>
-      <c r="BY9" s="97"/>
-      <c r="BZ9" s="97"/>
-      <c r="CA9" s="97"/>
-      <c r="CB9" s="97"/>
-      <c r="CC9" s="98"/>
+      <c r="BW9" s="98"/>
+      <c r="BX9" s="98"/>
+      <c r="BY9" s="98"/>
+      <c r="BZ9" s="98"/>
+      <c r="CA9" s="98"/>
+      <c r="CB9" s="98"/>
+      <c r="CC9" s="99"/>
       <c r="CD9" s="57" t="s">
-        <v>258</v>
-      </c>
-      <c r="CE9" s="117" t="s">
-        <v>245</v>
-      </c>
-      <c r="CF9" s="117"/>
-      <c r="CG9" s="117"/>
-      <c r="CH9" s="117" t="s">
+        <v>257</v>
+      </c>
+      <c r="CE9" s="118" t="s">
+        <v>244</v>
+      </c>
+      <c r="CF9" s="118"/>
+      <c r="CG9" s="118"/>
+      <c r="CH9" s="118" t="s">
         <v>214</v>
       </c>
-      <c r="CI9" s="117"/>
-      <c r="CJ9" s="117"/>
-      <c r="CK9" s="118"/>
+      <c r="CI9" s="118"/>
+      <c r="CJ9" s="118"/>
+      <c r="CK9" s="119"/>
       <c r="CL9" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="CM9" s="117"/>
-      <c r="CN9" s="117"/>
-      <c r="CO9" s="117"/>
-      <c r="CP9" s="117"/>
-      <c r="CQ9" s="117"/>
-      <c r="CR9" s="117"/>
-      <c r="CS9" s="117"/>
-      <c r="CT9" s="117"/>
-      <c r="CU9" s="117"/>
-      <c r="CV9" s="117"/>
-      <c r="CW9" s="117"/>
-      <c r="CX9" s="117"/>
-      <c r="CY9" s="117"/>
-      <c r="CZ9" s="117"/>
-      <c r="DA9" s="118"/>
+      <c r="CM9" s="118"/>
+      <c r="CN9" s="118"/>
+      <c r="CO9" s="118"/>
+      <c r="CP9" s="118"/>
+      <c r="CQ9" s="118"/>
+      <c r="CR9" s="118"/>
+      <c r="CS9" s="118"/>
+      <c r="CT9" s="118"/>
+      <c r="CU9" s="118"/>
+      <c r="CV9" s="118"/>
+      <c r="CW9" s="118"/>
+      <c r="CX9" s="118"/>
+      <c r="CY9" s="118"/>
+      <c r="CZ9" s="118"/>
+      <c r="DA9" s="119"/>
       <c r="DB9" s="151" t="s">
         <v>231</v>
       </c>
@@ -5578,7 +5580,7 @@
       </c>
       <c r="DH9" s="51"/>
       <c r="DI9" s="55" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="DJ9" s="151" t="s">
         <v>197</v>
@@ -5601,39 +5603,39 @@
       <c r="DV9" s="95" t="s">
         <v>222</v>
       </c>
-      <c r="DW9" s="117"/>
-      <c r="DX9" s="117"/>
-      <c r="DY9" s="117"/>
-      <c r="DZ9" s="117"/>
-      <c r="EA9" s="118"/>
+      <c r="DW9" s="118"/>
+      <c r="DX9" s="118"/>
+      <c r="DY9" s="118"/>
+      <c r="DZ9" s="118"/>
+      <c r="EA9" s="119"/>
       <c r="EB9" s="95" t="s">
         <v>221</v>
       </c>
-      <c r="EC9" s="117"/>
-      <c r="ED9" s="117"/>
-      <c r="EE9" s="117"/>
-      <c r="EF9" s="117"/>
-      <c r="EG9" s="118"/>
+      <c r="EC9" s="118"/>
+      <c r="ED9" s="118"/>
+      <c r="EE9" s="118"/>
+      <c r="EF9" s="118"/>
+      <c r="EG9" s="119"/>
       <c r="EP9" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="EQ9" s="117"/>
-      <c r="ER9" s="117"/>
-      <c r="ES9" s="117"/>
-      <c r="ET9" s="117"/>
-      <c r="EU9" s="117"/>
-      <c r="EV9" s="117"/>
-      <c r="EW9" s="118"/>
+      <c r="EQ9" s="118"/>
+      <c r="ER9" s="118"/>
+      <c r="ES9" s="118"/>
+      <c r="ET9" s="118"/>
+      <c r="EU9" s="118"/>
+      <c r="EV9" s="118"/>
+      <c r="EW9" s="119"/>
       <c r="EX9" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="EY9" s="117"/>
-      <c r="EZ9" s="117"/>
-      <c r="FA9" s="117"/>
-      <c r="FB9" s="117"/>
-      <c r="FC9" s="117"/>
-      <c r="FD9" s="117"/>
-      <c r="FE9" s="118"/>
+      <c r="EY9" s="118"/>
+      <c r="EZ9" s="118"/>
+      <c r="FA9" s="118"/>
+      <c r="FB9" s="118"/>
+      <c r="FC9" s="118"/>
+      <c r="FD9" s="118"/>
+      <c r="FE9" s="119"/>
       <c r="FG9" t="s">
         <v>216</v>
       </c>
@@ -5643,31 +5645,31 @@
       <c r="FL9" s="89"/>
       <c r="FM9" s="148"/>
       <c r="FN9" s="95" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="FO9" s="59"/>
       <c r="FP9" s="16"/>
       <c r="FQ9" s="46"/>
       <c r="FR9" s="46"/>
       <c r="FU9" s="30"/>
-      <c r="FV9" s="117" t="s">
+      <c r="FV9" s="118" t="s">
         <v>201</v>
       </c>
-      <c r="FW9" s="97"/>
-      <c r="FX9" s="97"/>
-      <c r="FY9" s="97"/>
-      <c r="FZ9" s="97"/>
-      <c r="GA9" s="98"/>
+      <c r="FW9" s="98"/>
+      <c r="FX9" s="98"/>
+      <c r="FY9" s="98"/>
+      <c r="FZ9" s="98"/>
+      <c r="GA9" s="99"/>
       <c r="GB9" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="GC9" s="97"/>
-      <c r="GD9" s="97"/>
-      <c r="GE9" s="97"/>
-      <c r="GF9" s="97"/>
-      <c r="GG9" s="98"/>
+      <c r="GC9" s="98"/>
+      <c r="GD9" s="98"/>
+      <c r="GE9" s="98"/>
+      <c r="GF9" s="98"/>
+      <c r="GG9" s="99"/>
       <c r="GH9" s="77" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="GI9" s="78"/>
       <c r="GJ9" s="78"/>
@@ -5680,69 +5682,69 @@
       <c r="GO9" s="95" t="s">
         <v>195</v>
       </c>
-      <c r="GP9" s="117"/>
-      <c r="GQ9" s="117"/>
-      <c r="GR9" s="117"/>
-      <c r="GS9" s="118"/>
+      <c r="GP9" s="118"/>
+      <c r="GQ9" s="118"/>
+      <c r="GR9" s="118"/>
+      <c r="GS9" s="119"/>
       <c r="GT9" s="95" t="s">
-        <v>241</v>
-      </c>
-      <c r="GU9" s="117"/>
-      <c r="GV9" s="117"/>
-      <c r="GW9" s="117"/>
-      <c r="GX9" s="117"/>
-      <c r="GY9" s="117"/>
-      <c r="GZ9" s="117"/>
-      <c r="HA9" s="119"/>
+        <v>270</v>
+      </c>
+      <c r="GU9" s="118"/>
+      <c r="GV9" s="118"/>
+      <c r="GW9" s="118"/>
+      <c r="GX9" s="118"/>
+      <c r="GY9" s="118"/>
+      <c r="GZ9" s="118"/>
+      <c r="HA9" s="97"/>
       <c r="HB9" s="95" t="s">
         <v>191</v>
       </c>
-      <c r="HC9" s="117"/>
-      <c r="HD9" s="117"/>
-      <c r="HE9" s="117"/>
-      <c r="HF9" s="117"/>
-      <c r="HG9" s="117"/>
-      <c r="HH9" s="117"/>
-      <c r="HI9" s="118"/>
+      <c r="HC9" s="118"/>
+      <c r="HD9" s="118"/>
+      <c r="HE9" s="118"/>
+      <c r="HF9" s="118"/>
+      <c r="HG9" s="118"/>
+      <c r="HH9" s="118"/>
+      <c r="HI9" s="119"/>
     </row>
     <row r="10" spans="1:217" ht="77.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="7"/>
       <c r="B10" s="64"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="74" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G10" s="75"/>
       <c r="H10" s="76"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="99"/>
-      <c r="N10" s="99"/>
-      <c r="O10" s="99"/>
-      <c r="P10" s="99"/>
-      <c r="Q10" s="100"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="100"/>
+      <c r="O10" s="100"/>
+      <c r="P10" s="100"/>
+      <c r="Q10" s="101"/>
       <c r="R10" s="77"/>
       <c r="S10" s="78"/>
-      <c r="T10" s="119"/>
+      <c r="T10" s="97"/>
       <c r="U10" s="77"/>
       <c r="V10" s="78"/>
-      <c r="W10" s="119"/>
+      <c r="W10" s="97"/>
       <c r="X10" s="77"/>
       <c r="Y10" s="78"/>
-      <c r="Z10" s="119"/>
+      <c r="Z10" s="97"/>
       <c r="AA10" s="77"/>
       <c r="AB10" s="78"/>
       <c r="AC10" s="78"/>
       <c r="AD10" s="78"/>
       <c r="AE10" s="78"/>
       <c r="AF10" s="78"/>
-      <c r="AG10" s="119"/>
+      <c r="AG10" s="97"/>
       <c r="AH10" s="77"/>
       <c r="AI10" s="78"/>
       <c r="AJ10" s="78"/>
@@ -5752,13 +5754,13 @@
       <c r="AN10" s="78"/>
       <c r="AO10" s="78"/>
       <c r="AP10" s="78"/>
-      <c r="AQ10" s="119"/>
+      <c r="AQ10" s="97"/>
       <c r="AR10" s="77"/>
       <c r="AS10" s="78"/>
       <c r="AT10" s="78"/>
       <c r="AU10" s="78"/>
       <c r="AV10" s="78"/>
-      <c r="AW10" s="119"/>
+      <c r="AW10" s="97"/>
       <c r="AX10" s="78"/>
       <c r="AY10" s="78"/>
       <c r="AZ10" s="78"/>
@@ -5768,34 +5770,34 @@
       <c r="BD10" s="78"/>
       <c r="BE10" s="78"/>
       <c r="BF10" s="78"/>
-      <c r="BG10" s="119"/>
+      <c r="BG10" s="97"/>
       <c r="BH10" s="77"/>
       <c r="BI10" s="78"/>
       <c r="BJ10" s="78"/>
       <c r="BK10" s="78"/>
       <c r="BL10" s="78"/>
-      <c r="BM10" s="119"/>
-      <c r="BN10" s="101"/>
-      <c r="BO10" s="99"/>
-      <c r="BP10" s="99"/>
-      <c r="BQ10" s="99"/>
-      <c r="BR10" s="99"/>
-      <c r="BS10" s="99"/>
-      <c r="BT10" s="99"/>
-      <c r="BU10" s="100"/>
-      <c r="BV10" s="101"/>
-      <c r="BW10" s="99"/>
-      <c r="BX10" s="99"/>
-      <c r="BY10" s="99"/>
-      <c r="BZ10" s="99"/>
-      <c r="CA10" s="99"/>
-      <c r="CB10" s="99"/>
-      <c r="CC10" s="100"/>
+      <c r="BM10" s="97"/>
+      <c r="BN10" s="102"/>
+      <c r="BO10" s="100"/>
+      <c r="BP10" s="100"/>
+      <c r="BQ10" s="100"/>
+      <c r="BR10" s="100"/>
+      <c r="BS10" s="100"/>
+      <c r="BT10" s="100"/>
+      <c r="BU10" s="101"/>
+      <c r="BV10" s="102"/>
+      <c r="BW10" s="100"/>
+      <c r="BX10" s="100"/>
+      <c r="BY10" s="100"/>
+      <c r="BZ10" s="100"/>
+      <c r="CA10" s="100"/>
+      <c r="CB10" s="100"/>
+      <c r="CC10" s="101"/>
       <c r="CD10" s="47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="CE10" s="78" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="CF10" s="78"/>
       <c r="CG10" s="78"/>
@@ -5818,7 +5820,7 @@
       <c r="CX10" s="78"/>
       <c r="CY10" s="78"/>
       <c r="CZ10" s="78"/>
-      <c r="DA10" s="119"/>
+      <c r="DA10" s="97"/>
       <c r="DB10" s="153"/>
       <c r="DC10" s="154"/>
       <c r="DD10" s="164"/>
@@ -5844,13 +5846,13 @@
       <c r="DX10" s="78"/>
       <c r="DY10" s="78"/>
       <c r="DZ10" s="78"/>
-      <c r="EA10" s="119"/>
+      <c r="EA10" s="97"/>
       <c r="EB10" s="77"/>
       <c r="EC10" s="78"/>
       <c r="ED10" s="78"/>
       <c r="EE10" s="78"/>
       <c r="EF10" s="78"/>
-      <c r="EG10" s="119"/>
+      <c r="EG10" s="97"/>
       <c r="EP10" s="77"/>
       <c r="EQ10" s="78"/>
       <c r="ER10" s="78"/>
@@ -5858,7 +5860,7 @@
       <c r="ET10" s="78"/>
       <c r="EU10" s="78"/>
       <c r="EV10" s="78"/>
-      <c r="EW10" s="119"/>
+      <c r="EW10" s="97"/>
       <c r="EX10" s="17"/>
       <c r="EY10" t="s">
         <v>207</v>
@@ -5875,18 +5877,18 @@
       <c r="FQ10" s="16"/>
       <c r="FR10" s="16"/>
       <c r="FU10" s="30"/>
-      <c r="FV10" s="99"/>
-      <c r="FW10" s="99"/>
-      <c r="FX10" s="99"/>
-      <c r="FY10" s="99"/>
-      <c r="FZ10" s="99"/>
-      <c r="GA10" s="100"/>
-      <c r="GB10" s="101"/>
-      <c r="GC10" s="99"/>
-      <c r="GD10" s="99"/>
-      <c r="GE10" s="99"/>
-      <c r="GF10" s="99"/>
-      <c r="GG10" s="100"/>
+      <c r="FV10" s="100"/>
+      <c r="FW10" s="100"/>
+      <c r="FX10" s="100"/>
+      <c r="FY10" s="100"/>
+      <c r="FZ10" s="100"/>
+      <c r="GA10" s="101"/>
+      <c r="GB10" s="102"/>
+      <c r="GC10" s="100"/>
+      <c r="GD10" s="100"/>
+      <c r="GE10" s="100"/>
+      <c r="GF10" s="100"/>
+      <c r="GG10" s="101"/>
       <c r="GH10" s="77"/>
       <c r="GI10" s="78"/>
       <c r="GJ10" s="78"/>
@@ -5906,7 +5908,7 @@
       <c r="GX10" s="78"/>
       <c r="GY10" s="78"/>
       <c r="GZ10" s="78"/>
-      <c r="HA10" s="119"/>
+      <c r="HA10" s="97"/>
       <c r="HB10" s="77"/>
       <c r="HC10" s="78"/>
       <c r="HD10" s="78"/>
@@ -5914,44 +5916,44 @@
       <c r="HF10" s="78"/>
       <c r="HG10" s="78"/>
       <c r="HH10" s="78"/>
-      <c r="HI10" s="119"/>
+      <c r="HI10" s="97"/>
     </row>
     <row r="11" spans="1:217" ht="55.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="7"/>
       <c r="B11" s="65"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E11" s="66"/>
       <c r="F11" s="66"/>
       <c r="G11" s="66"/>
       <c r="H11" s="67"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="99"/>
-      <c r="K11" s="99"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="99"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="100"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="100"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="100"/>
+      <c r="P11" s="100"/>
+      <c r="Q11" s="101"/>
       <c r="R11" s="77"/>
       <c r="S11" s="78"/>
-      <c r="T11" s="119"/>
+      <c r="T11" s="97"/>
       <c r="U11" s="77"/>
       <c r="V11" s="78"/>
-      <c r="W11" s="119"/>
+      <c r="W11" s="97"/>
       <c r="X11" s="77"/>
       <c r="Y11" s="78"/>
-      <c r="Z11" s="119"/>
+      <c r="Z11" s="97"/>
       <c r="AA11" s="77"/>
       <c r="AB11" s="78"/>
       <c r="AC11" s="78"/>
       <c r="AD11" s="78"/>
       <c r="AE11" s="78"/>
       <c r="AF11" s="78"/>
-      <c r="AG11" s="119"/>
+      <c r="AG11" s="97"/>
       <c r="AH11" s="77"/>
       <c r="AI11" s="78"/>
       <c r="AJ11" s="78"/>
@@ -5961,13 +5963,13 @@
       <c r="AN11" s="78"/>
       <c r="AO11" s="78"/>
       <c r="AP11" s="78"/>
-      <c r="AQ11" s="119"/>
+      <c r="AQ11" s="97"/>
       <c r="AR11" s="77"/>
       <c r="AS11" s="78"/>
       <c r="AT11" s="78"/>
       <c r="AU11" s="78"/>
       <c r="AV11" s="78"/>
-      <c r="AW11" s="119"/>
+      <c r="AW11" s="97"/>
       <c r="AX11" s="78"/>
       <c r="AY11" s="78"/>
       <c r="AZ11" s="78"/>
@@ -5977,31 +5979,31 @@
       <c r="BD11" s="78"/>
       <c r="BE11" s="78"/>
       <c r="BF11" s="78"/>
-      <c r="BG11" s="119"/>
+      <c r="BG11" s="97"/>
       <c r="BH11" s="77"/>
       <c r="BI11" s="78"/>
       <c r="BJ11" s="78"/>
       <c r="BK11" s="78"/>
       <c r="BL11" s="78"/>
-      <c r="BM11" s="119"/>
-      <c r="BN11" s="101"/>
-      <c r="BO11" s="99"/>
-      <c r="BP11" s="99"/>
-      <c r="BQ11" s="99"/>
-      <c r="BR11" s="99"/>
-      <c r="BS11" s="99"/>
-      <c r="BT11" s="99"/>
-      <c r="BU11" s="100"/>
-      <c r="BV11" s="101"/>
-      <c r="BW11" s="99"/>
-      <c r="BX11" s="99"/>
-      <c r="BY11" s="99"/>
-      <c r="BZ11" s="99"/>
-      <c r="CA11" s="99"/>
-      <c r="CB11" s="99"/>
-      <c r="CC11" s="100"/>
+      <c r="BM11" s="97"/>
+      <c r="BN11" s="102"/>
+      <c r="BO11" s="100"/>
+      <c r="BP11" s="100"/>
+      <c r="BQ11" s="100"/>
+      <c r="BR11" s="100"/>
+      <c r="BS11" s="100"/>
+      <c r="BT11" s="100"/>
+      <c r="BU11" s="101"/>
+      <c r="BV11" s="102"/>
+      <c r="BW11" s="100"/>
+      <c r="BX11" s="100"/>
+      <c r="BY11" s="100"/>
+      <c r="BZ11" s="100"/>
+      <c r="CA11" s="100"/>
+      <c r="CB11" s="100"/>
+      <c r="CC11" s="101"/>
       <c r="CD11" s="56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="CE11" s="16"/>
       <c r="CF11" s="16"/>
@@ -6025,7 +6027,7 @@
       <c r="CX11" s="78"/>
       <c r="CY11" s="78"/>
       <c r="CZ11" s="78"/>
-      <c r="DA11" s="119"/>
+      <c r="DA11" s="97"/>
       <c r="DB11" s="153"/>
       <c r="DC11" s="154"/>
       <c r="DD11" s="164"/>
@@ -6069,7 +6071,7 @@
       <c r="EL11" s="78"/>
       <c r="EM11" s="78"/>
       <c r="EN11" s="78"/>
-      <c r="EO11" s="119"/>
+      <c r="EO11" s="97"/>
       <c r="EP11" s="77"/>
       <c r="EQ11" s="78"/>
       <c r="ER11" s="78"/>
@@ -6077,7 +6079,7 @@
       <c r="ET11" s="78"/>
       <c r="EU11" s="78"/>
       <c r="EV11" s="78"/>
-      <c r="EW11" s="119"/>
+      <c r="EW11" s="97"/>
       <c r="EX11" s="47" t="s">
         <v>211</v>
       </c>
@@ -6089,7 +6091,7 @@
       <c r="FB11" s="78"/>
       <c r="FC11" s="78"/>
       <c r="FD11" s="78"/>
-      <c r="FE11" s="119"/>
+      <c r="FE11" s="97"/>
       <c r="FF11" s="146" t="s">
         <v>204</v>
       </c>
@@ -6102,7 +6104,7 @@
       <c r="FL11" s="89"/>
       <c r="FM11" s="90"/>
       <c r="FN11" s="144" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="FO11" s="145"/>
       <c r="FP11" s="144" t="s">
@@ -6113,27 +6115,27 @@
       <c r="FS11" s="78"/>
       <c r="FT11" s="78"/>
       <c r="FU11" s="145"/>
-      <c r="FV11" s="99"/>
-      <c r="FW11" s="99"/>
-      <c r="FX11" s="99"/>
-      <c r="FY11" s="99"/>
-      <c r="FZ11" s="99"/>
-      <c r="GA11" s="100"/>
-      <c r="GB11" s="101"/>
-      <c r="GC11" s="99"/>
-      <c r="GD11" s="99"/>
-      <c r="GE11" s="99"/>
-      <c r="GF11" s="99"/>
-      <c r="GG11" s="100"/>
+      <c r="FV11" s="100"/>
+      <c r="FW11" s="100"/>
+      <c r="FX11" s="100"/>
+      <c r="FY11" s="100"/>
+      <c r="FZ11" s="100"/>
+      <c r="GA11" s="101"/>
+      <c r="GB11" s="102"/>
+      <c r="GC11" s="100"/>
+      <c r="GD11" s="100"/>
+      <c r="GE11" s="100"/>
+      <c r="GF11" s="100"/>
+      <c r="GG11" s="101"/>
       <c r="GH11" s="77"/>
       <c r="GI11" s="78"/>
       <c r="GJ11" s="78"/>
       <c r="GK11" s="78"/>
-      <c r="GL11" s="117" t="s">
+      <c r="GL11" s="118" t="s">
         <v>198</v>
       </c>
-      <c r="GM11" s="117"/>
-      <c r="GN11" s="117"/>
+      <c r="GM11" s="118"/>
+      <c r="GN11" s="118"/>
       <c r="GT11" s="77"/>
       <c r="GU11" s="78"/>
       <c r="GV11" s="78"/>
@@ -6141,7 +6143,7 @@
       <c r="GX11" s="78"/>
       <c r="GY11" s="78"/>
       <c r="GZ11" s="78"/>
-      <c r="HA11" s="119"/>
+      <c r="HA11" s="97"/>
       <c r="HB11" s="77"/>
       <c r="HC11" s="78"/>
       <c r="HD11" s="78"/>
@@ -6149,45 +6151,45 @@
       <c r="HF11" s="78"/>
       <c r="HG11" s="78"/>
       <c r="HH11" s="78"/>
-      <c r="HI11" s="119"/>
+      <c r="HI11" s="97"/>
     </row>
     <row r="12" spans="1:217" ht="88.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="7"/>
       <c r="B12" s="47"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="48"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="99"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="99"/>
-      <c r="N12" s="99"/>
-      <c r="O12" s="99"/>
-      <c r="P12" s="99"/>
-      <c r="Q12" s="100"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="100"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="100"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="100"/>
+      <c r="O12" s="100"/>
+      <c r="P12" s="100"/>
+      <c r="Q12" s="101"/>
       <c r="R12" s="77"/>
       <c r="S12" s="78"/>
-      <c r="T12" s="119"/>
+      <c r="T12" s="97"/>
       <c r="U12" s="77"/>
       <c r="V12" s="78"/>
-      <c r="W12" s="119"/>
+      <c r="W12" s="97"/>
       <c r="X12" s="77"/>
       <c r="Y12" s="78"/>
-      <c r="Z12" s="119"/>
+      <c r="Z12" s="97"/>
       <c r="AA12" s="77"/>
       <c r="AB12" s="78"/>
       <c r="AC12" s="78"/>
       <c r="AD12" s="78"/>
       <c r="AE12" s="78"/>
       <c r="AF12" s="78"/>
-      <c r="AG12" s="119"/>
+      <c r="AG12" s="97"/>
       <c r="AH12" s="77"/>
       <c r="AI12" s="78"/>
       <c r="AJ12" s="78"/>
@@ -6197,13 +6199,13 @@
       <c r="AN12" s="78"/>
       <c r="AO12" s="78"/>
       <c r="AP12" s="78"/>
-      <c r="AQ12" s="119"/>
+      <c r="AQ12" s="97"/>
       <c r="AR12" s="77"/>
       <c r="AS12" s="78"/>
       <c r="AT12" s="78"/>
       <c r="AU12" s="78"/>
       <c r="AV12" s="78"/>
-      <c r="AW12" s="119"/>
+      <c r="AW12" s="97"/>
       <c r="AX12" s="78"/>
       <c r="AY12" s="78"/>
       <c r="AZ12" s="78"/>
@@ -6213,34 +6215,34 @@
       <c r="BD12" s="78"/>
       <c r="BE12" s="78"/>
       <c r="BF12" s="78"/>
-      <c r="BG12" s="119"/>
+      <c r="BG12" s="97"/>
       <c r="BH12" s="77"/>
       <c r="BI12" s="78"/>
       <c r="BJ12" s="78"/>
       <c r="BK12" s="78"/>
       <c r="BL12" s="78"/>
-      <c r="BM12" s="119"/>
-      <c r="BN12" s="101"/>
-      <c r="BO12" s="99"/>
-      <c r="BP12" s="99"/>
-      <c r="BQ12" s="99"/>
-      <c r="BR12" s="99"/>
-      <c r="BS12" s="99"/>
-      <c r="BT12" s="99"/>
-      <c r="BU12" s="100"/>
-      <c r="BV12" s="101"/>
-      <c r="BW12" s="99"/>
-      <c r="BX12" s="99"/>
-      <c r="BY12" s="99"/>
-      <c r="BZ12" s="99"/>
-      <c r="CA12" s="99"/>
-      <c r="CB12" s="99"/>
-      <c r="CC12" s="100"/>
+      <c r="BM12" s="97"/>
+      <c r="BN12" s="102"/>
+      <c r="BO12" s="100"/>
+      <c r="BP12" s="100"/>
+      <c r="BQ12" s="100"/>
+      <c r="BR12" s="100"/>
+      <c r="BS12" s="100"/>
+      <c r="BT12" s="100"/>
+      <c r="BU12" s="101"/>
+      <c r="BV12" s="102"/>
+      <c r="BW12" s="100"/>
+      <c r="BX12" s="100"/>
+      <c r="BY12" s="100"/>
+      <c r="BZ12" s="100"/>
+      <c r="CA12" s="100"/>
+      <c r="CB12" s="100"/>
+      <c r="CC12" s="101"/>
       <c r="CD12" s="47" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="CE12" s="78" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="CF12" s="78"/>
       <c r="CG12" s="78"/>
@@ -6249,15 +6251,15 @@
       <c r="CK12" s="48"/>
       <c r="CL12" s="17"/>
       <c r="CP12" s="78" t="s">
-        <v>251</v>
-      </c>
-      <c r="CQ12" s="99"/>
-      <c r="CR12" s="99"/>
-      <c r="CS12" s="99"/>
-      <c r="CT12" s="99"/>
-      <c r="CU12" s="99"/>
-      <c r="CV12" s="99"/>
-      <c r="CW12" s="99"/>
+        <v>250</v>
+      </c>
+      <c r="CQ12" s="100"/>
+      <c r="CR12" s="100"/>
+      <c r="CS12" s="100"/>
+      <c r="CT12" s="100"/>
+      <c r="CU12" s="100"/>
+      <c r="CV12" s="100"/>
+      <c r="CW12" s="100"/>
       <c r="DB12" s="155"/>
       <c r="DC12" s="156"/>
       <c r="DD12" s="164"/>
@@ -6297,7 +6299,7 @@
       <c r="EL12" s="78"/>
       <c r="EM12" s="78"/>
       <c r="EN12" s="78"/>
-      <c r="EO12" s="119"/>
+      <c r="EO12" s="97"/>
       <c r="EP12" s="77"/>
       <c r="EQ12" s="78"/>
       <c r="ER12" s="78"/>
@@ -6305,7 +6307,7 @@
       <c r="ET12" s="78"/>
       <c r="EU12" s="78"/>
       <c r="EV12" s="78"/>
-      <c r="EW12" s="119"/>
+      <c r="EW12" s="97"/>
       <c r="EX12" s="128" t="s">
         <v>210</v>
       </c>
@@ -6324,18 +6326,18 @@
       <c r="FS12" s="78"/>
       <c r="FT12" s="78"/>
       <c r="FU12" s="145"/>
-      <c r="FV12" s="99"/>
-      <c r="FW12" s="99"/>
-      <c r="FX12" s="99"/>
-      <c r="FY12" s="99"/>
-      <c r="FZ12" s="99"/>
-      <c r="GA12" s="100"/>
-      <c r="GB12" s="101"/>
-      <c r="GC12" s="99"/>
-      <c r="GD12" s="99"/>
-      <c r="GE12" s="99"/>
-      <c r="GF12" s="99"/>
-      <c r="GG12" s="100"/>
+      <c r="FV12" s="100"/>
+      <c r="FW12" s="100"/>
+      <c r="FX12" s="100"/>
+      <c r="FY12" s="100"/>
+      <c r="FZ12" s="100"/>
+      <c r="GA12" s="101"/>
+      <c r="GB12" s="102"/>
+      <c r="GC12" s="100"/>
+      <c r="GD12" s="100"/>
+      <c r="GE12" s="100"/>
+      <c r="GF12" s="100"/>
+      <c r="GG12" s="101"/>
       <c r="GH12" s="77"/>
       <c r="GI12" s="78"/>
       <c r="GJ12" s="78"/>
@@ -6350,7 +6352,7 @@
       <c r="GX12" s="78"/>
       <c r="GY12" s="78"/>
       <c r="GZ12" s="78"/>
-      <c r="HA12" s="119"/>
+      <c r="HA12" s="97"/>
       <c r="HB12" s="77"/>
       <c r="HC12" s="78"/>
       <c r="HD12" s="78"/>
@@ -6358,7 +6360,7 @@
       <c r="HF12" s="78"/>
       <c r="HG12" s="78"/>
       <c r="HH12" s="78"/>
-      <c r="HI12" s="119"/>
+      <c r="HI12" s="97"/>
     </row>
     <row r="13" spans="1:217" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
@@ -6372,38 +6374,38 @@
         <v>234</v>
       </c>
       <c r="E13" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="F13" s="78" t="s">
         <v>269</v>
       </c>
-      <c r="F13" s="78" t="s">
-        <v>270</v>
-      </c>
       <c r="G13" s="78"/>
-      <c r="H13" s="119"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="99"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="99"/>
-      <c r="O13" s="99"/>
-      <c r="P13" s="99"/>
-      <c r="Q13" s="100"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="100"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="100"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="100"/>
+      <c r="Q13" s="101"/>
       <c r="R13" s="77"/>
       <c r="S13" s="78"/>
-      <c r="T13" s="119"/>
+      <c r="T13" s="97"/>
       <c r="U13" s="77"/>
       <c r="V13" s="78"/>
-      <c r="W13" s="119"/>
+      <c r="W13" s="97"/>
       <c r="X13" s="77"/>
       <c r="Y13" s="78"/>
-      <c r="Z13" s="119"/>
+      <c r="Z13" s="97"/>
       <c r="AA13" s="77"/>
       <c r="AB13" s="78"/>
       <c r="AC13" s="78"/>
       <c r="AD13" s="78"/>
       <c r="AE13" s="78"/>
       <c r="AF13" s="78"/>
-      <c r="AG13" s="119"/>
+      <c r="AG13" s="97"/>
       <c r="AH13" s="77"/>
       <c r="AI13" s="78"/>
       <c r="AJ13" s="78"/>
@@ -6413,13 +6415,13 @@
       <c r="AN13" s="78"/>
       <c r="AO13" s="78"/>
       <c r="AP13" s="78"/>
-      <c r="AQ13" s="119"/>
+      <c r="AQ13" s="97"/>
       <c r="AR13" s="77"/>
       <c r="AS13" s="78"/>
       <c r="AT13" s="78"/>
       <c r="AU13" s="78"/>
       <c r="AV13" s="78"/>
-      <c r="AW13" s="119"/>
+      <c r="AW13" s="97"/>
       <c r="AX13" s="78"/>
       <c r="AY13" s="78"/>
       <c r="AZ13" s="78"/>
@@ -6429,34 +6431,34 @@
       <c r="BD13" s="78"/>
       <c r="BE13" s="78"/>
       <c r="BF13" s="78"/>
-      <c r="BG13" s="119"/>
+      <c r="BG13" s="97"/>
       <c r="BH13" s="77"/>
       <c r="BI13" s="78"/>
       <c r="BJ13" s="78"/>
       <c r="BK13" s="78"/>
       <c r="BL13" s="78"/>
-      <c r="BM13" s="119"/>
-      <c r="BN13" s="101"/>
-      <c r="BO13" s="99"/>
-      <c r="BP13" s="99"/>
-      <c r="BQ13" s="99"/>
-      <c r="BR13" s="99"/>
-      <c r="BS13" s="99"/>
-      <c r="BT13" s="99"/>
-      <c r="BU13" s="100"/>
-      <c r="BV13" s="101"/>
-      <c r="BW13" s="99"/>
-      <c r="BX13" s="99"/>
-      <c r="BY13" s="99"/>
-      <c r="BZ13" s="99"/>
-      <c r="CA13" s="99"/>
-      <c r="CB13" s="99"/>
-      <c r="CC13" s="100"/>
+      <c r="BM13" s="97"/>
+      <c r="BN13" s="102"/>
+      <c r="BO13" s="100"/>
+      <c r="BP13" s="100"/>
+      <c r="BQ13" s="100"/>
+      <c r="BR13" s="100"/>
+      <c r="BS13" s="100"/>
+      <c r="BT13" s="100"/>
+      <c r="BU13" s="101"/>
+      <c r="BV13" s="102"/>
+      <c r="BW13" s="100"/>
+      <c r="BX13" s="100"/>
+      <c r="BY13" s="100"/>
+      <c r="BZ13" s="100"/>
+      <c r="CA13" s="100"/>
+      <c r="CB13" s="100"/>
+      <c r="CC13" s="101"/>
       <c r="CD13" s="47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="CE13" s="78" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="CF13" s="78"/>
       <c r="CG13" s="78"/>
@@ -6465,14 +6467,14 @@
       <c r="CJ13" s="16"/>
       <c r="CK13" s="48"/>
       <c r="CL13" s="17"/>
-      <c r="CP13" s="99"/>
-      <c r="CQ13" s="99"/>
-      <c r="CR13" s="99"/>
-      <c r="CS13" s="99"/>
-      <c r="CT13" s="99"/>
-      <c r="CU13" s="99"/>
-      <c r="CV13" s="99"/>
-      <c r="CW13" s="99"/>
+      <c r="CP13" s="100"/>
+      <c r="CQ13" s="100"/>
+      <c r="CR13" s="100"/>
+      <c r="CS13" s="100"/>
+      <c r="CT13" s="100"/>
+      <c r="CU13" s="100"/>
+      <c r="CV13" s="100"/>
+      <c r="CW13" s="100"/>
       <c r="DB13" s="144" t="s">
         <v>194</v>
       </c>
@@ -6516,7 +6518,7 @@
       <c r="EL13" s="78"/>
       <c r="EM13" s="78"/>
       <c r="EN13" s="78"/>
-      <c r="EO13" s="119"/>
+      <c r="EO13" s="97"/>
       <c r="EP13" s="77"/>
       <c r="EQ13" s="78"/>
       <c r="ER13" s="78"/>
@@ -6524,7 +6526,7 @@
       <c r="ET13" s="78"/>
       <c r="EU13" s="78"/>
       <c r="EV13" s="78"/>
-      <c r="EW13" s="119"/>
+      <c r="EW13" s="97"/>
       <c r="EX13" s="128"/>
       <c r="EY13" s="17" t="s">
         <v>208</v>
@@ -6543,18 +6545,18 @@
       <c r="FS13" s="78"/>
       <c r="FT13" s="78"/>
       <c r="FU13" s="145"/>
-      <c r="FV13" s="99"/>
-      <c r="FW13" s="99"/>
-      <c r="FX13" s="99"/>
-      <c r="FY13" s="99"/>
-      <c r="FZ13" s="99"/>
-      <c r="GA13" s="100"/>
-      <c r="GB13" s="101"/>
-      <c r="GC13" s="99"/>
-      <c r="GD13" s="99"/>
-      <c r="GE13" s="99"/>
-      <c r="GF13" s="99"/>
-      <c r="GG13" s="100"/>
+      <c r="FV13" s="100"/>
+      <c r="FW13" s="100"/>
+      <c r="FX13" s="100"/>
+      <c r="FY13" s="100"/>
+      <c r="FZ13" s="100"/>
+      <c r="GA13" s="101"/>
+      <c r="GB13" s="102"/>
+      <c r="GC13" s="100"/>
+      <c r="GD13" s="100"/>
+      <c r="GE13" s="100"/>
+      <c r="GF13" s="100"/>
+      <c r="GG13" s="101"/>
       <c r="GH13" s="77"/>
       <c r="GI13" s="78"/>
       <c r="GJ13" s="78"/>
@@ -6569,7 +6571,7 @@
       <c r="GX13" s="78"/>
       <c r="GY13" s="78"/>
       <c r="GZ13" s="78"/>
-      <c r="HA13" s="119"/>
+      <c r="HA13" s="97"/>
       <c r="HB13" s="77"/>
       <c r="HC13" s="78"/>
       <c r="HD13" s="78"/>
@@ -6577,7 +6579,7 @@
       <c r="HF13" s="78"/>
       <c r="HG13" s="78"/>
       <c r="HH13" s="78"/>
-      <c r="HI13" s="119"/>
+      <c r="HI13" s="97"/>
     </row>
     <row r="14" spans="1:217" ht="77.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="7"/>
@@ -6588,15 +6590,15 @@
       <c r="F14" s="49"/>
       <c r="G14" s="49"/>
       <c r="H14" s="50"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="103"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="103"/>
-      <c r="N14" s="103"/>
-      <c r="O14" s="103"/>
-      <c r="P14" s="103"/>
-      <c r="Q14" s="104"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104"/>
+      <c r="L14" s="104"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="104"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="105"/>
       <c r="R14" s="96"/>
       <c r="S14" s="120"/>
       <c r="T14" s="121"/>
@@ -6645,24 +6647,24 @@
       <c r="BK14" s="120"/>
       <c r="BL14" s="120"/>
       <c r="BM14" s="121"/>
-      <c r="BN14" s="102"/>
-      <c r="BO14" s="103"/>
-      <c r="BP14" s="103"/>
-      <c r="BQ14" s="103"/>
-      <c r="BR14" s="103"/>
-      <c r="BS14" s="103"/>
-      <c r="BT14" s="103"/>
-      <c r="BU14" s="104"/>
-      <c r="BV14" s="102"/>
-      <c r="BW14" s="103"/>
-      <c r="BX14" s="103"/>
-      <c r="BY14" s="103"/>
-      <c r="BZ14" s="103"/>
-      <c r="CA14" s="103"/>
-      <c r="CB14" s="103"/>
-      <c r="CC14" s="104"/>
+      <c r="BN14" s="103"/>
+      <c r="BO14" s="104"/>
+      <c r="BP14" s="104"/>
+      <c r="BQ14" s="104"/>
+      <c r="BR14" s="104"/>
+      <c r="BS14" s="104"/>
+      <c r="BT14" s="104"/>
+      <c r="BU14" s="105"/>
+      <c r="BV14" s="103"/>
+      <c r="BW14" s="104"/>
+      <c r="BX14" s="104"/>
+      <c r="BY14" s="104"/>
+      <c r="BZ14" s="104"/>
+      <c r="CA14" s="104"/>
+      <c r="CB14" s="104"/>
+      <c r="CC14" s="105"/>
       <c r="CD14" s="47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="CE14" s="20"/>
       <c r="CF14" s="20"/>
@@ -6675,14 +6677,14 @@
       <c r="CM14" s="20"/>
       <c r="CN14" s="20"/>
       <c r="CO14" s="20"/>
-      <c r="CP14" s="103"/>
-      <c r="CQ14" s="103"/>
-      <c r="CR14" s="103"/>
-      <c r="CS14" s="103"/>
-      <c r="CT14" s="103"/>
-      <c r="CU14" s="103"/>
-      <c r="CV14" s="103"/>
-      <c r="CW14" s="103"/>
+      <c r="CP14" s="104"/>
+      <c r="CQ14" s="104"/>
+      <c r="CR14" s="104"/>
+      <c r="CS14" s="104"/>
+      <c r="CT14" s="104"/>
+      <c r="CU14" s="104"/>
+      <c r="CV14" s="104"/>
+      <c r="CW14" s="104"/>
       <c r="CX14" s="20"/>
       <c r="CY14" s="20"/>
       <c r="CZ14" s="20"/>
@@ -6752,18 +6754,18 @@
       <c r="FS14" s="75"/>
       <c r="FT14" s="75"/>
       <c r="FU14" s="76"/>
-      <c r="FV14" s="103"/>
-      <c r="FW14" s="103"/>
-      <c r="FX14" s="103"/>
-      <c r="FY14" s="103"/>
-      <c r="FZ14" s="103"/>
-      <c r="GA14" s="104"/>
-      <c r="GB14" s="102"/>
-      <c r="GC14" s="103"/>
-      <c r="GD14" s="103"/>
-      <c r="GE14" s="103"/>
-      <c r="GF14" s="103"/>
-      <c r="GG14" s="104"/>
+      <c r="FV14" s="104"/>
+      <c r="FW14" s="104"/>
+      <c r="FX14" s="104"/>
+      <c r="FY14" s="104"/>
+      <c r="FZ14" s="104"/>
+      <c r="GA14" s="105"/>
+      <c r="GB14" s="103"/>
+      <c r="GC14" s="104"/>
+      <c r="GD14" s="104"/>
+      <c r="GE14" s="104"/>
+      <c r="GF14" s="104"/>
+      <c r="GG14" s="105"/>
       <c r="GH14" s="79"/>
       <c r="GI14" s="75"/>
       <c r="GJ14" s="75"/>

</xml_diff>

<commit_message>
Misc updates to types in guide. added melee data table
</commit_message>
<xml_diff>
--- a/File Research/Game Object Research File.xlsx
+++ b/File Research/Game Object Research File.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F903DEAB-8990-4D92-A174-368FC9F73CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF1B02B-CB0F-4432-88E7-1DDE244CCEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1328" yWindow="2070" windowWidth="18421" windowHeight="11453" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Object" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="273">
   <si>
     <t>Static Object</t>
   </si>
@@ -917,6 +917,12 @@
   <si>
     <t>Value affects Hp returned by study monster
 When whoamis is 64h(krillner?) a value of 30d is returned is this is not 0</t>
+  </si>
+  <si>
+    <t>Bit 7 set in create_object_trap when spawing a template based on the adventurer</t>
+  </si>
+  <si>
+    <t>when set door opens in the opposite direction</t>
   </si>
 </sst>
 </file>
@@ -2280,10 +2286,10 @@
   <dimension ref="A1:HI48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="BO38" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="CE12" sqref="CE12:CG12"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6584,7 +6590,9 @@
       <c r="A14" s="7"/>
       <c r="B14" s="141"/>
       <c r="C14" s="141"/>
-      <c r="D14" s="49"/>
+      <c r="D14" s="49" t="s">
+        <v>272</v>
+      </c>
       <c r="E14" s="49"/>
       <c r="F14" s="49"/>
       <c r="G14" s="49"/>
@@ -7482,7 +7490,7 @@
         <v>4284</v>
       </c>
     </row>
-    <row r="37" spans="1:87" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:87" ht="28.5" x14ac:dyDescent="0.45">
       <c r="G37">
         <v>15</v>
       </c>
@@ -7507,6 +7515,9 @@
       <c r="BO37" t="str">
         <f>DEC2HEX(BN37)</f>
         <v>3248</v>
+      </c>
+      <c r="CD37" s="16" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:87" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Combat related save game values
</commit_message>
<xml_diff>
--- a/File Research/Game Object Research File.xlsx
+++ b/File Research/Game Object Research File.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0225CEE7-DDC4-4077-98D6-CF07486D0841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6295070-530B-4910-B216-C7DAB310E074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{349C9796-1BFF-4A71-A28F-BEE29BD20DAE}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="274">
   <si>
     <t>Static Object</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>bits (h)</t>
-  </si>
-  <si>
-    <t>npc_height</t>
   </si>
   <si>
     <t>unk0x11</t>
@@ -722,11 +719,6 @@
     <t>TargetTileX - tile the NPC wants to go to
  gets compared to a TileX Param to see if npc is at a target tile
 0x3F</t>
-  </si>
-  <si>
-    <t>TargetTileY - tile the NPC wants to go to
-gets compared to a TileY Param to see if npc is at a target tile
-0xFC0</t>
   </si>
   <si>
     <t>Bit 5 set when arrived at destination in function DetermineIfAtTarget()</t>
@@ -884,13 +876,51 @@
     <t>Tracks motion of  the closing or opening door animation</t>
   </si>
   <si>
+    <t>Use to control spawing of the NPC default loot list. Loot only generated when trading with or on npc death. If NPC already has inventory this will be set set. Loot items are selected by the critter data for the npc</t>
+  </si>
+  <si>
+    <t>bit 7 is unset when a projectile is launched, it gets set to 1 when it hits an NPC
+bit 7 might mean the npc is in combat?
+When the avatar is killed the bit 7 is used to check if the avatar has to go to jail in the castle
+bit 7 checked in set_Race_attitude
+bit 7 is checked in special death cases relating to lady tory
+DOES IT MEAN OBJECT IS AN NPC???? not sure since bit 7 is unset after a missile hits it target
+possibly a tileY reference used closely with projectilesourceID value</t>
+  </si>
+  <si>
+    <t>Value affects Hp returned by study monster
+When whoamis is 64h(krillner?) a value of 30d is returned is this is not 0</t>
+  </si>
+  <si>
+    <t>Bit 7 set in create_object_trap when spawing a template based on the adventurer</t>
+  </si>
+  <si>
+    <t>when set door opens in the opposite direction</t>
+  </si>
+  <si>
+    <t>In damage objects this controls if a object is immune to damage</t>
+  </si>
+  <si>
+    <t>TargetTileY</t>
+  </si>
+  <si>
+    <t>TargetTileY - tile the NPC wants to go to
+gets compared to a TileY Param to see if npc is at a target tile
+(npc_height in uwformats)
+0xFC0</t>
+  </si>
+  <si>
+    <t>TargetZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">When standing still with an attitude of 0 an attempt will be made to detect the player. If found set bit 0 and set attack goals
 Bit 0 indicates that the npc is aware of the avatar's position, use in combat to chase the avatar
 Bit 1 is somehow connect to bit 0 behaviours, maybe used to indicate npc should turn towards target
 Bits 2 &amp; 3 when &lt;&gt; 0 the npc will execute a magic attack when it's animation is a ranged attack, value is alookup into critter data at 0x2Ah (bytes 2Ah to 2Ch) to get spell effect id to use. Value of lookup is based on RNG call in NpcStartMagicAttack()
 Bit 4 referenced in NpcGoal6(ranged attack),
 Bit 5 set when unable to do a magic attack
-Bit 6 - related to checking has the avatar struck the npc with a weapon? If unset npc in combat with avatar. if set npc in combat with last npc to damage them?? Impacts npc_attitude in conversations. When set an attitude of 6 is imported to the conversation???? If attitude&gt;3 at end of conversation bit is set again???
+Bit 6 - related to checking has the avatar struck the npc with a weapon? If unset npc in combat with avatar. if set npc in combat with last npc to damage them?? Impacts npc_attitude in conversations. When set an attitude of 6 is imported to the conversation???? If attitude&gt;3 at end of conversation bit is set again???,
+Bit 6 is also set on player summoned monsters
 Bit 7 can be set after a conversation
 Bits 6 and 7 randomly set in a subfunction of player updates()!!!
 Bit 6 and 7 stop npcs from hurting each other in combat when they are the same? 
@@ -898,31 +928,6 @@
 Possibly a series of bit fields representing combat and AI decisions
 Bit 6 used in conversations. when set  it will import 6 as the value of npc_attitude (when goal&lt;&gt;5 and gtart&lt;&gt;1)
 Bit 7 is used in conversations. when used as a imported it will either import 16 (when bit is set) or 192(when bit is 0) into the conversation </t>
-  </si>
-  <si>
-    <t>Use to control spawing of the NPC default loot list. Loot only generated when trading with or on npc death. If NPC already has inventory this will be set set. Loot items are selected by the critter data for the npc</t>
-  </si>
-  <si>
-    <t>bit 7 is unset when a projectile is launched, it gets set to 1 when it hits an NPC
-bit 7 might mean the npc is in combat?
-When the avatar is killed the bit 7 is used to check if the avatar has to go to jail in the castle
-bit 7 checked in set_Race_attitude
-bit 7 is checked in special death cases relating to lady tory
-DOES IT MEAN OBJECT IS AN NPC???? not sure since bit 7 is unset after a missile hits it target
-possibly a tileY reference used closely with projectilesourceID value</t>
-  </si>
-  <si>
-    <t>Value affects Hp returned by study monster
-When whoamis is 64h(krillner?) a value of 30d is returned is this is not 0</t>
-  </si>
-  <si>
-    <t>Bit 7 set in create_object_trap when spawing a template based on the adventurer</t>
-  </si>
-  <si>
-    <t>when set door opens in the opposite direction</t>
-  </si>
-  <si>
-    <t>In damage objects this controls if a object is immune to damage</t>
   </si>
 </sst>
 </file>
@@ -2286,10 +2291,10 @@
   <dimension ref="A1:HI48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="AB9" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="GM13" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="GT15" sqref="GT15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2350,7 +2355,7 @@
     <col min="111" max="111" width="43.796875" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="1.73046875" bestFit="1" customWidth="1"/>
     <col min="113" max="113" width="40.53125" bestFit="1" customWidth="1"/>
-    <col min="114" max="117" width="1.73046875" bestFit="1" customWidth="1"/>
+    <col min="114" max="117" width="4.9296875" customWidth="1"/>
     <col min="118" max="118" width="44.46484375" bestFit="1" customWidth="1"/>
     <col min="119" max="121" width="1.73046875" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="49.1328125" bestFit="1" customWidth="1"/>
@@ -4990,7 +4995,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>12</v>
@@ -5086,7 +5091,7 @@
       <c r="BT7" s="129"/>
       <c r="BU7" s="130"/>
       <c r="BV7" s="128" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BW7" s="129"/>
       <c r="BX7" s="129"/>
@@ -5106,7 +5111,7 @@
       <c r="CJ7" s="101"/>
       <c r="CK7" s="150"/>
       <c r="CL7" s="128" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="CM7" s="129"/>
       <c r="CN7" s="129"/>
@@ -5135,32 +5140,34 @@
         <v>28</v>
       </c>
       <c r="DE7" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="DF7" s="27"/>
       <c r="DG7" s="54" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="DH7" s="28"/>
       <c r="DI7" s="28"/>
-      <c r="DJ7" s="28"/>
-      <c r="DK7" s="28"/>
-      <c r="DL7" s="28"/>
-      <c r="DM7" s="29"/>
-      <c r="DN7" s="125" t="s">
+      <c r="DJ7" s="134" t="s">
+        <v>272</v>
+      </c>
+      <c r="DK7" s="135"/>
+      <c r="DL7" s="135"/>
+      <c r="DM7" s="136"/>
+      <c r="DN7" s="126" t="s">
         <v>26</v>
       </c>
       <c r="DO7" s="126"/>
       <c r="DP7" s="126"/>
       <c r="DQ7" s="127"/>
       <c r="DR7" s="137" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="DS7" s="138"/>
       <c r="DT7" s="138"/>
       <c r="DU7" s="139"/>
       <c r="DV7" s="155" t="s">
-        <v>31</v>
+        <v>270</v>
       </c>
       <c r="DW7" s="156"/>
       <c r="DX7" s="156"/>
@@ -5168,7 +5175,7 @@
       <c r="DZ7" s="156"/>
       <c r="EA7" s="157"/>
       <c r="EB7" s="158" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="EC7" s="156"/>
       <c r="ED7" s="156"/>
@@ -5176,7 +5183,7 @@
       <c r="EF7" s="156"/>
       <c r="EG7" s="157"/>
       <c r="EH7" s="122" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="EI7" s="123"/>
       <c r="EJ7" s="123"/>
@@ -5186,7 +5193,7 @@
       <c r="EN7" s="123"/>
       <c r="EO7" s="124"/>
       <c r="EP7" s="146" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="EQ7" s="147"/>
       <c r="ER7" s="147"/>
@@ -5197,7 +5204,7 @@
       <c r="EW7" s="148"/>
       <c r="EX7" s="22"/>
       <c r="EY7" s="134" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="EZ7" s="135"/>
       <c r="FA7" s="135"/>
@@ -5206,23 +5213,23 @@
       <c r="FD7" s="135"/>
       <c r="FE7" s="136"/>
       <c r="FF7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="FG7" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="FH7" s="24"/>
       <c r="FI7" s="24"/>
       <c r="FJ7" s="25"/>
       <c r="FK7" s="140" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="FL7" s="141"/>
       <c r="FM7" s="142"/>
       <c r="FN7" s="38"/>
       <c r="FO7" s="39"/>
       <c r="FP7" s="143" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="FQ7" s="144"/>
       <c r="FR7" s="144"/>
@@ -5230,7 +5237,7 @@
       <c r="FT7" s="144"/>
       <c r="FU7" s="145"/>
       <c r="FV7" s="138" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="FW7" s="138"/>
       <c r="FX7" s="138"/>
@@ -5238,7 +5245,7 @@
       <c r="FZ7" s="138"/>
       <c r="GA7" s="139"/>
       <c r="GB7" s="137" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="GC7" s="138"/>
       <c r="GD7" s="138"/>
@@ -5246,29 +5253,29 @@
       <c r="GF7" s="138"/>
       <c r="GG7" s="139"/>
       <c r="GH7" s="122" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="GI7" s="123"/>
       <c r="GJ7" s="123"/>
       <c r="GK7" s="124"/>
       <c r="GL7" s="122" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="GM7" s="123"/>
       <c r="GN7" s="124"/>
       <c r="GO7" s="137" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="GP7" s="138"/>
       <c r="GQ7" s="138"/>
       <c r="GR7" s="138"/>
       <c r="GS7" s="139"/>
       <c r="GT7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="GU7" s="2"/>
       <c r="GV7" s="109" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="GW7" s="110"/>
       <c r="GX7" s="110"/>
@@ -5276,7 +5283,7 @@
       <c r="GZ7" s="110"/>
       <c r="HA7" s="152"/>
       <c r="HB7" s="137" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="HC7" s="138"/>
       <c r="HD7" s="138"/>
@@ -5300,10 +5307,10 @@
       <c r="G8" s="138"/>
       <c r="H8" s="139"/>
       <c r="R8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="X8" s="134">
         <v>380</v>
@@ -5311,22 +5318,22 @@
       <c r="Y8" s="135"/>
       <c r="Z8" s="136"/>
       <c r="AD8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AL8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AN8" t="s">
         <v>131</v>
       </c>
-      <c r="AN8" t="s">
-        <v>132</v>
-      </c>
       <c r="AT8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AZ8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BJ8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="CD8" s="22"/>
       <c r="CE8" s="43"/>
@@ -5337,7 +5344,7 @@
       <c r="CJ8" s="44"/>
       <c r="CK8" s="45"/>
       <c r="CL8" s="152" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="CM8" s="153"/>
       <c r="CN8" s="153"/>
@@ -5355,7 +5362,7 @@
       <c r="CZ8" s="153"/>
       <c r="DA8" s="153"/>
       <c r="DB8" s="153" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="DC8" s="153"/>
       <c r="DD8" s="153"/>
@@ -5364,16 +5371,16 @@
       <c r="DG8" s="154"/>
       <c r="DH8" s="153"/>
       <c r="DI8" s="153"/>
-      <c r="DJ8" s="153"/>
-      <c r="DK8" s="153"/>
-      <c r="DL8" s="153"/>
-      <c r="DM8" s="153"/>
+      <c r="DJ8" s="154"/>
+      <c r="DK8" s="154"/>
+      <c r="DL8" s="154"/>
+      <c r="DM8" s="154"/>
       <c r="DN8" s="153"/>
       <c r="DO8" s="153"/>
       <c r="DP8" s="153"/>
       <c r="DQ8" s="153"/>
       <c r="DR8" s="153" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="DS8" s="153"/>
       <c r="DT8" s="153"/>
@@ -5391,7 +5398,7 @@
       <c r="EF8" s="153"/>
       <c r="EG8" s="153"/>
       <c r="EH8" s="109" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="EI8" s="110"/>
       <c r="EJ8" s="110"/>
@@ -5401,10 +5408,10 @@
       <c r="EN8" s="110"/>
       <c r="EO8" s="110"/>
       <c r="FH8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="FN8" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="FO8" s="13"/>
       <c r="FP8" s="43"/>
@@ -5414,10 +5421,10 @@
       <c r="FT8" s="44"/>
       <c r="FU8" s="45"/>
       <c r="FV8" t="s">
+        <v>124</v>
+      </c>
+      <c r="GB8" t="s">
         <v>125</v>
-      </c>
-      <c r="GB8" t="s">
-        <v>126</v>
       </c>
       <c r="GV8" s="22"/>
       <c r="GW8" s="22"/>
@@ -5429,21 +5436,21 @@
     </row>
     <row r="9" spans="1:217" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="62"/>
       <c r="C9" s="63"/>
       <c r="D9" s="63" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E9" s="163" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F9" s="159"/>
       <c r="G9" s="159"/>
       <c r="H9" s="160"/>
       <c r="I9" s="98" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="98"/>
       <c r="K9" s="98"/>
@@ -5454,22 +5461,22 @@
       <c r="P9" s="98"/>
       <c r="Q9" s="99"/>
       <c r="R9" s="90" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S9" s="91"/>
       <c r="T9" s="92"/>
       <c r="U9" s="90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V9" s="91"/>
       <c r="W9" s="92"/>
       <c r="X9" s="90" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Y9" s="91"/>
       <c r="Z9" s="92"/>
       <c r="AA9" s="90" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AB9" s="91"/>
       <c r="AC9" s="91"/>
@@ -5478,7 +5485,7 @@
       <c r="AF9" s="91"/>
       <c r="AG9" s="92"/>
       <c r="AH9" s="90" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AI9" s="91"/>
       <c r="AJ9" s="91"/>
@@ -5490,7 +5497,7 @@
       <c r="AP9" s="91"/>
       <c r="AQ9" s="92"/>
       <c r="AR9" s="90" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AS9" s="91"/>
       <c r="AT9" s="91"/>
@@ -5498,7 +5505,7 @@
       <c r="AV9" s="91"/>
       <c r="AW9" s="92"/>
       <c r="AX9" s="91" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AY9" s="91"/>
       <c r="AZ9" s="91"/>
@@ -5510,7 +5517,7 @@
       <c r="BF9" s="91"/>
       <c r="BG9" s="92"/>
       <c r="BH9" s="90" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="BI9" s="91"/>
       <c r="BJ9" s="91"/>
@@ -5518,7 +5525,7 @@
       <c r="BL9" s="91"/>
       <c r="BM9" s="92"/>
       <c r="BN9" s="106" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BO9" s="98"/>
       <c r="BP9" s="98"/>
@@ -5528,7 +5535,7 @@
       <c r="BT9" s="98"/>
       <c r="BU9" s="99"/>
       <c r="BV9" s="90" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BW9" s="98"/>
       <c r="BX9" s="98"/>
@@ -5538,21 +5545,21 @@
       <c r="CB9" s="98"/>
       <c r="CC9" s="99"/>
       <c r="CD9" s="57" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="CE9" s="91" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CF9" s="91"/>
       <c r="CG9" s="91"/>
       <c r="CH9" s="91" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="CI9" s="91"/>
       <c r="CJ9" s="91"/>
       <c r="CK9" s="92"/>
       <c r="CL9" s="90" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="CM9" s="91"/>
       <c r="CN9" s="91"/>
@@ -5570,43 +5577,43 @@
       <c r="CZ9" s="91"/>
       <c r="DA9" s="92"/>
       <c r="DB9" s="76" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="DC9" s="77"/>
       <c r="DD9" s="88" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="DE9" s="88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="DF9" s="51"/>
       <c r="DG9" s="82" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="DH9" s="51"/>
       <c r="DI9" s="55" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="DJ9" s="76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="DK9" s="85"/>
       <c r="DL9" s="85"/>
       <c r="DM9" s="77"/>
       <c r="DN9" s="76" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="DO9" s="85"/>
       <c r="DP9" s="85"/>
       <c r="DQ9" s="77"/>
       <c r="DR9" s="112" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="DS9" s="112"/>
       <c r="DT9" s="112"/>
       <c r="DU9" s="112"/>
       <c r="DV9" s="90" t="s">
-        <v>222</v>
+        <v>271</v>
       </c>
       <c r="DW9" s="91"/>
       <c r="DX9" s="91"/>
@@ -5614,7 +5621,7 @@
       <c r="DZ9" s="91"/>
       <c r="EA9" s="92"/>
       <c r="EB9" s="90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="EC9" s="91"/>
       <c r="ED9" s="91"/>
@@ -5622,7 +5629,7 @@
       <c r="EF9" s="91"/>
       <c r="EG9" s="92"/>
       <c r="EP9" s="90" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="EQ9" s="91"/>
       <c r="ER9" s="91"/>
@@ -5632,7 +5639,7 @@
       <c r="EV9" s="91"/>
       <c r="EW9" s="92"/>
       <c r="EX9" s="90" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="EY9" s="91"/>
       <c r="EZ9" s="91"/>
@@ -5642,15 +5649,15 @@
       <c r="FD9" s="91"/>
       <c r="FE9" s="92"/>
       <c r="FG9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="FK9" s="117" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="FL9" s="117"/>
       <c r="FM9" s="118"/>
       <c r="FN9" s="90" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="FO9" s="59"/>
       <c r="FP9" s="16"/>
@@ -5658,7 +5665,7 @@
       <c r="FR9" s="46"/>
       <c r="FU9" s="30"/>
       <c r="FV9" s="91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="FW9" s="98"/>
       <c r="FX9" s="98"/>
@@ -5666,7 +5673,7 @@
       <c r="FZ9" s="98"/>
       <c r="GA9" s="99"/>
       <c r="GB9" s="90" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="GC9" s="98"/>
       <c r="GD9" s="98"/>
@@ -5674,7 +5681,7 @@
       <c r="GF9" s="98"/>
       <c r="GG9" s="99"/>
       <c r="GH9" s="93" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="GI9" s="71"/>
       <c r="GJ9" s="71"/>
@@ -5682,17 +5689,17 @@
       <c r="GL9" s="113"/>
       <c r="GM9" s="113"/>
       <c r="GN9" s="165" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="GO9" s="90" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="GP9" s="91"/>
       <c r="GQ9" s="91"/>
       <c r="GR9" s="91"/>
       <c r="GS9" s="92"/>
       <c r="GT9" s="90" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="GU9" s="91"/>
       <c r="GV9" s="91"/>
@@ -5702,7 +5709,7 @@
       <c r="GZ9" s="91"/>
       <c r="HA9" s="94"/>
       <c r="HB9" s="90" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="HC9" s="91"/>
       <c r="HD9" s="91"/>
@@ -5717,11 +5724,11 @@
       <c r="B10" s="64"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="73" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G10" s="74"/>
       <c r="H10" s="75"/>
@@ -5799,10 +5806,10 @@
       <c r="CB10" s="101"/>
       <c r="CC10" s="102"/>
       <c r="CD10" s="47" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="CE10" s="71" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="CF10" s="71"/>
       <c r="CG10" s="71"/>
@@ -5868,11 +5875,11 @@
       <c r="EW10" s="94"/>
       <c r="EX10" s="17"/>
       <c r="EY10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="FE10" s="18"/>
       <c r="FK10" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="FL10" s="117"/>
       <c r="FM10" s="118"/>
@@ -5928,7 +5935,7 @@
       <c r="B11" s="65"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E11" s="66"/>
       <c r="F11" s="66"/>
@@ -6008,7 +6015,7 @@
       <c r="CB11" s="101"/>
       <c r="CC11" s="102"/>
       <c r="CD11" s="56" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CE11" s="16"/>
       <c r="CF11" s="16"/>
@@ -6050,7 +6057,7 @@
       <c r="DP11" s="86"/>
       <c r="DQ11" s="79"/>
       <c r="DR11" s="159" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="DS11" s="159"/>
       <c r="DT11" s="159"/>
@@ -6068,7 +6075,7 @@
       <c r="EF11" s="159"/>
       <c r="EG11" s="160"/>
       <c r="EH11" s="71" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="EI11" s="71"/>
       <c r="EJ11" s="71"/>
@@ -6086,10 +6093,10 @@
       <c r="EV11" s="71"/>
       <c r="EW11" s="94"/>
       <c r="EX11" s="47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="EY11" s="93" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="EZ11" s="71"/>
       <c r="FA11" s="71"/>
@@ -6098,22 +6105,22 @@
       <c r="FD11" s="71"/>
       <c r="FE11" s="94"/>
       <c r="FF11" s="115" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="FG11" s="112"/>
       <c r="FH11" s="112"/>
       <c r="FI11" s="116"/>
       <c r="FK11" s="117" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="FL11" s="117"/>
       <c r="FM11" s="119"/>
       <c r="FN11" s="70" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="FO11" s="72"/>
       <c r="FP11" s="70" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="FQ11" s="71"/>
       <c r="FR11" s="71"/>
@@ -6137,7 +6144,7 @@
       <c r="GJ11" s="71"/>
       <c r="GK11" s="71"/>
       <c r="GL11" s="91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="GM11" s="91"/>
       <c r="GN11" s="91"/>
@@ -6163,10 +6170,10 @@
       <c r="B12" s="47"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="48"/>
@@ -6244,10 +6251,10 @@
       <c r="CB12" s="101"/>
       <c r="CC12" s="102"/>
       <c r="CD12" s="47" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="CE12" s="71" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="CF12" s="71"/>
       <c r="CG12" s="71"/>
@@ -6256,7 +6263,7 @@
       <c r="CK12" s="48"/>
       <c r="CL12" s="17"/>
       <c r="CP12" s="71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CQ12" s="101"/>
       <c r="CR12" s="101"/>
@@ -6314,12 +6321,12 @@
       <c r="EV12" s="71"/>
       <c r="EW12" s="94"/>
       <c r="EX12" s="161" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="EY12" s="17"/>
       <c r="FE12" s="18"/>
       <c r="FK12" s="111" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="FL12" s="111"/>
       <c r="FM12" s="111"/>
@@ -6348,7 +6355,7 @@
       <c r="GJ12" s="71"/>
       <c r="GK12" s="71"/>
       <c r="GL12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="GT12" s="93"/>
       <c r="GU12" s="71"/>
@@ -6370,19 +6377,19 @@
     <row r="13" spans="1:217" ht="65.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="69" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C13" s="69" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>234</v>
-      </c>
       <c r="E13" s="16" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F13" s="71" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G13" s="71"/>
       <c r="H13" s="94"/>
@@ -6460,10 +6467,10 @@
       <c r="CB13" s="101"/>
       <c r="CC13" s="102"/>
       <c r="CD13" s="47" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="CE13" s="71" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CF13" s="71"/>
       <c r="CG13" s="71"/>
@@ -6481,7 +6488,7 @@
       <c r="CV13" s="101"/>
       <c r="CW13" s="101"/>
       <c r="DB13" s="70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="DC13" s="71"/>
       <c r="DD13" s="71"/>
@@ -6499,7 +6506,7 @@
       <c r="DP13" s="71"/>
       <c r="DQ13" s="72"/>
       <c r="DR13" s="69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="DS13" s="69"/>
       <c r="DT13" s="69"/>
@@ -6534,11 +6541,11 @@
       <c r="EW13" s="94"/>
       <c r="EX13" s="161"/>
       <c r="EY13" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="FE13" s="18"/>
       <c r="FK13" s="117" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="FL13" s="117"/>
       <c r="FM13" s="119"/>
@@ -6567,7 +6574,7 @@
       <c r="GJ13" s="71"/>
       <c r="GK13" s="71"/>
       <c r="GN13" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="GT13" s="93"/>
       <c r="GU13" s="71"/>
@@ -6591,7 +6598,7 @@
       <c r="B14" s="69"/>
       <c r="C14" s="69"/>
       <c r="D14" s="49" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E14" s="49"/>
       <c r="F14" s="49"/>
@@ -6671,7 +6678,7 @@
       <c r="CB14" s="104"/>
       <c r="CC14" s="105"/>
       <c r="CD14" s="47" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="CE14" s="20"/>
       <c r="CF14" s="20"/>
@@ -6713,7 +6720,7 @@
       <c r="DP14" s="74"/>
       <c r="DQ14" s="75"/>
       <c r="DR14" s="69" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="DS14" s="69"/>
       <c r="DT14" s="69"/>
@@ -6742,14 +6749,14 @@
       <c r="EY14" s="19"/>
       <c r="EZ14" s="20"/>
       <c r="FA14" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="FB14" s="20"/>
       <c r="FC14" s="20"/>
       <c r="FD14" s="20"/>
       <c r="FE14" s="21"/>
       <c r="FK14" s="120" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="FL14" s="120"/>
       <c r="FM14" s="121"/>
@@ -6778,7 +6785,7 @@
       <c r="GJ14" s="74"/>
       <c r="GK14" s="74"/>
       <c r="GM14" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="GT14" s="95"/>
       <c r="GU14" s="96"/>
@@ -6800,14 +6807,14 @@
     <row r="15" spans="1:217" x14ac:dyDescent="0.45">
       <c r="A15" s="7"/>
       <c r="F15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U15" s="13"/>
       <c r="V15" s="13"/>
       <c r="W15" s="13"/>
       <c r="AX15" s="14"/>
       <c r="CD15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="CO15">
         <v>0</v>
@@ -6819,7 +6826,7 @@
         <v>15</v>
       </c>
       <c r="DS15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="EH15" s="13"/>
       <c r="EI15" s="13"/>
@@ -6830,11 +6837,11 @@
       <c r="EN15" s="13"/>
       <c r="EO15" s="13"/>
       <c r="EY15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="FF15" s="13"/>
       <c r="FG15" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="FH15" s="13"/>
       <c r="FI15" s="13"/>
@@ -6864,7 +6871,7 @@
     <row r="16" spans="1:217" x14ac:dyDescent="0.45">
       <c r="A16" s="7"/>
       <c r="N16" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
@@ -6881,7 +6888,7 @@
       <c r="AA16" s="26"/>
       <c r="AB16" s="26"/>
       <c r="CD16" s="107" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="CE16" s="108"/>
       <c r="CF16" s="108"/>
@@ -6891,24 +6898,24 @@
       <c r="CJ16" s="108"/>
       <c r="CK16" s="108"/>
       <c r="DE16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="DS16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="FA16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="FG16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N17" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
@@ -6933,27 +6940,27 @@
       <c r="CJ17" s="108"/>
       <c r="CK17" s="108"/>
       <c r="DE17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="DN17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="EC17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="FG17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="GV17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N18" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O18" s="26"/>
       <c r="P18" s="26"/>
@@ -6978,27 +6985,27 @@
       <c r="CJ18" s="108"/>
       <c r="CK18" s="108"/>
       <c r="CL18" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="CM18" s="28"/>
       <c r="CN18" s="28"/>
       <c r="CO18" s="29"/>
       <c r="DE18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="EC18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="EY18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N19" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O19" s="26"/>
       <c r="P19" s="26"/>
@@ -7023,22 +7030,22 @@
       <c r="CJ19" s="108"/>
       <c r="CK19" s="108"/>
       <c r="CM19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="DE19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="EC19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="FG19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A20" s="7"/>
       <c r="N20" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O20" s="26"/>
       <c r="P20" s="26"/>
@@ -7063,25 +7070,25 @@
       <c r="CJ20" s="108"/>
       <c r="CK20" s="108"/>
       <c r="DI20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="FG20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A21" s="7"/>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" t="s">
         <v>64</v>
       </c>
-      <c r="H21" t="s">
-        <v>65</v>
-      </c>
       <c r="N21" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
@@ -7106,16 +7113,16 @@
       <c r="CJ21" s="108"/>
       <c r="CK21" s="108"/>
       <c r="CL21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="DR21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="EY21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="FG21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:204" x14ac:dyDescent="0.45">
@@ -7139,7 +7146,7 @@
         <v>5972</v>
       </c>
       <c r="N22" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
@@ -7164,10 +7171,10 @@
       <c r="CJ22" s="108"/>
       <c r="CK22" s="108"/>
       <c r="DR22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="FH22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:204" x14ac:dyDescent="0.45">
@@ -7184,7 +7191,7 @@
         <v>5973</v>
       </c>
       <c r="N23" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
@@ -7209,10 +7216,10 @@
       <c r="CJ23" s="108"/>
       <c r="CK23" s="108"/>
       <c r="DE23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="FH23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:204" x14ac:dyDescent="0.45">
@@ -7237,10 +7244,10 @@
       <c r="CJ24" s="108"/>
       <c r="CK24" s="108"/>
       <c r="DG24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="EX24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:204" x14ac:dyDescent="0.45">
@@ -7265,10 +7272,10 @@
       <c r="CJ25" s="108"/>
       <c r="CK25" s="108"/>
       <c r="DG25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="EX25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:204" x14ac:dyDescent="0.45">
@@ -7293,7 +7300,7 @@
       <c r="CJ26" s="108"/>
       <c r="CK26" s="108"/>
       <c r="DG26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:204" x14ac:dyDescent="0.45">
@@ -7318,7 +7325,7 @@
       <c r="CJ27" s="108"/>
       <c r="CK27" s="108"/>
       <c r="DG27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:204" x14ac:dyDescent="0.45">
@@ -7343,7 +7350,7 @@
       <c r="CJ28" s="108"/>
       <c r="CK28" s="108"/>
       <c r="EX28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:204" x14ac:dyDescent="0.45">
@@ -7382,7 +7389,7 @@
         <v>597A</v>
       </c>
       <c r="CD30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:204" x14ac:dyDescent="0.45">
@@ -7402,7 +7409,7 @@
     <row r="32" spans="1:204" x14ac:dyDescent="0.45">
       <c r="A32" s="7"/>
       <c r="F32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G32">
         <v>10</v>
@@ -7430,7 +7437,7 @@
         <v>597D</v>
       </c>
       <c r="CD33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:87" x14ac:dyDescent="0.45">
@@ -7447,7 +7454,7 @@
         <v>597E</v>
       </c>
       <c r="BN34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:87" x14ac:dyDescent="0.45">
@@ -7463,10 +7470,10 @@
         <v>597F</v>
       </c>
       <c r="BN35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="CD35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:87" x14ac:dyDescent="0.45">
@@ -7503,7 +7510,7 @@
         <v>5981</v>
       </c>
       <c r="BL37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="BM37">
         <v>1003</v>
@@ -7517,7 +7524,7 @@
         <v>3248</v>
       </c>
       <c r="CD37" s="16" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:87" x14ac:dyDescent="0.45">
@@ -7554,13 +7561,13 @@
         <v>5983</v>
       </c>
       <c r="BL39" s="68" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BZ39" t="s">
+        <v>57</v>
+      </c>
+      <c r="CE39" t="s">
         <v>58</v>
-      </c>
-      <c r="CE39" t="s">
-        <v>59</v>
       </c>
       <c r="CG39">
         <v>9</v>
@@ -7587,7 +7594,7 @@
         <v>Object at 7CD6:74CC</v>
       </c>
       <c r="CE40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="CG40">
         <v>7</v>
@@ -7730,7 +7737,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="177">
+  <mergeCells count="178">
     <mergeCell ref="E8:H8"/>
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="F10:H10"/>
@@ -7770,6 +7777,7 @@
     <mergeCell ref="DR8:EG8"/>
     <mergeCell ref="EY11:FE11"/>
     <mergeCell ref="EX12:EX14"/>
+    <mergeCell ref="DJ7:DM7"/>
     <mergeCell ref="HB3:HI3"/>
     <mergeCell ref="AR7:AW7"/>
     <mergeCell ref="BH7:BM7"/>
@@ -7929,7 +7937,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="166">
         <v>0</v>
@@ -8247,7 +8255,7 @@
     </row>
     <row r="5" spans="1:33" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" s="34">
         <f t="shared" ref="B5:H5" si="1">B2-8</f>
@@ -8375,37 +8383,37 @@
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="134" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6" s="135"/>
       <c r="F6" s="135"/>
       <c r="G6" s="136"/>
       <c r="H6" s="54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I6" s="58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J6" s="169" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K6" s="170"/>
       <c r="L6" s="170"/>
       <c r="M6" s="171"/>
       <c r="N6" s="169" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O6" s="170"/>
       <c r="P6" s="170"/>
       <c r="Q6" s="171"/>
       <c r="R6" s="169" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S6" s="170"/>
       <c r="T6" s="170"/>
@@ -8417,7 +8425,7 @@
       <c r="Z6" s="170"/>
       <c r="AA6" s="171"/>
       <c r="AB6" s="169" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AC6" s="170"/>
       <c r="AD6" s="170"/>
@@ -8427,40 +8435,40 @@
     </row>
     <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="172" t="s">
         <v>182</v>
-      </c>
-      <c r="D7" s="172" t="s">
-        <v>183</v>
       </c>
       <c r="E7" s="172"/>
       <c r="F7" s="172"/>
       <c r="G7" s="172"/>
       <c r="H7" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>185</v>
-      </c>
       <c r="J7" s="172" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K7" s="172"/>
       <c r="L7" s="172"/>
       <c r="M7" s="172"/>
       <c r="N7" s="172" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O7" s="172"/>
       <c r="P7" s="172"/>
       <c r="Q7" s="172"/>
       <c r="R7" s="172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S7" s="172"/>
       <c r="T7" s="172"/>
@@ -8472,7 +8480,7 @@
       <c r="Z7" s="172"/>
       <c r="AA7" s="172"/>
       <c r="AB7" s="172" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC7" s="172"/>
       <c r="AD7" s="172"/>
@@ -8483,7 +8491,7 @@
     <row r="8" spans="1:33" ht="114" x14ac:dyDescent="0.45">
       <c r="A8" s="7"/>
       <c r="I8" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -8532,7 +8540,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C1">
         <f>HEX2DEC("2654")</f>
@@ -8541,22 +8549,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -8572,10 +8580,10 @@
         <v>2654</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -8604,13 +8612,13 @@
         <v>2656</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -8639,13 +8647,13 @@
         <v>2658</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -8674,7 +8682,7 @@
         <v>265A</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -8703,7 +8711,7 @@
         <v>265C</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -8732,7 +8740,7 @@
         <v>265E</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -8761,10 +8769,10 @@
         <v>2660</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -8793,7 +8801,7 @@
         <v>2662</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -8822,7 +8830,7 @@
         <v>2664</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -8851,7 +8859,7 @@
         <v>2666</v>
       </c>
       <c r="D21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -8880,10 +8888,10 @@
         <v>2668</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -8912,7 +8920,7 @@
         <v>266A</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -8928,7 +8936,7 @@
         <v>266B</v>
       </c>
       <c r="D26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -8944,7 +8952,7 @@
         <v>266C</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -8960,7 +8968,7 @@
         <v>266D</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -8976,7 +8984,7 @@
         <v>266E</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -9008,7 +9016,7 @@
         <v>2670</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -9037,10 +9045,10 @@
         <v>2672</v>
       </c>
       <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" t="s">
         <v>75</v>
-      </c>
-      <c r="E33" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
@@ -9069,7 +9077,7 @@
         <v>2674</v>
       </c>
       <c r="D35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
@@ -9098,7 +9106,7 @@
         <v>2676</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
@@ -9114,7 +9122,7 @@
         <v>2677</v>
       </c>
       <c r="D38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
@@ -9143,7 +9151,7 @@
         <v>2679</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
@@ -9159,7 +9167,7 @@
         <v>267A</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>